<commit_message>
add form order detail
</commit_message>
<xml_diff>
--- a/_Doc/Feature.xlsx
+++ b/_Doc/Feature.xlsx
@@ -226,7 +226,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2410" uniqueCount="1688">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2415" uniqueCount="1693">
   <si>
     <t>No.</t>
   </si>
@@ -5633,6 +5633,21 @@
   </si>
   <si>
     <t>update ProductList set RateUnit=1;</t>
+  </si>
+  <si>
+    <t>สินค้าเพิ่มหน่อยขายหลัก</t>
+  </si>
+  <si>
+    <t>หน่วยย่อยใช้กำหนดตัวมาหารแทน เช่น 1/12 โหล</t>
+  </si>
+  <si>
+    <t>update stock ให้ทำ SN ได้</t>
+  </si>
+  <si>
+    <t>PO เพิ่มหน่วย</t>
+  </si>
+  <si>
+    <t>update stock เปลี่ยนเป็น list สินค้ามา update เลย</t>
   </si>
 </sst>
 </file>
@@ -6609,6 +6624,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -6616,6 +6640,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -6629,18 +6656,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -7505,20 +7520,20 @@
       <c r="B1" s="2"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="196" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="196" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="196" t="s">
+      <c r="A2" s="200" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="200" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="200" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="197"/>
-      <c r="B3" s="197"/>
-      <c r="C3" s="197"/>
+      <c r="A3" s="201"/>
+      <c r="B3" s="201"/>
+      <c r="C3" s="201"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
@@ -8720,12 +8735,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
     <mergeCell ref="B43:C43"/>
     <mergeCell ref="B44:C44"/>
     <mergeCell ref="B45:C45"/>
@@ -8736,6 +8745,12 @@
     <mergeCell ref="B40:C40"/>
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -10648,10 +10663,10 @@
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
-  <dimension ref="A1:C362"/>
+  <dimension ref="A1:C372"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A339" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C344" sqref="C344:C347"/>
+    <sheetView tabSelected="1" topLeftCell="A342" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B345" sqref="B345"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21.75" x14ac:dyDescent="0.5"/>
@@ -12611,80 +12626,107 @@
       </c>
     </row>
     <row r="347" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="B347" s="151" t="s">
-        <v>1525</v>
-      </c>
       <c r="C347" s="151" t="s">
         <v>1687</v>
       </c>
     </row>
-    <row r="348" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="B348" s="151" t="s">
-        <v>1451</v>
-      </c>
-    </row>
     <row r="349" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B349" s="151" t="s">
-        <v>1624</v>
+        <v>1688</v>
       </c>
     </row>
     <row r="350" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B350" s="151" t="s">
-        <v>1526</v>
+        <v>1689</v>
       </c>
     </row>
     <row r="351" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B351" s="151" t="s">
-        <v>1625</v>
-      </c>
-    </row>
-    <row r="352" spans="1:3" ht="87" x14ac:dyDescent="0.5">
-      <c r="B352" s="152" t="s">
-        <v>1626</v>
-      </c>
-    </row>
-    <row r="354" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B354" s="187" t="s">
-        <v>1644</v>
-      </c>
-    </row>
-    <row r="355" spans="2:2" ht="65.25" x14ac:dyDescent="0.5">
-      <c r="B355" s="188" t="s">
-        <v>1642</v>
-      </c>
-    </row>
-    <row r="356" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B356" s="189" t="s">
-        <v>1643</v>
+        <v>1690</v>
+      </c>
+    </row>
+    <row r="352" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="B352" s="151" t="s">
+        <v>1692</v>
+      </c>
+    </row>
+    <row r="353" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B353" s="151" t="s">
+        <v>1691</v>
       </c>
     </row>
     <row r="357" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B357" s="190" t="s">
-        <v>1645</v>
+      <c r="B357" s="151" t="s">
+        <v>1525</v>
       </c>
     </row>
     <row r="358" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B358" s="186" t="s">
-        <v>1646</v>
+      <c r="B358" s="151" t="s">
+        <v>1451</v>
       </c>
     </row>
     <row r="359" spans="2:2" x14ac:dyDescent="0.5">
       <c r="B359" s="151" t="s">
-        <v>1647</v>
+        <v>1624</v>
       </c>
     </row>
     <row r="360" spans="2:2" x14ac:dyDescent="0.5">
       <c r="B360" s="151" t="s">
+        <v>1526</v>
+      </c>
+    </row>
+    <row r="361" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B361" s="151" t="s">
+        <v>1625</v>
+      </c>
+    </row>
+    <row r="362" spans="2:2" ht="87" x14ac:dyDescent="0.5">
+      <c r="B362" s="152" t="s">
+        <v>1626</v>
+      </c>
+    </row>
+    <row r="364" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B364" s="187" t="s">
+        <v>1644</v>
+      </c>
+    </row>
+    <row r="365" spans="2:2" ht="65.25" x14ac:dyDescent="0.5">
+      <c r="B365" s="188" t="s">
+        <v>1642</v>
+      </c>
+    </row>
+    <row r="366" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B366" s="189" t="s">
+        <v>1643</v>
+      </c>
+    </row>
+    <row r="367" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B367" s="190" t="s">
+        <v>1645</v>
+      </c>
+    </row>
+    <row r="368" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B368" s="186" t="s">
+        <v>1646</v>
+      </c>
+    </row>
+    <row r="369" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B369" s="151" t="s">
+        <v>1647</v>
+      </c>
+    </row>
+    <row r="370" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B370" s="151" t="s">
         <v>1648</v>
       </c>
     </row>
-    <row r="361" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B361" s="187" t="s">
+    <row r="371" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B371" s="187" t="s">
         <v>1649</v>
       </c>
     </row>
-    <row r="362" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B362" s="151" t="s">
+    <row r="372" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B372" s="151" t="s">
         <v>1650</v>
       </c>
     </row>
@@ -21239,97 +21281,97 @@
     </row>
     <row r="2" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
-      <c r="B2" s="196" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="196" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="196" t="s">
+      <c r="B2" s="200" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="200" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="200" t="s">
         <v>130</v>
       </c>
-      <c r="E2" s="198" t="s">
+      <c r="E2" s="202" t="s">
         <v>723</v>
       </c>
-      <c r="F2" s="193" t="s">
+      <c r="F2" s="196" t="s">
         <v>651</v>
       </c>
-      <c r="G2" s="194"/>
-      <c r="H2" s="194"/>
-      <c r="I2" s="195"/>
-      <c r="J2" s="193" t="s">
+      <c r="G2" s="197"/>
+      <c r="H2" s="197"/>
+      <c r="I2" s="198"/>
+      <c r="J2" s="196" t="s">
         <v>652</v>
       </c>
-      <c r="K2" s="194"/>
-      <c r="L2" s="194"/>
-      <c r="M2" s="195"/>
-      <c r="N2" s="193" t="s">
+      <c r="K2" s="197"/>
+      <c r="L2" s="197"/>
+      <c r="M2" s="198"/>
+      <c r="N2" s="196" t="s">
         <v>653</v>
       </c>
-      <c r="O2" s="194"/>
-      <c r="P2" s="194"/>
-      <c r="Q2" s="195"/>
-      <c r="R2" s="193" t="s">
+      <c r="O2" s="197"/>
+      <c r="P2" s="197"/>
+      <c r="Q2" s="198"/>
+      <c r="R2" s="196" t="s">
         <v>654</v>
       </c>
-      <c r="S2" s="194"/>
-      <c r="T2" s="194"/>
-      <c r="U2" s="203"/>
-      <c r="V2" s="193" t="s">
+      <c r="S2" s="197"/>
+      <c r="T2" s="197"/>
+      <c r="U2" s="199"/>
+      <c r="V2" s="196" t="s">
         <v>655</v>
       </c>
-      <c r="W2" s="194"/>
-      <c r="X2" s="194"/>
-      <c r="Y2" s="203"/>
-      <c r="Z2" s="200" t="s">
+      <c r="W2" s="197"/>
+      <c r="X2" s="197"/>
+      <c r="Y2" s="199"/>
+      <c r="Z2" s="193" t="s">
         <v>656</v>
       </c>
-      <c r="AA2" s="201"/>
-      <c r="AB2" s="201"/>
-      <c r="AC2" s="202"/>
-      <c r="AD2" s="200" t="s">
+      <c r="AA2" s="194"/>
+      <c r="AB2" s="194"/>
+      <c r="AC2" s="195"/>
+      <c r="AD2" s="193" t="s">
         <v>657</v>
       </c>
-      <c r="AE2" s="201"/>
-      <c r="AF2" s="201"/>
-      <c r="AG2" s="202"/>
-      <c r="AH2" s="200" t="s">
+      <c r="AE2" s="194"/>
+      <c r="AF2" s="194"/>
+      <c r="AG2" s="195"/>
+      <c r="AH2" s="193" t="s">
         <v>658</v>
       </c>
-      <c r="AI2" s="201"/>
-      <c r="AJ2" s="201"/>
-      <c r="AK2" s="202"/>
-      <c r="AL2" s="200" t="s">
+      <c r="AI2" s="194"/>
+      <c r="AJ2" s="194"/>
+      <c r="AK2" s="195"/>
+      <c r="AL2" s="193" t="s">
         <v>659</v>
       </c>
-      <c r="AM2" s="201"/>
-      <c r="AN2" s="201"/>
-      <c r="AO2" s="202"/>
-      <c r="AP2" s="200" t="s">
+      <c r="AM2" s="194"/>
+      <c r="AN2" s="194"/>
+      <c r="AO2" s="195"/>
+      <c r="AP2" s="193" t="s">
         <v>660</v>
       </c>
-      <c r="AQ2" s="201"/>
-      <c r="AR2" s="201"/>
-      <c r="AS2" s="202"/>
-      <c r="AT2" s="200" t="s">
+      <c r="AQ2" s="194"/>
+      <c r="AR2" s="194"/>
+      <c r="AS2" s="195"/>
+      <c r="AT2" s="193" t="s">
         <v>722</v>
       </c>
-      <c r="AU2" s="201"/>
-      <c r="AV2" s="201"/>
-      <c r="AW2" s="202"/>
-      <c r="AX2" s="200" t="s">
+      <c r="AU2" s="194"/>
+      <c r="AV2" s="194"/>
+      <c r="AW2" s="195"/>
+      <c r="AX2" s="193" t="s">
         <v>729</v>
       </c>
-      <c r="AY2" s="201"/>
-      <c r="AZ2" s="201"/>
-      <c r="BA2" s="202"/>
+      <c r="AY2" s="194"/>
+      <c r="AZ2" s="194"/>
+      <c r="BA2" s="195"/>
     </row>
     <row r="3" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
-      <c r="B3" s="197"/>
-      <c r="C3" s="197"/>
-      <c r="D3" s="197"/>
-      <c r="E3" s="199"/>
+      <c r="B3" s="201"/>
+      <c r="C3" s="201"/>
+      <c r="D3" s="201"/>
+      <c r="E3" s="203"/>
       <c r="F3" s="80">
         <v>1</v>
       </c>
@@ -26483,6 +26525,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:I2"/>
     <mergeCell ref="AL2:AO2"/>
     <mergeCell ref="AP2:AS2"/>
     <mergeCell ref="AT2:AW2"/>
@@ -26493,12 +26541,6 @@
     <mergeCell ref="Z2:AC2"/>
     <mergeCell ref="AD2:AG2"/>
     <mergeCell ref="AH2:AK2"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:I2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D84" location="ลูกค้า!A1" display="ลูกค้า!A1"/>
@@ -27016,16 +27058,16 @@
     <row r="2" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
-      <c r="C2" s="196" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="196" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="196" t="s">
+      <c r="C2" s="200" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="200" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="200" t="s">
         <v>130</v>
       </c>
-      <c r="F2" s="198" t="s">
+      <c r="F2" s="202" t="s">
         <v>723</v>
       </c>
       <c r="G2" s="204" t="s">
@@ -27092,10 +27134,10 @@
     <row r="3" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
-      <c r="C3" s="197"/>
-      <c r="D3" s="197"/>
-      <c r="E3" s="197"/>
-      <c r="F3" s="199"/>
+      <c r="C3" s="201"/>
+      <c r="D3" s="201"/>
+      <c r="E3" s="201"/>
+      <c r="F3" s="203"/>
       <c r="G3" s="80">
         <v>1</v>
       </c>
@@ -32891,6 +32933,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="AE2:AH2"/>
+    <mergeCell ref="AI2:AL2"/>
+    <mergeCell ref="AM2:AP2"/>
+    <mergeCell ref="AQ2:AT2"/>
+    <mergeCell ref="AA2:AD2"/>
     <mergeCell ref="K2:N2"/>
     <mergeCell ref="O2:R2"/>
     <mergeCell ref="S2:V2"/>
@@ -32900,11 +32947,6 @@
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="G2:J2"/>
-    <mergeCell ref="AE2:AH2"/>
-    <mergeCell ref="AI2:AL2"/>
-    <mergeCell ref="AM2:AP2"/>
-    <mergeCell ref="AQ2:AT2"/>
-    <mergeCell ref="AA2:AD2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E84" location="ลูกค้า!A1" display="ลูกค้า!A1"/>
@@ -33382,98 +33424,98 @@
     <row r="2" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
-      <c r="C2" s="196" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="196" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="196" t="s">
+      <c r="C2" s="200" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="200" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="200" t="s">
         <v>130</v>
       </c>
-      <c r="F2" s="198" t="s">
+      <c r="F2" s="202" t="s">
         <v>723</v>
       </c>
-      <c r="G2" s="193" t="s">
+      <c r="G2" s="196" t="s">
         <v>651</v>
       </c>
-      <c r="H2" s="194"/>
-      <c r="I2" s="194"/>
-      <c r="J2" s="195"/>
-      <c r="K2" s="193" t="s">
+      <c r="H2" s="197"/>
+      <c r="I2" s="197"/>
+      <c r="J2" s="198"/>
+      <c r="K2" s="196" t="s">
         <v>652</v>
       </c>
-      <c r="L2" s="194"/>
-      <c r="M2" s="194"/>
-      <c r="N2" s="195"/>
-      <c r="O2" s="193" t="s">
+      <c r="L2" s="197"/>
+      <c r="M2" s="197"/>
+      <c r="N2" s="198"/>
+      <c r="O2" s="196" t="s">
         <v>653</v>
       </c>
-      <c r="P2" s="194"/>
-      <c r="Q2" s="194"/>
-      <c r="R2" s="195"/>
-      <c r="S2" s="193" t="s">
+      <c r="P2" s="197"/>
+      <c r="Q2" s="197"/>
+      <c r="R2" s="198"/>
+      <c r="S2" s="196" t="s">
         <v>654</v>
       </c>
-      <c r="T2" s="194"/>
-      <c r="U2" s="194"/>
-      <c r="V2" s="203"/>
-      <c r="W2" s="193" t="s">
+      <c r="T2" s="197"/>
+      <c r="U2" s="197"/>
+      <c r="V2" s="199"/>
+      <c r="W2" s="196" t="s">
         <v>655</v>
       </c>
-      <c r="X2" s="194"/>
-      <c r="Y2" s="194"/>
-      <c r="Z2" s="203"/>
-      <c r="AA2" s="200" t="s">
+      <c r="X2" s="197"/>
+      <c r="Y2" s="197"/>
+      <c r="Z2" s="199"/>
+      <c r="AA2" s="193" t="s">
         <v>656</v>
       </c>
-      <c r="AB2" s="201"/>
-      <c r="AC2" s="201"/>
-      <c r="AD2" s="202"/>
-      <c r="AE2" s="200" t="s">
+      <c r="AB2" s="194"/>
+      <c r="AC2" s="194"/>
+      <c r="AD2" s="195"/>
+      <c r="AE2" s="193" t="s">
         <v>657</v>
       </c>
-      <c r="AF2" s="201"/>
-      <c r="AG2" s="201"/>
-      <c r="AH2" s="202"/>
-      <c r="AI2" s="200" t="s">
+      <c r="AF2" s="194"/>
+      <c r="AG2" s="194"/>
+      <c r="AH2" s="195"/>
+      <c r="AI2" s="193" t="s">
         <v>658</v>
       </c>
-      <c r="AJ2" s="201"/>
-      <c r="AK2" s="201"/>
-      <c r="AL2" s="202"/>
-      <c r="AM2" s="200" t="s">
+      <c r="AJ2" s="194"/>
+      <c r="AK2" s="194"/>
+      <c r="AL2" s="195"/>
+      <c r="AM2" s="193" t="s">
         <v>659</v>
       </c>
-      <c r="AN2" s="201"/>
-      <c r="AO2" s="201"/>
-      <c r="AP2" s="202"/>
-      <c r="AQ2" s="200" t="s">
+      <c r="AN2" s="194"/>
+      <c r="AO2" s="194"/>
+      <c r="AP2" s="195"/>
+      <c r="AQ2" s="193" t="s">
         <v>660</v>
       </c>
-      <c r="AR2" s="201"/>
-      <c r="AS2" s="201"/>
-      <c r="AT2" s="202"/>
-      <c r="AU2" s="200" t="s">
+      <c r="AR2" s="194"/>
+      <c r="AS2" s="194"/>
+      <c r="AT2" s="195"/>
+      <c r="AU2" s="193" t="s">
         <v>722</v>
       </c>
-      <c r="AV2" s="201"/>
-      <c r="AW2" s="201"/>
-      <c r="AX2" s="202"/>
-      <c r="AY2" s="200" t="s">
+      <c r="AV2" s="194"/>
+      <c r="AW2" s="194"/>
+      <c r="AX2" s="195"/>
+      <c r="AY2" s="193" t="s">
         <v>729</v>
       </c>
-      <c r="AZ2" s="201"/>
-      <c r="BA2" s="201"/>
-      <c r="BB2" s="202"/>
+      <c r="AZ2" s="194"/>
+      <c r="BA2" s="194"/>
+      <c r="BB2" s="195"/>
     </row>
     <row r="3" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
-      <c r="C3" s="197"/>
-      <c r="D3" s="197"/>
-      <c r="E3" s="197"/>
-      <c r="F3" s="199"/>
+      <c r="C3" s="201"/>
+      <c r="D3" s="201"/>
+      <c r="E3" s="201"/>
+      <c r="F3" s="203"/>
       <c r="G3" s="80">
         <v>1</v>
       </c>
@@ -38886,11 +38928,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="O2:R2"/>
     <mergeCell ref="AU2:AX2"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="AY2:BB2"/>
@@ -38902,6 +38939,11 @@
     <mergeCell ref="AM2:AP2"/>
     <mergeCell ref="AQ2:AT2"/>
     <mergeCell ref="S2:V2"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="O2:R2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E84" location="ลูกค้า!A1" display="ลูกค้า!A1"/>
@@ -39092,7 +39134,7 @@
       <c r="A1" s="210" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="196" t="s">
+      <c r="B1" s="200" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="212" t="s">
@@ -39120,7 +39162,7 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="211"/>
-      <c r="B2" s="197"/>
+      <c r="B2" s="201"/>
       <c r="C2" s="1">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
save prolist with isdelete modifi save stock
</commit_message>
<xml_diff>
--- a/_Doc/Feature.xlsx
+++ b/_Doc/Feature.xlsx
@@ -56,7 +56,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Menu!$A$1:$R$57</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -5658,7 +5658,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="46" x14ac:knownFonts="1">
     <font>
@@ -6271,7 +6271,7 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
@@ -6355,20 +6355,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="1" fillId="6" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
@@ -6536,11 +6536,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="43" fontId="29" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="43" fontId="14" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -6627,6 +6627,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -6634,6 +6643,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -6647,18 +6659,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -7523,20 +7523,20 @@
       <c r="B1" s="2"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="196" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="196" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="196" t="s">
+      <c r="A2" s="200" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="200" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="200" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="197"/>
-      <c r="B3" s="197"/>
-      <c r="C3" s="197"/>
+      <c r="A3" s="201"/>
+      <c r="B3" s="201"/>
+      <c r="C3" s="201"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
@@ -8738,12 +8738,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
     <mergeCell ref="B43:C43"/>
     <mergeCell ref="B44:C44"/>
     <mergeCell ref="B45:C45"/>
@@ -8754,6 +8748,12 @@
     <mergeCell ref="B40:C40"/>
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -10668,8 +10668,8 @@
   </sheetPr>
   <dimension ref="A1:C372"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A345" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C353" sqref="C353"/>
+    <sheetView tabSelected="1" topLeftCell="A339" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C348" sqref="C348"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21.75" x14ac:dyDescent="0.5"/>
@@ -21289,97 +21289,97 @@
     </row>
     <row r="2" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
-      <c r="B2" s="196" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="196" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="196" t="s">
+      <c r="B2" s="200" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="200" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="200" t="s">
         <v>130</v>
       </c>
-      <c r="E2" s="198" t="s">
+      <c r="E2" s="202" t="s">
         <v>723</v>
       </c>
-      <c r="F2" s="193" t="s">
+      <c r="F2" s="196" t="s">
         <v>651</v>
       </c>
-      <c r="G2" s="194"/>
-      <c r="H2" s="194"/>
-      <c r="I2" s="195"/>
-      <c r="J2" s="193" t="s">
+      <c r="G2" s="197"/>
+      <c r="H2" s="197"/>
+      <c r="I2" s="198"/>
+      <c r="J2" s="196" t="s">
         <v>652</v>
       </c>
-      <c r="K2" s="194"/>
-      <c r="L2" s="194"/>
-      <c r="M2" s="195"/>
-      <c r="N2" s="193" t="s">
+      <c r="K2" s="197"/>
+      <c r="L2" s="197"/>
+      <c r="M2" s="198"/>
+      <c r="N2" s="196" t="s">
         <v>653</v>
       </c>
-      <c r="O2" s="194"/>
-      <c r="P2" s="194"/>
-      <c r="Q2" s="195"/>
-      <c r="R2" s="193" t="s">
+      <c r="O2" s="197"/>
+      <c r="P2" s="197"/>
+      <c r="Q2" s="198"/>
+      <c r="R2" s="196" t="s">
         <v>654</v>
       </c>
-      <c r="S2" s="194"/>
-      <c r="T2" s="194"/>
-      <c r="U2" s="203"/>
-      <c r="V2" s="193" t="s">
+      <c r="S2" s="197"/>
+      <c r="T2" s="197"/>
+      <c r="U2" s="199"/>
+      <c r="V2" s="196" t="s">
         <v>655</v>
       </c>
-      <c r="W2" s="194"/>
-      <c r="X2" s="194"/>
-      <c r="Y2" s="203"/>
-      <c r="Z2" s="200" t="s">
+      <c r="W2" s="197"/>
+      <c r="X2" s="197"/>
+      <c r="Y2" s="199"/>
+      <c r="Z2" s="193" t="s">
         <v>656</v>
       </c>
-      <c r="AA2" s="201"/>
-      <c r="AB2" s="201"/>
-      <c r="AC2" s="202"/>
-      <c r="AD2" s="200" t="s">
+      <c r="AA2" s="194"/>
+      <c r="AB2" s="194"/>
+      <c r="AC2" s="195"/>
+      <c r="AD2" s="193" t="s">
         <v>657</v>
       </c>
-      <c r="AE2" s="201"/>
-      <c r="AF2" s="201"/>
-      <c r="AG2" s="202"/>
-      <c r="AH2" s="200" t="s">
+      <c r="AE2" s="194"/>
+      <c r="AF2" s="194"/>
+      <c r="AG2" s="195"/>
+      <c r="AH2" s="193" t="s">
         <v>658</v>
       </c>
-      <c r="AI2" s="201"/>
-      <c r="AJ2" s="201"/>
-      <c r="AK2" s="202"/>
-      <c r="AL2" s="200" t="s">
+      <c r="AI2" s="194"/>
+      <c r="AJ2" s="194"/>
+      <c r="AK2" s="195"/>
+      <c r="AL2" s="193" t="s">
         <v>659</v>
       </c>
-      <c r="AM2" s="201"/>
-      <c r="AN2" s="201"/>
-      <c r="AO2" s="202"/>
-      <c r="AP2" s="200" t="s">
+      <c r="AM2" s="194"/>
+      <c r="AN2" s="194"/>
+      <c r="AO2" s="195"/>
+      <c r="AP2" s="193" t="s">
         <v>660</v>
       </c>
-      <c r="AQ2" s="201"/>
-      <c r="AR2" s="201"/>
-      <c r="AS2" s="202"/>
-      <c r="AT2" s="200" t="s">
+      <c r="AQ2" s="194"/>
+      <c r="AR2" s="194"/>
+      <c r="AS2" s="195"/>
+      <c r="AT2" s="193" t="s">
         <v>722</v>
       </c>
-      <c r="AU2" s="201"/>
-      <c r="AV2" s="201"/>
-      <c r="AW2" s="202"/>
-      <c r="AX2" s="200" t="s">
+      <c r="AU2" s="194"/>
+      <c r="AV2" s="194"/>
+      <c r="AW2" s="195"/>
+      <c r="AX2" s="193" t="s">
         <v>729</v>
       </c>
-      <c r="AY2" s="201"/>
-      <c r="AZ2" s="201"/>
-      <c r="BA2" s="202"/>
+      <c r="AY2" s="194"/>
+      <c r="AZ2" s="194"/>
+      <c r="BA2" s="195"/>
     </row>
     <row r="3" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
-      <c r="B3" s="197"/>
-      <c r="C3" s="197"/>
-      <c r="D3" s="197"/>
-      <c r="E3" s="199"/>
+      <c r="B3" s="201"/>
+      <c r="C3" s="201"/>
+      <c r="D3" s="201"/>
+      <c r="E3" s="203"/>
       <c r="F3" s="80">
         <v>1</v>
       </c>
@@ -26533,6 +26533,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:I2"/>
     <mergeCell ref="AL2:AO2"/>
     <mergeCell ref="AP2:AS2"/>
     <mergeCell ref="AT2:AW2"/>
@@ -26543,12 +26549,6 @@
     <mergeCell ref="Z2:AC2"/>
     <mergeCell ref="AD2:AG2"/>
     <mergeCell ref="AH2:AK2"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:I2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D84" location="ลูกค้า!A1" display="ลูกค้า!A1"/>
@@ -27066,16 +27066,16 @@
     <row r="2" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
-      <c r="C2" s="196" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="196" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="196" t="s">
+      <c r="C2" s="200" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="200" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="200" t="s">
         <v>130</v>
       </c>
-      <c r="F2" s="198" t="s">
+      <c r="F2" s="202" t="s">
         <v>723</v>
       </c>
       <c r="G2" s="204" t="s">
@@ -27142,10 +27142,10 @@
     <row r="3" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
-      <c r="C3" s="197"/>
-      <c r="D3" s="197"/>
-      <c r="E3" s="197"/>
-      <c r="F3" s="199"/>
+      <c r="C3" s="201"/>
+      <c r="D3" s="201"/>
+      <c r="E3" s="201"/>
+      <c r="F3" s="203"/>
       <c r="G3" s="80">
         <v>1</v>
       </c>
@@ -32941,6 +32941,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="AE2:AH2"/>
+    <mergeCell ref="AI2:AL2"/>
+    <mergeCell ref="AM2:AP2"/>
+    <mergeCell ref="AQ2:AT2"/>
+    <mergeCell ref="AA2:AD2"/>
     <mergeCell ref="K2:N2"/>
     <mergeCell ref="O2:R2"/>
     <mergeCell ref="S2:V2"/>
@@ -32950,11 +32955,6 @@
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="G2:J2"/>
-    <mergeCell ref="AE2:AH2"/>
-    <mergeCell ref="AI2:AL2"/>
-    <mergeCell ref="AM2:AP2"/>
-    <mergeCell ref="AQ2:AT2"/>
-    <mergeCell ref="AA2:AD2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E84" location="ลูกค้า!A1" display="ลูกค้า!A1"/>
@@ -33432,98 +33432,98 @@
     <row r="2" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
-      <c r="C2" s="196" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="196" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="196" t="s">
+      <c r="C2" s="200" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="200" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="200" t="s">
         <v>130</v>
       </c>
-      <c r="F2" s="198" t="s">
+      <c r="F2" s="202" t="s">
         <v>723</v>
       </c>
-      <c r="G2" s="193" t="s">
+      <c r="G2" s="196" t="s">
         <v>651</v>
       </c>
-      <c r="H2" s="194"/>
-      <c r="I2" s="194"/>
-      <c r="J2" s="195"/>
-      <c r="K2" s="193" t="s">
+      <c r="H2" s="197"/>
+      <c r="I2" s="197"/>
+      <c r="J2" s="198"/>
+      <c r="K2" s="196" t="s">
         <v>652</v>
       </c>
-      <c r="L2" s="194"/>
-      <c r="M2" s="194"/>
-      <c r="N2" s="195"/>
-      <c r="O2" s="193" t="s">
+      <c r="L2" s="197"/>
+      <c r="M2" s="197"/>
+      <c r="N2" s="198"/>
+      <c r="O2" s="196" t="s">
         <v>653</v>
       </c>
-      <c r="P2" s="194"/>
-      <c r="Q2" s="194"/>
-      <c r="R2" s="195"/>
-      <c r="S2" s="193" t="s">
+      <c r="P2" s="197"/>
+      <c r="Q2" s="197"/>
+      <c r="R2" s="198"/>
+      <c r="S2" s="196" t="s">
         <v>654</v>
       </c>
-      <c r="T2" s="194"/>
-      <c r="U2" s="194"/>
-      <c r="V2" s="203"/>
-      <c r="W2" s="193" t="s">
+      <c r="T2" s="197"/>
+      <c r="U2" s="197"/>
+      <c r="V2" s="199"/>
+      <c r="W2" s="196" t="s">
         <v>655</v>
       </c>
-      <c r="X2" s="194"/>
-      <c r="Y2" s="194"/>
-      <c r="Z2" s="203"/>
-      <c r="AA2" s="200" t="s">
+      <c r="X2" s="197"/>
+      <c r="Y2" s="197"/>
+      <c r="Z2" s="199"/>
+      <c r="AA2" s="193" t="s">
         <v>656</v>
       </c>
-      <c r="AB2" s="201"/>
-      <c r="AC2" s="201"/>
-      <c r="AD2" s="202"/>
-      <c r="AE2" s="200" t="s">
+      <c r="AB2" s="194"/>
+      <c r="AC2" s="194"/>
+      <c r="AD2" s="195"/>
+      <c r="AE2" s="193" t="s">
         <v>657</v>
       </c>
-      <c r="AF2" s="201"/>
-      <c r="AG2" s="201"/>
-      <c r="AH2" s="202"/>
-      <c r="AI2" s="200" t="s">
+      <c r="AF2" s="194"/>
+      <c r="AG2" s="194"/>
+      <c r="AH2" s="195"/>
+      <c r="AI2" s="193" t="s">
         <v>658</v>
       </c>
-      <c r="AJ2" s="201"/>
-      <c r="AK2" s="201"/>
-      <c r="AL2" s="202"/>
-      <c r="AM2" s="200" t="s">
+      <c r="AJ2" s="194"/>
+      <c r="AK2" s="194"/>
+      <c r="AL2" s="195"/>
+      <c r="AM2" s="193" t="s">
         <v>659</v>
       </c>
-      <c r="AN2" s="201"/>
-      <c r="AO2" s="201"/>
-      <c r="AP2" s="202"/>
-      <c r="AQ2" s="200" t="s">
+      <c r="AN2" s="194"/>
+      <c r="AO2" s="194"/>
+      <c r="AP2" s="195"/>
+      <c r="AQ2" s="193" t="s">
         <v>660</v>
       </c>
-      <c r="AR2" s="201"/>
-      <c r="AS2" s="201"/>
-      <c r="AT2" s="202"/>
-      <c r="AU2" s="200" t="s">
+      <c r="AR2" s="194"/>
+      <c r="AS2" s="194"/>
+      <c r="AT2" s="195"/>
+      <c r="AU2" s="193" t="s">
         <v>722</v>
       </c>
-      <c r="AV2" s="201"/>
-      <c r="AW2" s="201"/>
-      <c r="AX2" s="202"/>
-      <c r="AY2" s="200" t="s">
+      <c r="AV2" s="194"/>
+      <c r="AW2" s="194"/>
+      <c r="AX2" s="195"/>
+      <c r="AY2" s="193" t="s">
         <v>729</v>
       </c>
-      <c r="AZ2" s="201"/>
-      <c r="BA2" s="201"/>
-      <c r="BB2" s="202"/>
+      <c r="AZ2" s="194"/>
+      <c r="BA2" s="194"/>
+      <c r="BB2" s="195"/>
     </row>
     <row r="3" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
-      <c r="C3" s="197"/>
-      <c r="D3" s="197"/>
-      <c r="E3" s="197"/>
-      <c r="F3" s="199"/>
+      <c r="C3" s="201"/>
+      <c r="D3" s="201"/>
+      <c r="E3" s="201"/>
+      <c r="F3" s="203"/>
       <c r="G3" s="80">
         <v>1</v>
       </c>
@@ -38936,11 +38936,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="O2:R2"/>
     <mergeCell ref="AU2:AX2"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="AY2:BB2"/>
@@ -38952,6 +38947,11 @@
     <mergeCell ref="AM2:AP2"/>
     <mergeCell ref="AQ2:AT2"/>
     <mergeCell ref="S2:V2"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="O2:R2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E84" location="ลูกค้า!A1" display="ลูกค้า!A1"/>
@@ -39142,7 +39142,7 @@
       <c r="A1" s="210" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="196" t="s">
+      <c r="B1" s="200" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="212" t="s">
@@ -39170,7 +39170,7 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="211"/>
-      <c r="B2" s="197"/>
+      <c r="B2" s="201"/>
       <c r="C2" s="1">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
update stock by mainunit
</commit_message>
<xml_diff>
--- a/_Doc/Feature.xlsx
+++ b/_Doc/Feature.xlsx
@@ -56,7 +56,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Menu!$A$1:$R$57</definedName>
   </definedNames>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -226,7 +226,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2416" uniqueCount="1694">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2417" uniqueCount="1695">
   <si>
     <t>No.</t>
   </si>
@@ -5651,6 +5651,9 @@
   </si>
   <si>
     <t>หน้ารายการรวม เพิ่มคอลัมรหัสลูกค้า</t>
+  </si>
+  <si>
+    <t>หน้าข้อมูลจังหวัด</t>
   </si>
 </sst>
 </file>
@@ -6627,15 +6630,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -6643,9 +6637,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -6659,6 +6650,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -7523,20 +7526,20 @@
       <c r="B1" s="2"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="200" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="200" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="200" t="s">
+      <c r="A2" s="196" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="196" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="196" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="201"/>
-      <c r="B3" s="201"/>
-      <c r="C3" s="201"/>
+      <c r="A3" s="197"/>
+      <c r="B3" s="197"/>
+      <c r="C3" s="197"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
@@ -8738,6 +8741,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
     <mergeCell ref="B43:C43"/>
     <mergeCell ref="B44:C44"/>
     <mergeCell ref="B45:C45"/>
@@ -8748,12 +8757,6 @@
     <mergeCell ref="B40:C40"/>
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -10668,8 +10671,8 @@
   </sheetPr>
   <dimension ref="A1:C372"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A339" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C348" sqref="C348"/>
+    <sheetView tabSelected="1" topLeftCell="A342" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B356" sqref="B356"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21.75" x14ac:dyDescent="0.5"/>
@@ -12661,6 +12664,11 @@
     <row r="354" spans="2:2" x14ac:dyDescent="0.5">
       <c r="B354" s="151" t="s">
         <v>1693</v>
+      </c>
+    </row>
+    <row r="355" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B355" s="151" t="s">
+        <v>1694</v>
       </c>
     </row>
     <row r="357" spans="2:2" x14ac:dyDescent="0.5">
@@ -21289,97 +21297,97 @@
     </row>
     <row r="2" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
-      <c r="B2" s="200" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="200" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="200" t="s">
+      <c r="B2" s="196" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="196" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="196" t="s">
         <v>130</v>
       </c>
-      <c r="E2" s="202" t="s">
+      <c r="E2" s="198" t="s">
         <v>723</v>
       </c>
-      <c r="F2" s="196" t="s">
+      <c r="F2" s="193" t="s">
         <v>651</v>
       </c>
-      <c r="G2" s="197"/>
-      <c r="H2" s="197"/>
-      <c r="I2" s="198"/>
-      <c r="J2" s="196" t="s">
+      <c r="G2" s="194"/>
+      <c r="H2" s="194"/>
+      <c r="I2" s="195"/>
+      <c r="J2" s="193" t="s">
         <v>652</v>
       </c>
-      <c r="K2" s="197"/>
-      <c r="L2" s="197"/>
-      <c r="M2" s="198"/>
-      <c r="N2" s="196" t="s">
+      <c r="K2" s="194"/>
+      <c r="L2" s="194"/>
+      <c r="M2" s="195"/>
+      <c r="N2" s="193" t="s">
         <v>653</v>
       </c>
-      <c r="O2" s="197"/>
-      <c r="P2" s="197"/>
-      <c r="Q2" s="198"/>
-      <c r="R2" s="196" t="s">
+      <c r="O2" s="194"/>
+      <c r="P2" s="194"/>
+      <c r="Q2" s="195"/>
+      <c r="R2" s="193" t="s">
         <v>654</v>
       </c>
-      <c r="S2" s="197"/>
-      <c r="T2" s="197"/>
-      <c r="U2" s="199"/>
-      <c r="V2" s="196" t="s">
+      <c r="S2" s="194"/>
+      <c r="T2" s="194"/>
+      <c r="U2" s="203"/>
+      <c r="V2" s="193" t="s">
         <v>655</v>
       </c>
-      <c r="W2" s="197"/>
-      <c r="X2" s="197"/>
-      <c r="Y2" s="199"/>
-      <c r="Z2" s="193" t="s">
+      <c r="W2" s="194"/>
+      <c r="X2" s="194"/>
+      <c r="Y2" s="203"/>
+      <c r="Z2" s="200" t="s">
         <v>656</v>
       </c>
-      <c r="AA2" s="194"/>
-      <c r="AB2" s="194"/>
-      <c r="AC2" s="195"/>
-      <c r="AD2" s="193" t="s">
+      <c r="AA2" s="201"/>
+      <c r="AB2" s="201"/>
+      <c r="AC2" s="202"/>
+      <c r="AD2" s="200" t="s">
         <v>657</v>
       </c>
-      <c r="AE2" s="194"/>
-      <c r="AF2" s="194"/>
-      <c r="AG2" s="195"/>
-      <c r="AH2" s="193" t="s">
+      <c r="AE2" s="201"/>
+      <c r="AF2" s="201"/>
+      <c r="AG2" s="202"/>
+      <c r="AH2" s="200" t="s">
         <v>658</v>
       </c>
-      <c r="AI2" s="194"/>
-      <c r="AJ2" s="194"/>
-      <c r="AK2" s="195"/>
-      <c r="AL2" s="193" t="s">
+      <c r="AI2" s="201"/>
+      <c r="AJ2" s="201"/>
+      <c r="AK2" s="202"/>
+      <c r="AL2" s="200" t="s">
         <v>659</v>
       </c>
-      <c r="AM2" s="194"/>
-      <c r="AN2" s="194"/>
-      <c r="AO2" s="195"/>
-      <c r="AP2" s="193" t="s">
+      <c r="AM2" s="201"/>
+      <c r="AN2" s="201"/>
+      <c r="AO2" s="202"/>
+      <c r="AP2" s="200" t="s">
         <v>660</v>
       </c>
-      <c r="AQ2" s="194"/>
-      <c r="AR2" s="194"/>
-      <c r="AS2" s="195"/>
-      <c r="AT2" s="193" t="s">
+      <c r="AQ2" s="201"/>
+      <c r="AR2" s="201"/>
+      <c r="AS2" s="202"/>
+      <c r="AT2" s="200" t="s">
         <v>722</v>
       </c>
-      <c r="AU2" s="194"/>
-      <c r="AV2" s="194"/>
-      <c r="AW2" s="195"/>
-      <c r="AX2" s="193" t="s">
+      <c r="AU2" s="201"/>
+      <c r="AV2" s="201"/>
+      <c r="AW2" s="202"/>
+      <c r="AX2" s="200" t="s">
         <v>729</v>
       </c>
-      <c r="AY2" s="194"/>
-      <c r="AZ2" s="194"/>
-      <c r="BA2" s="195"/>
+      <c r="AY2" s="201"/>
+      <c r="AZ2" s="201"/>
+      <c r="BA2" s="202"/>
     </row>
     <row r="3" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
-      <c r="B3" s="201"/>
-      <c r="C3" s="201"/>
-      <c r="D3" s="201"/>
-      <c r="E3" s="203"/>
+      <c r="B3" s="197"/>
+      <c r="C3" s="197"/>
+      <c r="D3" s="197"/>
+      <c r="E3" s="199"/>
       <c r="F3" s="80">
         <v>1</v>
       </c>
@@ -26533,12 +26541,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:I2"/>
     <mergeCell ref="AL2:AO2"/>
     <mergeCell ref="AP2:AS2"/>
     <mergeCell ref="AT2:AW2"/>
@@ -26549,6 +26551,12 @@
     <mergeCell ref="Z2:AC2"/>
     <mergeCell ref="AD2:AG2"/>
     <mergeCell ref="AH2:AK2"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:I2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D84" location="ลูกค้า!A1" display="ลูกค้า!A1"/>
@@ -27066,16 +27074,16 @@
     <row r="2" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
-      <c r="C2" s="200" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="200" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="200" t="s">
+      <c r="C2" s="196" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="196" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="196" t="s">
         <v>130</v>
       </c>
-      <c r="F2" s="202" t="s">
+      <c r="F2" s="198" t="s">
         <v>723</v>
       </c>
       <c r="G2" s="204" t="s">
@@ -27142,10 +27150,10 @@
     <row r="3" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
-      <c r="C3" s="201"/>
-      <c r="D3" s="201"/>
-      <c r="E3" s="201"/>
-      <c r="F3" s="203"/>
+      <c r="C3" s="197"/>
+      <c r="D3" s="197"/>
+      <c r="E3" s="197"/>
+      <c r="F3" s="199"/>
       <c r="G3" s="80">
         <v>1</v>
       </c>
@@ -32941,11 +32949,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="AE2:AH2"/>
-    <mergeCell ref="AI2:AL2"/>
-    <mergeCell ref="AM2:AP2"/>
-    <mergeCell ref="AQ2:AT2"/>
-    <mergeCell ref="AA2:AD2"/>
     <mergeCell ref="K2:N2"/>
     <mergeCell ref="O2:R2"/>
     <mergeCell ref="S2:V2"/>
@@ -32955,6 +32958,11 @@
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="G2:J2"/>
+    <mergeCell ref="AE2:AH2"/>
+    <mergeCell ref="AI2:AL2"/>
+    <mergeCell ref="AM2:AP2"/>
+    <mergeCell ref="AQ2:AT2"/>
+    <mergeCell ref="AA2:AD2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E84" location="ลูกค้า!A1" display="ลูกค้า!A1"/>
@@ -33432,98 +33440,98 @@
     <row r="2" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
-      <c r="C2" s="200" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="200" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="200" t="s">
+      <c r="C2" s="196" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="196" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="196" t="s">
         <v>130</v>
       </c>
-      <c r="F2" s="202" t="s">
+      <c r="F2" s="198" t="s">
         <v>723</v>
       </c>
-      <c r="G2" s="196" t="s">
+      <c r="G2" s="193" t="s">
         <v>651</v>
       </c>
-      <c r="H2" s="197"/>
-      <c r="I2" s="197"/>
-      <c r="J2" s="198"/>
-      <c r="K2" s="196" t="s">
+      <c r="H2" s="194"/>
+      <c r="I2" s="194"/>
+      <c r="J2" s="195"/>
+      <c r="K2" s="193" t="s">
         <v>652</v>
       </c>
-      <c r="L2" s="197"/>
-      <c r="M2" s="197"/>
-      <c r="N2" s="198"/>
-      <c r="O2" s="196" t="s">
+      <c r="L2" s="194"/>
+      <c r="M2" s="194"/>
+      <c r="N2" s="195"/>
+      <c r="O2" s="193" t="s">
         <v>653</v>
       </c>
-      <c r="P2" s="197"/>
-      <c r="Q2" s="197"/>
-      <c r="R2" s="198"/>
-      <c r="S2" s="196" t="s">
+      <c r="P2" s="194"/>
+      <c r="Q2" s="194"/>
+      <c r="R2" s="195"/>
+      <c r="S2" s="193" t="s">
         <v>654</v>
       </c>
-      <c r="T2" s="197"/>
-      <c r="U2" s="197"/>
-      <c r="V2" s="199"/>
-      <c r="W2" s="196" t="s">
+      <c r="T2" s="194"/>
+      <c r="U2" s="194"/>
+      <c r="V2" s="203"/>
+      <c r="W2" s="193" t="s">
         <v>655</v>
       </c>
-      <c r="X2" s="197"/>
-      <c r="Y2" s="197"/>
-      <c r="Z2" s="199"/>
-      <c r="AA2" s="193" t="s">
+      <c r="X2" s="194"/>
+      <c r="Y2" s="194"/>
+      <c r="Z2" s="203"/>
+      <c r="AA2" s="200" t="s">
         <v>656</v>
       </c>
-      <c r="AB2" s="194"/>
-      <c r="AC2" s="194"/>
-      <c r="AD2" s="195"/>
-      <c r="AE2" s="193" t="s">
+      <c r="AB2" s="201"/>
+      <c r="AC2" s="201"/>
+      <c r="AD2" s="202"/>
+      <c r="AE2" s="200" t="s">
         <v>657</v>
       </c>
-      <c r="AF2" s="194"/>
-      <c r="AG2" s="194"/>
-      <c r="AH2" s="195"/>
-      <c r="AI2" s="193" t="s">
+      <c r="AF2" s="201"/>
+      <c r="AG2" s="201"/>
+      <c r="AH2" s="202"/>
+      <c r="AI2" s="200" t="s">
         <v>658</v>
       </c>
-      <c r="AJ2" s="194"/>
-      <c r="AK2" s="194"/>
-      <c r="AL2" s="195"/>
-      <c r="AM2" s="193" t="s">
+      <c r="AJ2" s="201"/>
+      <c r="AK2" s="201"/>
+      <c r="AL2" s="202"/>
+      <c r="AM2" s="200" t="s">
         <v>659</v>
       </c>
-      <c r="AN2" s="194"/>
-      <c r="AO2" s="194"/>
-      <c r="AP2" s="195"/>
-      <c r="AQ2" s="193" t="s">
+      <c r="AN2" s="201"/>
+      <c r="AO2" s="201"/>
+      <c r="AP2" s="202"/>
+      <c r="AQ2" s="200" t="s">
         <v>660</v>
       </c>
-      <c r="AR2" s="194"/>
-      <c r="AS2" s="194"/>
-      <c r="AT2" s="195"/>
-      <c r="AU2" s="193" t="s">
+      <c r="AR2" s="201"/>
+      <c r="AS2" s="201"/>
+      <c r="AT2" s="202"/>
+      <c r="AU2" s="200" t="s">
         <v>722</v>
       </c>
-      <c r="AV2" s="194"/>
-      <c r="AW2" s="194"/>
-      <c r="AX2" s="195"/>
-      <c r="AY2" s="193" t="s">
+      <c r="AV2" s="201"/>
+      <c r="AW2" s="201"/>
+      <c r="AX2" s="202"/>
+      <c r="AY2" s="200" t="s">
         <v>729</v>
       </c>
-      <c r="AZ2" s="194"/>
-      <c r="BA2" s="194"/>
-      <c r="BB2" s="195"/>
+      <c r="AZ2" s="201"/>
+      <c r="BA2" s="201"/>
+      <c r="BB2" s="202"/>
     </row>
     <row r="3" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
-      <c r="C3" s="201"/>
-      <c r="D3" s="201"/>
-      <c r="E3" s="201"/>
-      <c r="F3" s="203"/>
+      <c r="C3" s="197"/>
+      <c r="D3" s="197"/>
+      <c r="E3" s="197"/>
+      <c r="F3" s="199"/>
       <c r="G3" s="80">
         <v>1</v>
       </c>
@@ -38936,6 +38944,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="O2:R2"/>
     <mergeCell ref="AU2:AX2"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="AY2:BB2"/>
@@ -38947,11 +38960,6 @@
     <mergeCell ref="AM2:AP2"/>
     <mergeCell ref="AQ2:AT2"/>
     <mergeCell ref="S2:V2"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="O2:R2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E84" location="ลูกค้า!A1" display="ลูกค้า!A1"/>
@@ -39142,7 +39150,7 @@
       <c r="A1" s="210" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="200" t="s">
+      <c r="B1" s="196" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="212" t="s">
@@ -39170,7 +39178,7 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="211"/>
-      <c r="B2" s="201"/>
+      <c r="B2" s="197"/>
       <c r="C2" s="1">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
update stock unit & unitmain
</commit_message>
<xml_diff>
--- a/_Doc/Feature.xlsx
+++ b/_Doc/Feature.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="735" windowWidth="19080" windowHeight="6765" tabRatio="884" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="795" windowWidth="19080" windowHeight="6705" tabRatio="884" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="46" r:id="rId1"/>
@@ -226,7 +226,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2417" uniqueCount="1695">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2425" uniqueCount="1701">
   <si>
     <t>No.</t>
   </si>
@@ -5635,15 +5635,9 @@
     <t>update ProductList set RateUnit=1;</t>
   </si>
   <si>
-    <t>สินค้าเพิ่มหน่อยขายหลัก</t>
-  </si>
-  <si>
     <t>หน่วยย่อยใช้กำหนดตัวมาหารแทน เช่น 1/12 โหล</t>
   </si>
   <si>
-    <t>update stock ให้ทำ SN ได้</t>
-  </si>
-  <si>
     <t>PO เพิ่มหน่วย</t>
   </si>
   <si>
@@ -5654,6 +5648,30 @@
   </si>
   <si>
     <t>หน้าข้อมูลจังหวัด</t>
+  </si>
+  <si>
+    <t>1.0.0.90</t>
+  </si>
+  <si>
+    <t>สินค้าเพิ่มหน่วยหลักซื้อ</t>
+  </si>
+  <si>
+    <t>alter table Produc add UnitMainIDBuy  bigint;</t>
+  </si>
+  <si>
+    <t>Update Set UnitMainIDBuy=UnitMainID;</t>
+  </si>
+  <si>
+    <t>จังหวัด</t>
+  </si>
+  <si>
+    <t>ProvinceBar</t>
+  </si>
+  <si>
+    <t>Province</t>
+  </si>
+  <si>
+    <t>INSERT INTO  [Menu]([MenuID],[ShowMode],[System],[Module],[MenuName],[MenuDisplay],[TableName],[IsVisible],[IsEnable],[IsAdd],[IsEdit],[IsDelete],[IsPrint],[IsImport],[IsCreateQuick],[IsCopy],[IsAssign],[IsConvert]) VALUES (98,31,'ข้อมูลเริ่มต้น','ทั่วไป' ,'ProvinceBar','จังหวัด' ,'Province',1 ,1 ,1,1,1,0,0,0,0,0,0);</t>
   </si>
 </sst>
 </file>
@@ -6280,7 +6298,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="215">
+  <cellXfs count="216">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -6624,6 +6642,7 @@
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -7526,20 +7545,20 @@
       <c r="B1" s="2"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="196" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="196" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="196" t="s">
+      <c r="A2" s="197" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="197" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="197" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="197"/>
-      <c r="B3" s="197"/>
-      <c r="C3" s="197"/>
+      <c r="A3" s="198"/>
+      <c r="B3" s="198"/>
+      <c r="C3" s="198"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
@@ -8634,100 +8653,100 @@
       </c>
     </row>
     <row r="31" spans="2:3" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="B31" s="213" t="s">
+      <c r="B31" s="214" t="s">
         <v>162</v>
       </c>
-      <c r="C31" s="213"/>
+      <c r="C31" s="214"/>
     </row>
     <row r="32" spans="2:3" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="B32" s="213" t="s">
+      <c r="B32" s="214" t="s">
         <v>163</v>
       </c>
-      <c r="C32" s="213"/>
+      <c r="C32" s="214"/>
     </row>
     <row r="33" spans="2:3" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="B33" s="213" t="s">
+      <c r="B33" s="214" t="s">
         <v>164</v>
       </c>
-      <c r="C33" s="213"/>
+      <c r="C33" s="214"/>
     </row>
     <row r="34" spans="2:3" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="B34" s="213" t="s">
+      <c r="B34" s="214" t="s">
         <v>165</v>
       </c>
-      <c r="C34" s="213"/>
+      <c r="C34" s="214"/>
     </row>
     <row r="35" spans="2:3" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="B35" s="213" t="s">
+      <c r="B35" s="214" t="s">
         <v>166</v>
       </c>
-      <c r="C35" s="213"/>
+      <c r="C35" s="214"/>
     </row>
     <row r="36" spans="2:3" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="B36" s="213" t="s">
+      <c r="B36" s="214" t="s">
         <v>167</v>
       </c>
-      <c r="C36" s="213"/>
+      <c r="C36" s="214"/>
     </row>
     <row r="37" spans="2:3" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="B37" s="213" t="s">
+      <c r="B37" s="214" t="s">
         <v>168</v>
       </c>
-      <c r="C37" s="213"/>
+      <c r="C37" s="214"/>
     </row>
     <row r="38" spans="2:3" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="B38" s="213" t="s">
+      <c r="B38" s="214" t="s">
         <v>169</v>
       </c>
-      <c r="C38" s="213"/>
+      <c r="C38" s="214"/>
     </row>
     <row r="39" spans="2:3" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="B39" s="213" t="s">
+      <c r="B39" s="214" t="s">
         <v>170</v>
       </c>
-      <c r="C39" s="213"/>
+      <c r="C39" s="214"/>
     </row>
     <row r="40" spans="2:3" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="B40" s="213" t="s">
+      <c r="B40" s="214" t="s">
         <v>171</v>
       </c>
-      <c r="C40" s="213"/>
+      <c r="C40" s="214"/>
     </row>
     <row r="41" spans="2:3" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="B41" s="213" t="s">
+      <c r="B41" s="214" t="s">
         <v>172</v>
       </c>
-      <c r="C41" s="213"/>
+      <c r="C41" s="214"/>
     </row>
     <row r="42" spans="2:3" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="B42" s="213" t="s">
+      <c r="B42" s="214" t="s">
         <v>173</v>
       </c>
-      <c r="C42" s="213"/>
+      <c r="C42" s="214"/>
     </row>
     <row r="43" spans="2:3" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="B43" s="213" t="s">
+      <c r="B43" s="214" t="s">
         <v>174</v>
       </c>
-      <c r="C43" s="213"/>
+      <c r="C43" s="214"/>
     </row>
     <row r="44" spans="2:3" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="B44" s="213" t="s">
+      <c r="B44" s="214" t="s">
         <v>175</v>
       </c>
-      <c r="C44" s="213"/>
+      <c r="C44" s="214"/>
     </row>
     <row r="45" spans="2:3" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="B45" s="213" t="s">
+      <c r="B45" s="214" t="s">
         <v>176</v>
       </c>
-      <c r="C45" s="213"/>
+      <c r="C45" s="214"/>
     </row>
     <row r="46" spans="2:3" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="B46" s="213" t="s">
+      <c r="B46" s="214" t="s">
         <v>177</v>
       </c>
-      <c r="C46" s="213"/>
+      <c r="C46" s="214"/>
     </row>
     <row r="47" spans="2:3" ht="18.75" x14ac:dyDescent="0.45">
       <c r="B47" s="20" t="s">
@@ -10671,8 +10690,8 @@
   </sheetPr>
   <dimension ref="A1:C372"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A342" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B356" sqref="B356"/>
+    <sheetView tabSelected="1" topLeftCell="A363" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G376" sqref="G376"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21.75" x14ac:dyDescent="0.5"/>
@@ -10705,7 +10724,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="B4" s="191" t="s">
+      <c r="B4" s="192" t="s">
         <v>993</v>
       </c>
       <c r="C4" s="153" t="s">
@@ -10713,13 +10732,13 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="B5" s="191"/>
+      <c r="B5" s="192"/>
       <c r="C5" s="151" t="s">
         <v>991</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="B6" s="191"/>
+      <c r="B6" s="192"/>
       <c r="C6" s="151" t="s">
         <v>992</v>
       </c>
@@ -10910,7 +10929,7 @@
       <c r="B37" s="151" t="s">
         <v>1027</v>
       </c>
-      <c r="C37" s="192" t="s">
+      <c r="C37" s="193" t="s">
         <v>1061</v>
       </c>
     </row>
@@ -10918,61 +10937,61 @@
       <c r="B38" s="151" t="s">
         <v>1028</v>
       </c>
-      <c r="C38" s="192"/>
+      <c r="C38" s="193"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B39" s="151" t="s">
         <v>1053</v>
       </c>
-      <c r="C39" s="192"/>
+      <c r="C39" s="193"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B40" s="151" t="s">
         <v>1057</v>
       </c>
-      <c r="C40" s="192"/>
+      <c r="C40" s="193"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B41" s="151" t="s">
         <v>1058</v>
       </c>
-      <c r="C41" s="192"/>
+      <c r="C41" s="193"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B42" s="151" t="s">
         <v>1059</v>
       </c>
-      <c r="C42" s="192"/>
+      <c r="C42" s="193"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B43" s="151" t="s">
         <v>1063</v>
       </c>
-      <c r="C43" s="192"/>
+      <c r="C43" s="193"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B44" s="151" t="s">
         <v>1062</v>
       </c>
-      <c r="C44" s="192"/>
+      <c r="C44" s="193"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="C45" s="192"/>
+      <c r="C45" s="193"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="C46" s="192"/>
+      <c r="C46" s="193"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="C47" s="192"/>
+      <c r="C47" s="193"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="C48" s="192"/>
+      <c r="C48" s="193"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="C49" s="192"/>
+      <c r="C49" s="193"/>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="C50" s="192"/>
+      <c r="C50" s="193"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A51" s="151" t="s">
@@ -12612,7 +12631,7 @@
     </row>
     <row r="344" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A344" s="151" t="s">
-        <v>1678</v>
+        <v>1693</v>
       </c>
       <c r="B344" s="151" t="s">
         <v>1679</v>
@@ -12622,53 +12641,51 @@
       </c>
     </row>
     <row r="345" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="B345" s="151" t="s">
+        <v>1694</v>
+      </c>
       <c r="C345" s="152" t="s">
         <v>1685</v>
       </c>
     </row>
     <row r="346" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="B346" s="151" t="s">
+        <v>1688</v>
+      </c>
       <c r="C346" s="152" t="s">
         <v>1686</v>
       </c>
     </row>
     <row r="347" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="B347" s="151" t="s">
+        <v>1690</v>
+      </c>
       <c r="C347" s="151" t="s">
         <v>1687</v>
       </c>
     </row>
+    <row r="348" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="B348" s="151" t="s">
+        <v>1689</v>
+      </c>
+      <c r="C348" s="151" t="s">
+        <v>1695</v>
+      </c>
+    </row>
     <row r="349" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B349" s="151" t="s">
-        <v>1688</v>
+        <v>1691</v>
+      </c>
+      <c r="C349" s="151" t="s">
+        <v>1696</v>
       </c>
     </row>
     <row r="350" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B350" s="151" t="s">
-        <v>1689</v>
-      </c>
-    </row>
-    <row r="351" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="B351" s="151" t="s">
-        <v>1690</v>
-      </c>
-    </row>
-    <row r="352" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="B352" s="151" t="s">
         <v>1692</v>
       </c>
-    </row>
-    <row r="353" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B353" s="151" t="s">
-        <v>1691</v>
-      </c>
-    </row>
-    <row r="354" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B354" s="151" t="s">
-        <v>1693</v>
-      </c>
-    </row>
-    <row r="355" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B355" s="151" t="s">
-        <v>1694</v>
+      <c r="C350" s="191" t="s">
+        <v>1700</v>
       </c>
     </row>
     <row r="357" spans="2:2" x14ac:dyDescent="0.5">
@@ -13654,7 +13671,7 @@
       </c>
     </row>
     <row r="39" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="214" t="s">
+      <c r="A39" s="215" t="s">
         <v>927</v>
       </c>
       <c r="B39" s="19" t="s">
@@ -13662,19 +13679,19 @@
       </c>
     </row>
     <row r="40" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="214"/>
+      <c r="A40" s="215"/>
       <c r="B40" s="19" t="s">
         <v>613</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A41" s="214"/>
+      <c r="A41" s="215"/>
       <c r="B41" s="19" t="s">
         <v>614</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="A42" s="214" t="s">
+      <c r="A42" s="215" t="s">
         <v>927</v>
       </c>
       <c r="B42" s="19" t="s">
@@ -13682,13 +13699,13 @@
       </c>
     </row>
     <row r="43" spans="1:2" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="A43" s="214"/>
+      <c r="A43" s="215"/>
       <c r="B43" s="19" t="s">
         <v>616</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="A44" s="214"/>
+      <c r="A44" s="215"/>
       <c r="B44" s="19" t="s">
         <v>617</v>
       </c>
@@ -13734,12 +13751,12 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:R98"/>
+  <dimension ref="A1:S99"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B17" sqref="B17"/>
-      <selection pane="bottomLeft" activeCell="G98" sqref="G98"/>
+      <selection pane="bottomLeft" activeCell="E99" sqref="E99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19230,12 +19247,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:18" s="120" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:19" s="120" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="120">
         <v>96</v>
       </c>
       <c r="B97" s="120">
-        <f t="shared" ref="B97:B98" si="30">IF( H97=TRUE,1,0)+IF(I97=TRUE,2,0)+IF( J97=TRUE,4,0)+IF( K97=TRUE,8,0)+IF( L97=TRUE,16,0)+IF( M97=TRUE,32,0)+IF( N97=TRUE,64,0)+IF( O97=TRUE,128,0)+IF(P97=TRUE,256,0)+IF(Q97=TRUE,512,0)+IF(R97=TRUE,1024,0)</f>
+        <f t="shared" ref="B97:B99" si="30">IF( H97=TRUE,1,0)+IF(I97=TRUE,2,0)+IF( J97=TRUE,4,0)+IF( K97=TRUE,8,0)+IF( L97=TRUE,16,0)+IF( M97=TRUE,32,0)+IF( N97=TRUE,64,0)+IF( O97=TRUE,128,0)+IF(P97=TRUE,256,0)+IF(Q97=TRUE,512,0)+IF(R97=TRUE,1024,0)</f>
         <v>3</v>
       </c>
       <c r="C97" s="120" t="s">
@@ -19287,7 +19304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:18" s="120" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:19" s="120" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="120">
         <v>97</v>
       </c>
@@ -19342,6 +19359,66 @@
       </c>
       <c r="R98" s="121" t="b">
         <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:19" s="120" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="120">
+        <v>98</v>
+      </c>
+      <c r="B99" s="120">
+        <f t="shared" si="30"/>
+        <v>31</v>
+      </c>
+      <c r="C99" s="120" t="s">
+        <v>778</v>
+      </c>
+      <c r="D99" s="120" t="s">
+        <v>837</v>
+      </c>
+      <c r="E99" s="120" t="s">
+        <v>1698</v>
+      </c>
+      <c r="F99" s="120" t="s">
+        <v>1697</v>
+      </c>
+      <c r="G99" s="120" t="s">
+        <v>1699</v>
+      </c>
+      <c r="H99" s="121" t="b">
+        <v>1</v>
+      </c>
+      <c r="I99" s="121" t="b">
+        <v>1</v>
+      </c>
+      <c r="J99" s="121" t="b">
+        <v>1</v>
+      </c>
+      <c r="K99" s="121" t="b">
+        <v>1</v>
+      </c>
+      <c r="L99" s="121" t="b">
+        <v>1</v>
+      </c>
+      <c r="M99" s="121" t="b">
+        <v>0</v>
+      </c>
+      <c r="N99" s="121" t="b">
+        <v>0</v>
+      </c>
+      <c r="O99" s="121" t="b">
+        <v>0</v>
+      </c>
+      <c r="P99" s="121" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q99" s="121" t="b">
+        <v>0</v>
+      </c>
+      <c r="R99" s="121" t="b">
+        <v>0</v>
+      </c>
+      <c r="S99" s="191" t="s">
+        <v>1700</v>
       </c>
     </row>
   </sheetData>
@@ -21297,97 +21374,97 @@
     </row>
     <row r="2" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
-      <c r="B2" s="196" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="196" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="196" t="s">
+      <c r="B2" s="197" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="197" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="197" t="s">
         <v>130</v>
       </c>
-      <c r="E2" s="198" t="s">
+      <c r="E2" s="199" t="s">
         <v>723</v>
       </c>
-      <c r="F2" s="193" t="s">
+      <c r="F2" s="194" t="s">
         <v>651</v>
       </c>
-      <c r="G2" s="194"/>
-      <c r="H2" s="194"/>
-      <c r="I2" s="195"/>
-      <c r="J2" s="193" t="s">
+      <c r="G2" s="195"/>
+      <c r="H2" s="195"/>
+      <c r="I2" s="196"/>
+      <c r="J2" s="194" t="s">
         <v>652</v>
       </c>
-      <c r="K2" s="194"/>
-      <c r="L2" s="194"/>
-      <c r="M2" s="195"/>
-      <c r="N2" s="193" t="s">
+      <c r="K2" s="195"/>
+      <c r="L2" s="195"/>
+      <c r="M2" s="196"/>
+      <c r="N2" s="194" t="s">
         <v>653</v>
       </c>
-      <c r="O2" s="194"/>
-      <c r="P2" s="194"/>
-      <c r="Q2" s="195"/>
-      <c r="R2" s="193" t="s">
+      <c r="O2" s="195"/>
+      <c r="P2" s="195"/>
+      <c r="Q2" s="196"/>
+      <c r="R2" s="194" t="s">
         <v>654</v>
       </c>
-      <c r="S2" s="194"/>
-      <c r="T2" s="194"/>
-      <c r="U2" s="203"/>
-      <c r="V2" s="193" t="s">
+      <c r="S2" s="195"/>
+      <c r="T2" s="195"/>
+      <c r="U2" s="204"/>
+      <c r="V2" s="194" t="s">
         <v>655</v>
       </c>
-      <c r="W2" s="194"/>
-      <c r="X2" s="194"/>
-      <c r="Y2" s="203"/>
-      <c r="Z2" s="200" t="s">
+      <c r="W2" s="195"/>
+      <c r="X2" s="195"/>
+      <c r="Y2" s="204"/>
+      <c r="Z2" s="201" t="s">
         <v>656</v>
       </c>
-      <c r="AA2" s="201"/>
-      <c r="AB2" s="201"/>
-      <c r="AC2" s="202"/>
-      <c r="AD2" s="200" t="s">
+      <c r="AA2" s="202"/>
+      <c r="AB2" s="202"/>
+      <c r="AC2" s="203"/>
+      <c r="AD2" s="201" t="s">
         <v>657</v>
       </c>
-      <c r="AE2" s="201"/>
-      <c r="AF2" s="201"/>
-      <c r="AG2" s="202"/>
-      <c r="AH2" s="200" t="s">
+      <c r="AE2" s="202"/>
+      <c r="AF2" s="202"/>
+      <c r="AG2" s="203"/>
+      <c r="AH2" s="201" t="s">
         <v>658</v>
       </c>
-      <c r="AI2" s="201"/>
-      <c r="AJ2" s="201"/>
-      <c r="AK2" s="202"/>
-      <c r="AL2" s="200" t="s">
+      <c r="AI2" s="202"/>
+      <c r="AJ2" s="202"/>
+      <c r="AK2" s="203"/>
+      <c r="AL2" s="201" t="s">
         <v>659</v>
       </c>
-      <c r="AM2" s="201"/>
-      <c r="AN2" s="201"/>
-      <c r="AO2" s="202"/>
-      <c r="AP2" s="200" t="s">
+      <c r="AM2" s="202"/>
+      <c r="AN2" s="202"/>
+      <c r="AO2" s="203"/>
+      <c r="AP2" s="201" t="s">
         <v>660</v>
       </c>
-      <c r="AQ2" s="201"/>
-      <c r="AR2" s="201"/>
-      <c r="AS2" s="202"/>
-      <c r="AT2" s="200" t="s">
+      <c r="AQ2" s="202"/>
+      <c r="AR2" s="202"/>
+      <c r="AS2" s="203"/>
+      <c r="AT2" s="201" t="s">
         <v>722</v>
       </c>
-      <c r="AU2" s="201"/>
-      <c r="AV2" s="201"/>
-      <c r="AW2" s="202"/>
-      <c r="AX2" s="200" t="s">
+      <c r="AU2" s="202"/>
+      <c r="AV2" s="202"/>
+      <c r="AW2" s="203"/>
+      <c r="AX2" s="201" t="s">
         <v>729</v>
       </c>
-      <c r="AY2" s="201"/>
-      <c r="AZ2" s="201"/>
-      <c r="BA2" s="202"/>
+      <c r="AY2" s="202"/>
+      <c r="AZ2" s="202"/>
+      <c r="BA2" s="203"/>
     </row>
     <row r="3" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
-      <c r="B3" s="197"/>
-      <c r="C3" s="197"/>
-      <c r="D3" s="197"/>
-      <c r="E3" s="199"/>
+      <c r="B3" s="198"/>
+      <c r="C3" s="198"/>
+      <c r="D3" s="198"/>
+      <c r="E3" s="200"/>
       <c r="F3" s="80">
         <v>1</v>
       </c>
@@ -27074,86 +27151,86 @@
     <row r="2" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
-      <c r="C2" s="196" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="196" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="196" t="s">
+      <c r="C2" s="197" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="197" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="197" t="s">
         <v>130</v>
       </c>
-      <c r="F2" s="198" t="s">
+      <c r="F2" s="199" t="s">
         <v>723</v>
       </c>
-      <c r="G2" s="204" t="s">
+      <c r="G2" s="205" t="s">
         <v>660</v>
       </c>
-      <c r="H2" s="205"/>
-      <c r="I2" s="205"/>
-      <c r="J2" s="207"/>
-      <c r="K2" s="204" t="s">
+      <c r="H2" s="206"/>
+      <c r="I2" s="206"/>
+      <c r="J2" s="208"/>
+      <c r="K2" s="205" t="s">
         <v>722</v>
       </c>
-      <c r="L2" s="205"/>
-      <c r="M2" s="205"/>
-      <c r="N2" s="206"/>
-      <c r="O2" s="204" t="s">
+      <c r="L2" s="206"/>
+      <c r="M2" s="206"/>
+      <c r="N2" s="207"/>
+      <c r="O2" s="205" t="s">
         <v>729</v>
       </c>
-      <c r="P2" s="205"/>
-      <c r="Q2" s="205"/>
-      <c r="R2" s="206"/>
-      <c r="S2" s="204" t="s">
+      <c r="P2" s="206"/>
+      <c r="Q2" s="206"/>
+      <c r="R2" s="207"/>
+      <c r="S2" s="205" t="s">
         <v>651</v>
       </c>
-      <c r="T2" s="205"/>
-      <c r="U2" s="205"/>
-      <c r="V2" s="206"/>
-      <c r="W2" s="204" t="s">
+      <c r="T2" s="206"/>
+      <c r="U2" s="206"/>
+      <c r="V2" s="207"/>
+      <c r="W2" s="205" t="s">
         <v>730</v>
       </c>
-      <c r="X2" s="205"/>
-      <c r="Y2" s="205"/>
-      <c r="Z2" s="206"/>
-      <c r="AA2" s="204" t="s">
+      <c r="X2" s="206"/>
+      <c r="Y2" s="206"/>
+      <c r="Z2" s="207"/>
+      <c r="AA2" s="205" t="s">
         <v>653</v>
       </c>
-      <c r="AB2" s="205"/>
-      <c r="AC2" s="205"/>
-      <c r="AD2" s="206"/>
-      <c r="AE2" s="204" t="s">
+      <c r="AB2" s="206"/>
+      <c r="AC2" s="206"/>
+      <c r="AD2" s="207"/>
+      <c r="AE2" s="205" t="s">
         <v>731</v>
       </c>
-      <c r="AF2" s="205"/>
-      <c r="AG2" s="205"/>
-      <c r="AH2" s="206"/>
-      <c r="AI2" s="204" t="s">
+      <c r="AF2" s="206"/>
+      <c r="AG2" s="206"/>
+      <c r="AH2" s="207"/>
+      <c r="AI2" s="205" t="s">
         <v>655</v>
       </c>
-      <c r="AJ2" s="205"/>
-      <c r="AK2" s="205"/>
-      <c r="AL2" s="206"/>
-      <c r="AM2" s="204" t="s">
+      <c r="AJ2" s="206"/>
+      <c r="AK2" s="206"/>
+      <c r="AL2" s="207"/>
+      <c r="AM2" s="205" t="s">
         <v>656</v>
       </c>
-      <c r="AN2" s="205"/>
-      <c r="AO2" s="205"/>
-      <c r="AP2" s="206"/>
-      <c r="AQ2" s="204" t="s">
+      <c r="AN2" s="206"/>
+      <c r="AO2" s="206"/>
+      <c r="AP2" s="207"/>
+      <c r="AQ2" s="205" t="s">
         <v>657</v>
       </c>
-      <c r="AR2" s="205"/>
-      <c r="AS2" s="205"/>
-      <c r="AT2" s="206"/>
+      <c r="AR2" s="206"/>
+      <c r="AS2" s="206"/>
+      <c r="AT2" s="207"/>
     </row>
     <row r="3" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
-      <c r="C3" s="197"/>
-      <c r="D3" s="197"/>
-      <c r="E3" s="197"/>
-      <c r="F3" s="199"/>
+      <c r="C3" s="198"/>
+      <c r="D3" s="198"/>
+      <c r="E3" s="198"/>
+      <c r="F3" s="200"/>
       <c r="G3" s="80">
         <v>1</v>
       </c>
@@ -33440,98 +33517,98 @@
     <row r="2" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
-      <c r="C2" s="196" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="196" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="196" t="s">
+      <c r="C2" s="197" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="197" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="197" t="s">
         <v>130</v>
       </c>
-      <c r="F2" s="198" t="s">
+      <c r="F2" s="199" t="s">
         <v>723</v>
       </c>
-      <c r="G2" s="193" t="s">
+      <c r="G2" s="194" t="s">
         <v>651</v>
       </c>
-      <c r="H2" s="194"/>
-      <c r="I2" s="194"/>
-      <c r="J2" s="195"/>
-      <c r="K2" s="193" t="s">
+      <c r="H2" s="195"/>
+      <c r="I2" s="195"/>
+      <c r="J2" s="196"/>
+      <c r="K2" s="194" t="s">
         <v>652</v>
       </c>
-      <c r="L2" s="194"/>
-      <c r="M2" s="194"/>
-      <c r="N2" s="195"/>
-      <c r="O2" s="193" t="s">
+      <c r="L2" s="195"/>
+      <c r="M2" s="195"/>
+      <c r="N2" s="196"/>
+      <c r="O2" s="194" t="s">
         <v>653</v>
       </c>
-      <c r="P2" s="194"/>
-      <c r="Q2" s="194"/>
-      <c r="R2" s="195"/>
-      <c r="S2" s="193" t="s">
+      <c r="P2" s="195"/>
+      <c r="Q2" s="195"/>
+      <c r="R2" s="196"/>
+      <c r="S2" s="194" t="s">
         <v>654</v>
       </c>
-      <c r="T2" s="194"/>
-      <c r="U2" s="194"/>
-      <c r="V2" s="203"/>
-      <c r="W2" s="193" t="s">
+      <c r="T2" s="195"/>
+      <c r="U2" s="195"/>
+      <c r="V2" s="204"/>
+      <c r="W2" s="194" t="s">
         <v>655</v>
       </c>
-      <c r="X2" s="194"/>
-      <c r="Y2" s="194"/>
-      <c r="Z2" s="203"/>
-      <c r="AA2" s="200" t="s">
+      <c r="X2" s="195"/>
+      <c r="Y2" s="195"/>
+      <c r="Z2" s="204"/>
+      <c r="AA2" s="201" t="s">
         <v>656</v>
       </c>
-      <c r="AB2" s="201"/>
-      <c r="AC2" s="201"/>
-      <c r="AD2" s="202"/>
-      <c r="AE2" s="200" t="s">
+      <c r="AB2" s="202"/>
+      <c r="AC2" s="202"/>
+      <c r="AD2" s="203"/>
+      <c r="AE2" s="201" t="s">
         <v>657</v>
       </c>
-      <c r="AF2" s="201"/>
-      <c r="AG2" s="201"/>
-      <c r="AH2" s="202"/>
-      <c r="AI2" s="200" t="s">
+      <c r="AF2" s="202"/>
+      <c r="AG2" s="202"/>
+      <c r="AH2" s="203"/>
+      <c r="AI2" s="201" t="s">
         <v>658</v>
       </c>
-      <c r="AJ2" s="201"/>
-      <c r="AK2" s="201"/>
-      <c r="AL2" s="202"/>
-      <c r="AM2" s="200" t="s">
+      <c r="AJ2" s="202"/>
+      <c r="AK2" s="202"/>
+      <c r="AL2" s="203"/>
+      <c r="AM2" s="201" t="s">
         <v>659</v>
       </c>
-      <c r="AN2" s="201"/>
-      <c r="AO2" s="201"/>
-      <c r="AP2" s="202"/>
-      <c r="AQ2" s="200" t="s">
+      <c r="AN2" s="202"/>
+      <c r="AO2" s="202"/>
+      <c r="AP2" s="203"/>
+      <c r="AQ2" s="201" t="s">
         <v>660</v>
       </c>
-      <c r="AR2" s="201"/>
-      <c r="AS2" s="201"/>
-      <c r="AT2" s="202"/>
-      <c r="AU2" s="200" t="s">
+      <c r="AR2" s="202"/>
+      <c r="AS2" s="202"/>
+      <c r="AT2" s="203"/>
+      <c r="AU2" s="201" t="s">
         <v>722</v>
       </c>
-      <c r="AV2" s="201"/>
-      <c r="AW2" s="201"/>
-      <c r="AX2" s="202"/>
-      <c r="AY2" s="200" t="s">
+      <c r="AV2" s="202"/>
+      <c r="AW2" s="202"/>
+      <c r="AX2" s="203"/>
+      <c r="AY2" s="201" t="s">
         <v>729</v>
       </c>
-      <c r="AZ2" s="201"/>
-      <c r="BA2" s="201"/>
-      <c r="BB2" s="202"/>
+      <c r="AZ2" s="202"/>
+      <c r="BA2" s="202"/>
+      <c r="BB2" s="203"/>
     </row>
     <row r="3" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
-      <c r="C3" s="197"/>
-      <c r="D3" s="197"/>
-      <c r="E3" s="197"/>
-      <c r="F3" s="199"/>
+      <c r="C3" s="198"/>
+      <c r="D3" s="198"/>
+      <c r="E3" s="198"/>
+      <c r="F3" s="200"/>
       <c r="G3" s="80">
         <v>1</v>
       </c>
@@ -39147,38 +39224,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="210" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="196" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="212" t="s">
+      <c r="A1" s="211" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="197" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="213" t="s">
         <v>651</v>
       </c>
-      <c r="D1" s="212"/>
-      <c r="E1" s="212"/>
-      <c r="F1" s="209"/>
-      <c r="G1" s="212" t="s">
+      <c r="D1" s="213"/>
+      <c r="E1" s="213"/>
+      <c r="F1" s="210"/>
+      <c r="G1" s="213" t="s">
         <v>730</v>
       </c>
-      <c r="H1" s="212"/>
-      <c r="I1" s="212"/>
-      <c r="J1" s="209"/>
-      <c r="K1" s="212" t="s">
+      <c r="H1" s="213"/>
+      <c r="I1" s="213"/>
+      <c r="J1" s="210"/>
+      <c r="K1" s="213" t="s">
         <v>653</v>
       </c>
-      <c r="L1" s="212"/>
-      <c r="M1" s="212"/>
-      <c r="N1" s="209"/>
-      <c r="O1" s="208" t="s">
+      <c r="L1" s="213"/>
+      <c r="M1" s="213"/>
+      <c r="N1" s="210"/>
+      <c r="O1" s="209" t="s">
         <v>731</v>
       </c>
-      <c r="P1" s="209"/>
+      <c r="P1" s="210"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="211"/>
-      <c r="B2" s="197"/>
+      <c r="A2" s="212"/>
+      <c r="B2" s="198"/>
       <c r="C2" s="1">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
update stock to new form
</commit_message>
<xml_diff>
--- a/_Doc/Feature.xlsx
+++ b/_Doc/Feature.xlsx
@@ -5656,12 +5656,6 @@
     <t>สินค้าเพิ่มหน่วยหลักซื้อ</t>
   </si>
   <si>
-    <t>alter table Produc add UnitMainIDBuy  bigint;</t>
-  </si>
-  <si>
-    <t>Update Set UnitMainIDBuy=UnitMainID;</t>
-  </si>
-  <si>
     <t>จังหวัด</t>
   </si>
   <si>
@@ -5672,6 +5666,12 @@
   </si>
   <si>
     <t>INSERT INTO  [Menu]([MenuID],[ShowMode],[System],[Module],[MenuName],[MenuDisplay],[TableName],[IsVisible],[IsEnable],[IsAdd],[IsEdit],[IsDelete],[IsPrint],[IsImport],[IsCreateQuick],[IsCopy],[IsAssign],[IsConvert]) VALUES (98,31,'ข้อมูลเริ่มต้น','ทั่วไป' ,'ProvinceBar','จังหวัด' ,'Province',1 ,1 ,1,1,1,0,0,0,0,0,0);</t>
+  </si>
+  <si>
+    <t>alter table Product add UnitMainIDBuy  bigint;</t>
+  </si>
+  <si>
+    <t>Update Product Set UnitMainIDBuy=UnitMainID;</t>
   </si>
 </sst>
 </file>
@@ -6649,6 +6649,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -6656,6 +6665,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -6669,18 +6681,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -7545,20 +7545,20 @@
       <c r="B1" s="2"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="197" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="197" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="197" t="s">
+      <c r="A2" s="201" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="201" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="201" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="198"/>
-      <c r="B3" s="198"/>
-      <c r="C3" s="198"/>
+      <c r="A3" s="202"/>
+      <c r="B3" s="202"/>
+      <c r="C3" s="202"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
@@ -8760,12 +8760,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
     <mergeCell ref="B43:C43"/>
     <mergeCell ref="B44:C44"/>
     <mergeCell ref="B45:C45"/>
@@ -8776,6 +8770,12 @@
     <mergeCell ref="B40:C40"/>
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -10690,8 +10690,8 @@
   </sheetPr>
   <dimension ref="A1:C372"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A363" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G376" sqref="G376"/>
+    <sheetView tabSelected="1" topLeftCell="A339" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C349" sqref="C349"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21.75" x14ac:dyDescent="0.5"/>
@@ -12669,7 +12669,7 @@
         <v>1689</v>
       </c>
       <c r="C348" s="151" t="s">
-        <v>1695</v>
+        <v>1699</v>
       </c>
     </row>
     <row r="349" spans="1:3" x14ac:dyDescent="0.5">
@@ -12677,7 +12677,7 @@
         <v>1691</v>
       </c>
       <c r="C349" s="151" t="s">
-        <v>1696</v>
+        <v>1700</v>
       </c>
     </row>
     <row r="350" spans="1:3" x14ac:dyDescent="0.5">
@@ -12685,7 +12685,7 @@
         <v>1692</v>
       </c>
       <c r="C350" s="191" t="s">
-        <v>1700</v>
+        <v>1698</v>
       </c>
     </row>
     <row r="357" spans="2:2" x14ac:dyDescent="0.5">
@@ -19376,49 +19376,49 @@
         <v>837</v>
       </c>
       <c r="E99" s="120" t="s">
+        <v>1696</v>
+      </c>
+      <c r="F99" s="120" t="s">
+        <v>1695</v>
+      </c>
+      <c r="G99" s="120" t="s">
+        <v>1697</v>
+      </c>
+      <c r="H99" s="121" t="b">
+        <v>1</v>
+      </c>
+      <c r="I99" s="121" t="b">
+        <v>1</v>
+      </c>
+      <c r="J99" s="121" t="b">
+        <v>1</v>
+      </c>
+      <c r="K99" s="121" t="b">
+        <v>1</v>
+      </c>
+      <c r="L99" s="121" t="b">
+        <v>1</v>
+      </c>
+      <c r="M99" s="121" t="b">
+        <v>0</v>
+      </c>
+      <c r="N99" s="121" t="b">
+        <v>0</v>
+      </c>
+      <c r="O99" s="121" t="b">
+        <v>0</v>
+      </c>
+      <c r="P99" s="121" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q99" s="121" t="b">
+        <v>0</v>
+      </c>
+      <c r="R99" s="121" t="b">
+        <v>0</v>
+      </c>
+      <c r="S99" s="191" t="s">
         <v>1698</v>
-      </c>
-      <c r="F99" s="120" t="s">
-        <v>1697</v>
-      </c>
-      <c r="G99" s="120" t="s">
-        <v>1699</v>
-      </c>
-      <c r="H99" s="121" t="b">
-        <v>1</v>
-      </c>
-      <c r="I99" s="121" t="b">
-        <v>1</v>
-      </c>
-      <c r="J99" s="121" t="b">
-        <v>1</v>
-      </c>
-      <c r="K99" s="121" t="b">
-        <v>1</v>
-      </c>
-      <c r="L99" s="121" t="b">
-        <v>1</v>
-      </c>
-      <c r="M99" s="121" t="b">
-        <v>0</v>
-      </c>
-      <c r="N99" s="121" t="b">
-        <v>0</v>
-      </c>
-      <c r="O99" s="121" t="b">
-        <v>0</v>
-      </c>
-      <c r="P99" s="121" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q99" s="121" t="b">
-        <v>0</v>
-      </c>
-      <c r="R99" s="121" t="b">
-        <v>0</v>
-      </c>
-      <c r="S99" s="191" t="s">
-        <v>1700</v>
       </c>
     </row>
   </sheetData>
@@ -21374,97 +21374,97 @@
     </row>
     <row r="2" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
-      <c r="B2" s="197" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="197" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="197" t="s">
+      <c r="B2" s="201" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="201" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="201" t="s">
         <v>130</v>
       </c>
-      <c r="E2" s="199" t="s">
+      <c r="E2" s="203" t="s">
         <v>723</v>
       </c>
-      <c r="F2" s="194" t="s">
+      <c r="F2" s="197" t="s">
         <v>651</v>
       </c>
-      <c r="G2" s="195"/>
-      <c r="H2" s="195"/>
-      <c r="I2" s="196"/>
-      <c r="J2" s="194" t="s">
+      <c r="G2" s="198"/>
+      <c r="H2" s="198"/>
+      <c r="I2" s="199"/>
+      <c r="J2" s="197" t="s">
         <v>652</v>
       </c>
-      <c r="K2" s="195"/>
-      <c r="L2" s="195"/>
-      <c r="M2" s="196"/>
-      <c r="N2" s="194" t="s">
+      <c r="K2" s="198"/>
+      <c r="L2" s="198"/>
+      <c r="M2" s="199"/>
+      <c r="N2" s="197" t="s">
         <v>653</v>
       </c>
-      <c r="O2" s="195"/>
-      <c r="P2" s="195"/>
-      <c r="Q2" s="196"/>
-      <c r="R2" s="194" t="s">
+      <c r="O2" s="198"/>
+      <c r="P2" s="198"/>
+      <c r="Q2" s="199"/>
+      <c r="R2" s="197" t="s">
         <v>654</v>
       </c>
-      <c r="S2" s="195"/>
-      <c r="T2" s="195"/>
-      <c r="U2" s="204"/>
-      <c r="V2" s="194" t="s">
+      <c r="S2" s="198"/>
+      <c r="T2" s="198"/>
+      <c r="U2" s="200"/>
+      <c r="V2" s="197" t="s">
         <v>655</v>
       </c>
-      <c r="W2" s="195"/>
-      <c r="X2" s="195"/>
-      <c r="Y2" s="204"/>
-      <c r="Z2" s="201" t="s">
+      <c r="W2" s="198"/>
+      <c r="X2" s="198"/>
+      <c r="Y2" s="200"/>
+      <c r="Z2" s="194" t="s">
         <v>656</v>
       </c>
-      <c r="AA2" s="202"/>
-      <c r="AB2" s="202"/>
-      <c r="AC2" s="203"/>
-      <c r="AD2" s="201" t="s">
+      <c r="AA2" s="195"/>
+      <c r="AB2" s="195"/>
+      <c r="AC2" s="196"/>
+      <c r="AD2" s="194" t="s">
         <v>657</v>
       </c>
-      <c r="AE2" s="202"/>
-      <c r="AF2" s="202"/>
-      <c r="AG2" s="203"/>
-      <c r="AH2" s="201" t="s">
+      <c r="AE2" s="195"/>
+      <c r="AF2" s="195"/>
+      <c r="AG2" s="196"/>
+      <c r="AH2" s="194" t="s">
         <v>658</v>
       </c>
-      <c r="AI2" s="202"/>
-      <c r="AJ2" s="202"/>
-      <c r="AK2" s="203"/>
-      <c r="AL2" s="201" t="s">
+      <c r="AI2" s="195"/>
+      <c r="AJ2" s="195"/>
+      <c r="AK2" s="196"/>
+      <c r="AL2" s="194" t="s">
         <v>659</v>
       </c>
-      <c r="AM2" s="202"/>
-      <c r="AN2" s="202"/>
-      <c r="AO2" s="203"/>
-      <c r="AP2" s="201" t="s">
+      <c r="AM2" s="195"/>
+      <c r="AN2" s="195"/>
+      <c r="AO2" s="196"/>
+      <c r="AP2" s="194" t="s">
         <v>660</v>
       </c>
-      <c r="AQ2" s="202"/>
-      <c r="AR2" s="202"/>
-      <c r="AS2" s="203"/>
-      <c r="AT2" s="201" t="s">
+      <c r="AQ2" s="195"/>
+      <c r="AR2" s="195"/>
+      <c r="AS2" s="196"/>
+      <c r="AT2" s="194" t="s">
         <v>722</v>
       </c>
-      <c r="AU2" s="202"/>
-      <c r="AV2" s="202"/>
-      <c r="AW2" s="203"/>
-      <c r="AX2" s="201" t="s">
+      <c r="AU2" s="195"/>
+      <c r="AV2" s="195"/>
+      <c r="AW2" s="196"/>
+      <c r="AX2" s="194" t="s">
         <v>729</v>
       </c>
-      <c r="AY2" s="202"/>
-      <c r="AZ2" s="202"/>
-      <c r="BA2" s="203"/>
+      <c r="AY2" s="195"/>
+      <c r="AZ2" s="195"/>
+      <c r="BA2" s="196"/>
     </row>
     <row r="3" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
-      <c r="B3" s="198"/>
-      <c r="C3" s="198"/>
-      <c r="D3" s="198"/>
-      <c r="E3" s="200"/>
+      <c r="B3" s="202"/>
+      <c r="C3" s="202"/>
+      <c r="D3" s="202"/>
+      <c r="E3" s="204"/>
       <c r="F3" s="80">
         <v>1</v>
       </c>
@@ -26618,6 +26618,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:I2"/>
     <mergeCell ref="AL2:AO2"/>
     <mergeCell ref="AP2:AS2"/>
     <mergeCell ref="AT2:AW2"/>
@@ -26628,12 +26634,6 @@
     <mergeCell ref="Z2:AC2"/>
     <mergeCell ref="AD2:AG2"/>
     <mergeCell ref="AH2:AK2"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:I2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D84" location="ลูกค้า!A1" display="ลูกค้า!A1"/>
@@ -27151,16 +27151,16 @@
     <row r="2" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
-      <c r="C2" s="197" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="197" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="197" t="s">
+      <c r="C2" s="201" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="201" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="201" t="s">
         <v>130</v>
       </c>
-      <c r="F2" s="199" t="s">
+      <c r="F2" s="203" t="s">
         <v>723</v>
       </c>
       <c r="G2" s="205" t="s">
@@ -27227,10 +27227,10 @@
     <row r="3" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
-      <c r="C3" s="198"/>
-      <c r="D3" s="198"/>
-      <c r="E3" s="198"/>
-      <c r="F3" s="200"/>
+      <c r="C3" s="202"/>
+      <c r="D3" s="202"/>
+      <c r="E3" s="202"/>
+      <c r="F3" s="204"/>
       <c r="G3" s="80">
         <v>1</v>
       </c>
@@ -33026,6 +33026,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="AE2:AH2"/>
+    <mergeCell ref="AI2:AL2"/>
+    <mergeCell ref="AM2:AP2"/>
+    <mergeCell ref="AQ2:AT2"/>
+    <mergeCell ref="AA2:AD2"/>
     <mergeCell ref="K2:N2"/>
     <mergeCell ref="O2:R2"/>
     <mergeCell ref="S2:V2"/>
@@ -33035,11 +33040,6 @@
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="G2:J2"/>
-    <mergeCell ref="AE2:AH2"/>
-    <mergeCell ref="AI2:AL2"/>
-    <mergeCell ref="AM2:AP2"/>
-    <mergeCell ref="AQ2:AT2"/>
-    <mergeCell ref="AA2:AD2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E84" location="ลูกค้า!A1" display="ลูกค้า!A1"/>
@@ -33517,98 +33517,98 @@
     <row r="2" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
-      <c r="C2" s="197" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="197" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="197" t="s">
+      <c r="C2" s="201" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="201" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="201" t="s">
         <v>130</v>
       </c>
-      <c r="F2" s="199" t="s">
+      <c r="F2" s="203" t="s">
         <v>723</v>
       </c>
-      <c r="G2" s="194" t="s">
+      <c r="G2" s="197" t="s">
         <v>651</v>
       </c>
-      <c r="H2" s="195"/>
-      <c r="I2" s="195"/>
-      <c r="J2" s="196"/>
-      <c r="K2" s="194" t="s">
+      <c r="H2" s="198"/>
+      <c r="I2" s="198"/>
+      <c r="J2" s="199"/>
+      <c r="K2" s="197" t="s">
         <v>652</v>
       </c>
-      <c r="L2" s="195"/>
-      <c r="M2" s="195"/>
-      <c r="N2" s="196"/>
-      <c r="O2" s="194" t="s">
+      <c r="L2" s="198"/>
+      <c r="M2" s="198"/>
+      <c r="N2" s="199"/>
+      <c r="O2" s="197" t="s">
         <v>653</v>
       </c>
-      <c r="P2" s="195"/>
-      <c r="Q2" s="195"/>
-      <c r="R2" s="196"/>
-      <c r="S2" s="194" t="s">
+      <c r="P2" s="198"/>
+      <c r="Q2" s="198"/>
+      <c r="R2" s="199"/>
+      <c r="S2" s="197" t="s">
         <v>654</v>
       </c>
-      <c r="T2" s="195"/>
-      <c r="U2" s="195"/>
-      <c r="V2" s="204"/>
-      <c r="W2" s="194" t="s">
+      <c r="T2" s="198"/>
+      <c r="U2" s="198"/>
+      <c r="V2" s="200"/>
+      <c r="W2" s="197" t="s">
         <v>655</v>
       </c>
-      <c r="X2" s="195"/>
-      <c r="Y2" s="195"/>
-      <c r="Z2" s="204"/>
-      <c r="AA2" s="201" t="s">
+      <c r="X2" s="198"/>
+      <c r="Y2" s="198"/>
+      <c r="Z2" s="200"/>
+      <c r="AA2" s="194" t="s">
         <v>656</v>
       </c>
-      <c r="AB2" s="202"/>
-      <c r="AC2" s="202"/>
-      <c r="AD2" s="203"/>
-      <c r="AE2" s="201" t="s">
+      <c r="AB2" s="195"/>
+      <c r="AC2" s="195"/>
+      <c r="AD2" s="196"/>
+      <c r="AE2" s="194" t="s">
         <v>657</v>
       </c>
-      <c r="AF2" s="202"/>
-      <c r="AG2" s="202"/>
-      <c r="AH2" s="203"/>
-      <c r="AI2" s="201" t="s">
+      <c r="AF2" s="195"/>
+      <c r="AG2" s="195"/>
+      <c r="AH2" s="196"/>
+      <c r="AI2" s="194" t="s">
         <v>658</v>
       </c>
-      <c r="AJ2" s="202"/>
-      <c r="AK2" s="202"/>
-      <c r="AL2" s="203"/>
-      <c r="AM2" s="201" t="s">
+      <c r="AJ2" s="195"/>
+      <c r="AK2" s="195"/>
+      <c r="AL2" s="196"/>
+      <c r="AM2" s="194" t="s">
         <v>659</v>
       </c>
-      <c r="AN2" s="202"/>
-      <c r="AO2" s="202"/>
-      <c r="AP2" s="203"/>
-      <c r="AQ2" s="201" t="s">
+      <c r="AN2" s="195"/>
+      <c r="AO2" s="195"/>
+      <c r="AP2" s="196"/>
+      <c r="AQ2" s="194" t="s">
         <v>660</v>
       </c>
-      <c r="AR2" s="202"/>
-      <c r="AS2" s="202"/>
-      <c r="AT2" s="203"/>
-      <c r="AU2" s="201" t="s">
+      <c r="AR2" s="195"/>
+      <c r="AS2" s="195"/>
+      <c r="AT2" s="196"/>
+      <c r="AU2" s="194" t="s">
         <v>722</v>
       </c>
-      <c r="AV2" s="202"/>
-      <c r="AW2" s="202"/>
-      <c r="AX2" s="203"/>
-      <c r="AY2" s="201" t="s">
+      <c r="AV2" s="195"/>
+      <c r="AW2" s="195"/>
+      <c r="AX2" s="196"/>
+      <c r="AY2" s="194" t="s">
         <v>729</v>
       </c>
-      <c r="AZ2" s="202"/>
-      <c r="BA2" s="202"/>
-      <c r="BB2" s="203"/>
+      <c r="AZ2" s="195"/>
+      <c r="BA2" s="195"/>
+      <c r="BB2" s="196"/>
     </row>
     <row r="3" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
-      <c r="C3" s="198"/>
-      <c r="D3" s="198"/>
-      <c r="E3" s="198"/>
-      <c r="F3" s="200"/>
+      <c r="C3" s="202"/>
+      <c r="D3" s="202"/>
+      <c r="E3" s="202"/>
+      <c r="F3" s="204"/>
       <c r="G3" s="80">
         <v>1</v>
       </c>
@@ -39021,11 +39021,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="O2:R2"/>
     <mergeCell ref="AU2:AX2"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="AY2:BB2"/>
@@ -39037,6 +39032,11 @@
     <mergeCell ref="AM2:AP2"/>
     <mergeCell ref="AQ2:AT2"/>
     <mergeCell ref="S2:V2"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="O2:R2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E84" location="ลูกค้า!A1" display="ลูกค้า!A1"/>
@@ -39227,7 +39227,7 @@
       <c r="A1" s="211" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="197" t="s">
+      <c r="B1" s="201" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="213" t="s">
@@ -39255,7 +39255,7 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="212"/>
-      <c r="B2" s="198"/>
+      <c r="B2" s="202"/>
       <c r="C2" s="1">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
price for unit main
</commit_message>
<xml_diff>
--- a/_Doc/Feature.xlsx
+++ b/_Doc/Feature.xlsx
@@ -226,7 +226,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2426" uniqueCount="1702">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2428" uniqueCount="1704">
   <si>
     <t>No.</t>
   </si>
@@ -5739,6 +5739,12 @@
 EXECUTE (@query)
 END
 </t>
+  </si>
+  <si>
+    <t>alter table ProductList add PriceMain  numeric(18,2);</t>
+  </si>
+  <si>
+    <t>update  ProductList set PriceMain=Price;</t>
   </si>
 </sst>
 </file>
@@ -6716,6 +6722,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -6723,6 +6738,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -6736,18 +6754,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -7612,20 +7618,20 @@
       <c r="B1" s="2"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="197" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="197" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="197" t="s">
+      <c r="A2" s="201" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="201" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="201" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="198"/>
-      <c r="B3" s="198"/>
-      <c r="C3" s="198"/>
+      <c r="A3" s="202"/>
+      <c r="B3" s="202"/>
+      <c r="C3" s="202"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
@@ -8827,12 +8833,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
     <mergeCell ref="B43:C43"/>
     <mergeCell ref="B44:C44"/>
     <mergeCell ref="B45:C45"/>
@@ -8843,6 +8843,12 @@
     <mergeCell ref="B40:C40"/>
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -10757,8 +10763,8 @@
   </sheetPr>
   <dimension ref="A1:C372"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A345" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B360" sqref="B360"/>
+    <sheetView tabSelected="1" topLeftCell="A342" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C353" sqref="C352:C353"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21.75" x14ac:dyDescent="0.5"/>
@@ -12760,57 +12766,67 @@
         <v>1701</v>
       </c>
     </row>
-    <row r="357" spans="2:2" x14ac:dyDescent="0.5">
+    <row r="352" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="C352" s="152" t="s">
+        <v>1702</v>
+      </c>
+    </row>
+    <row r="353" spans="2:3" x14ac:dyDescent="0.5">
+      <c r="C353" s="151" t="s">
+        <v>1703</v>
+      </c>
+    </row>
+    <row r="357" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B357" s="151" t="s">
         <v>1525</v>
       </c>
     </row>
-    <row r="358" spans="2:2" x14ac:dyDescent="0.5">
+    <row r="358" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B358" s="151" t="s">
         <v>1451</v>
       </c>
     </row>
-    <row r="359" spans="2:2" x14ac:dyDescent="0.5">
+    <row r="359" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B359" s="151" t="s">
         <v>1624</v>
       </c>
     </row>
-    <row r="360" spans="2:2" x14ac:dyDescent="0.5">
+    <row r="360" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B360" s="151" t="s">
         <v>1526</v>
       </c>
     </row>
-    <row r="361" spans="2:2" x14ac:dyDescent="0.5">
+    <row r="361" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B361" s="151" t="s">
         <v>1625</v>
       </c>
     </row>
-    <row r="362" spans="2:2" ht="87" x14ac:dyDescent="0.5">
+    <row r="362" spans="2:3" ht="87" x14ac:dyDescent="0.5">
       <c r="B362" s="152" t="s">
         <v>1626</v>
       </c>
     </row>
-    <row r="364" spans="2:2" x14ac:dyDescent="0.5">
+    <row r="364" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B364" s="187" t="s">
         <v>1644</v>
       </c>
     </row>
-    <row r="365" spans="2:2" ht="65.25" x14ac:dyDescent="0.5">
+    <row r="365" spans="2:3" ht="65.25" x14ac:dyDescent="0.5">
       <c r="B365" s="188" t="s">
         <v>1642</v>
       </c>
     </row>
-    <row r="366" spans="2:2" x14ac:dyDescent="0.5">
+    <row r="366" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B366" s="189" t="s">
         <v>1643</v>
       </c>
     </row>
-    <row r="367" spans="2:2" x14ac:dyDescent="0.5">
+    <row r="367" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B367" s="190" t="s">
         <v>1645</v>
       </c>
     </row>
-    <row r="368" spans="2:2" x14ac:dyDescent="0.5">
+    <row r="368" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B368" s="186" t="s">
         <v>1646</v>
       </c>
@@ -21446,97 +21462,97 @@
     </row>
     <row r="2" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
-      <c r="B2" s="197" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="197" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="197" t="s">
+      <c r="B2" s="201" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="201" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="201" t="s">
         <v>130</v>
       </c>
-      <c r="E2" s="199" t="s">
+      <c r="E2" s="203" t="s">
         <v>723</v>
       </c>
-      <c r="F2" s="194" t="s">
+      <c r="F2" s="197" t="s">
         <v>651</v>
       </c>
-      <c r="G2" s="195"/>
-      <c r="H2" s="195"/>
-      <c r="I2" s="196"/>
-      <c r="J2" s="194" t="s">
+      <c r="G2" s="198"/>
+      <c r="H2" s="198"/>
+      <c r="I2" s="199"/>
+      <c r="J2" s="197" t="s">
         <v>652</v>
       </c>
-      <c r="K2" s="195"/>
-      <c r="L2" s="195"/>
-      <c r="M2" s="196"/>
-      <c r="N2" s="194" t="s">
+      <c r="K2" s="198"/>
+      <c r="L2" s="198"/>
+      <c r="M2" s="199"/>
+      <c r="N2" s="197" t="s">
         <v>653</v>
       </c>
-      <c r="O2" s="195"/>
-      <c r="P2" s="195"/>
-      <c r="Q2" s="196"/>
-      <c r="R2" s="194" t="s">
+      <c r="O2" s="198"/>
+      <c r="P2" s="198"/>
+      <c r="Q2" s="199"/>
+      <c r="R2" s="197" t="s">
         <v>654</v>
       </c>
-      <c r="S2" s="195"/>
-      <c r="T2" s="195"/>
-      <c r="U2" s="204"/>
-      <c r="V2" s="194" t="s">
+      <c r="S2" s="198"/>
+      <c r="T2" s="198"/>
+      <c r="U2" s="200"/>
+      <c r="V2" s="197" t="s">
         <v>655</v>
       </c>
-      <c r="W2" s="195"/>
-      <c r="X2" s="195"/>
-      <c r="Y2" s="204"/>
-      <c r="Z2" s="201" t="s">
+      <c r="W2" s="198"/>
+      <c r="X2" s="198"/>
+      <c r="Y2" s="200"/>
+      <c r="Z2" s="194" t="s">
         <v>656</v>
       </c>
-      <c r="AA2" s="202"/>
-      <c r="AB2" s="202"/>
-      <c r="AC2" s="203"/>
-      <c r="AD2" s="201" t="s">
+      <c r="AA2" s="195"/>
+      <c r="AB2" s="195"/>
+      <c r="AC2" s="196"/>
+      <c r="AD2" s="194" t="s">
         <v>657</v>
       </c>
-      <c r="AE2" s="202"/>
-      <c r="AF2" s="202"/>
-      <c r="AG2" s="203"/>
-      <c r="AH2" s="201" t="s">
+      <c r="AE2" s="195"/>
+      <c r="AF2" s="195"/>
+      <c r="AG2" s="196"/>
+      <c r="AH2" s="194" t="s">
         <v>658</v>
       </c>
-      <c r="AI2" s="202"/>
-      <c r="AJ2" s="202"/>
-      <c r="AK2" s="203"/>
-      <c r="AL2" s="201" t="s">
+      <c r="AI2" s="195"/>
+      <c r="AJ2" s="195"/>
+      <c r="AK2" s="196"/>
+      <c r="AL2" s="194" t="s">
         <v>659</v>
       </c>
-      <c r="AM2" s="202"/>
-      <c r="AN2" s="202"/>
-      <c r="AO2" s="203"/>
-      <c r="AP2" s="201" t="s">
+      <c r="AM2" s="195"/>
+      <c r="AN2" s="195"/>
+      <c r="AO2" s="196"/>
+      <c r="AP2" s="194" t="s">
         <v>660</v>
       </c>
-      <c r="AQ2" s="202"/>
-      <c r="AR2" s="202"/>
-      <c r="AS2" s="203"/>
-      <c r="AT2" s="201" t="s">
+      <c r="AQ2" s="195"/>
+      <c r="AR2" s="195"/>
+      <c r="AS2" s="196"/>
+      <c r="AT2" s="194" t="s">
         <v>722</v>
       </c>
-      <c r="AU2" s="202"/>
-      <c r="AV2" s="202"/>
-      <c r="AW2" s="203"/>
-      <c r="AX2" s="201" t="s">
+      <c r="AU2" s="195"/>
+      <c r="AV2" s="195"/>
+      <c r="AW2" s="196"/>
+      <c r="AX2" s="194" t="s">
         <v>729</v>
       </c>
-      <c r="AY2" s="202"/>
-      <c r="AZ2" s="202"/>
-      <c r="BA2" s="203"/>
+      <c r="AY2" s="195"/>
+      <c r="AZ2" s="195"/>
+      <c r="BA2" s="196"/>
     </row>
     <row r="3" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
-      <c r="B3" s="198"/>
-      <c r="C3" s="198"/>
-      <c r="D3" s="198"/>
-      <c r="E3" s="200"/>
+      <c r="B3" s="202"/>
+      <c r="C3" s="202"/>
+      <c r="D3" s="202"/>
+      <c r="E3" s="204"/>
       <c r="F3" s="80">
         <v>1</v>
       </c>
@@ -26690,6 +26706,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:I2"/>
     <mergeCell ref="AL2:AO2"/>
     <mergeCell ref="AP2:AS2"/>
     <mergeCell ref="AT2:AW2"/>
@@ -26700,12 +26722,6 @@
     <mergeCell ref="Z2:AC2"/>
     <mergeCell ref="AD2:AG2"/>
     <mergeCell ref="AH2:AK2"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:I2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D84" location="ลูกค้า!A1" display="ลูกค้า!A1"/>
@@ -27223,16 +27239,16 @@
     <row r="2" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
-      <c r="C2" s="197" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="197" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="197" t="s">
+      <c r="C2" s="201" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="201" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="201" t="s">
         <v>130</v>
       </c>
-      <c r="F2" s="199" t="s">
+      <c r="F2" s="203" t="s">
         <v>723</v>
       </c>
       <c r="G2" s="205" t="s">
@@ -27299,10 +27315,10 @@
     <row r="3" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
-      <c r="C3" s="198"/>
-      <c r="D3" s="198"/>
-      <c r="E3" s="198"/>
-      <c r="F3" s="200"/>
+      <c r="C3" s="202"/>
+      <c r="D3" s="202"/>
+      <c r="E3" s="202"/>
+      <c r="F3" s="204"/>
       <c r="G3" s="80">
         <v>1</v>
       </c>
@@ -33098,6 +33114,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="AE2:AH2"/>
+    <mergeCell ref="AI2:AL2"/>
+    <mergeCell ref="AM2:AP2"/>
+    <mergeCell ref="AQ2:AT2"/>
+    <mergeCell ref="AA2:AD2"/>
     <mergeCell ref="K2:N2"/>
     <mergeCell ref="O2:R2"/>
     <mergeCell ref="S2:V2"/>
@@ -33107,11 +33128,6 @@
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="G2:J2"/>
-    <mergeCell ref="AE2:AH2"/>
-    <mergeCell ref="AI2:AL2"/>
-    <mergeCell ref="AM2:AP2"/>
-    <mergeCell ref="AQ2:AT2"/>
-    <mergeCell ref="AA2:AD2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E84" location="ลูกค้า!A1" display="ลูกค้า!A1"/>
@@ -33589,98 +33605,98 @@
     <row r="2" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
-      <c r="C2" s="197" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="197" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="197" t="s">
+      <c r="C2" s="201" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="201" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="201" t="s">
         <v>130</v>
       </c>
-      <c r="F2" s="199" t="s">
+      <c r="F2" s="203" t="s">
         <v>723</v>
       </c>
-      <c r="G2" s="194" t="s">
+      <c r="G2" s="197" t="s">
         <v>651</v>
       </c>
-      <c r="H2" s="195"/>
-      <c r="I2" s="195"/>
-      <c r="J2" s="196"/>
-      <c r="K2" s="194" t="s">
+      <c r="H2" s="198"/>
+      <c r="I2" s="198"/>
+      <c r="J2" s="199"/>
+      <c r="K2" s="197" t="s">
         <v>652</v>
       </c>
-      <c r="L2" s="195"/>
-      <c r="M2" s="195"/>
-      <c r="N2" s="196"/>
-      <c r="O2" s="194" t="s">
+      <c r="L2" s="198"/>
+      <c r="M2" s="198"/>
+      <c r="N2" s="199"/>
+      <c r="O2" s="197" t="s">
         <v>653</v>
       </c>
-      <c r="P2" s="195"/>
-      <c r="Q2" s="195"/>
-      <c r="R2" s="196"/>
-      <c r="S2" s="194" t="s">
+      <c r="P2" s="198"/>
+      <c r="Q2" s="198"/>
+      <c r="R2" s="199"/>
+      <c r="S2" s="197" t="s">
         <v>654</v>
       </c>
-      <c r="T2" s="195"/>
-      <c r="U2" s="195"/>
-      <c r="V2" s="204"/>
-      <c r="W2" s="194" t="s">
+      <c r="T2" s="198"/>
+      <c r="U2" s="198"/>
+      <c r="V2" s="200"/>
+      <c r="W2" s="197" t="s">
         <v>655</v>
       </c>
-      <c r="X2" s="195"/>
-      <c r="Y2" s="195"/>
-      <c r="Z2" s="204"/>
-      <c r="AA2" s="201" t="s">
+      <c r="X2" s="198"/>
+      <c r="Y2" s="198"/>
+      <c r="Z2" s="200"/>
+      <c r="AA2" s="194" t="s">
         <v>656</v>
       </c>
-      <c r="AB2" s="202"/>
-      <c r="AC2" s="202"/>
-      <c r="AD2" s="203"/>
-      <c r="AE2" s="201" t="s">
+      <c r="AB2" s="195"/>
+      <c r="AC2" s="195"/>
+      <c r="AD2" s="196"/>
+      <c r="AE2" s="194" t="s">
         <v>657</v>
       </c>
-      <c r="AF2" s="202"/>
-      <c r="AG2" s="202"/>
-      <c r="AH2" s="203"/>
-      <c r="AI2" s="201" t="s">
+      <c r="AF2" s="195"/>
+      <c r="AG2" s="195"/>
+      <c r="AH2" s="196"/>
+      <c r="AI2" s="194" t="s">
         <v>658</v>
       </c>
-      <c r="AJ2" s="202"/>
-      <c r="AK2" s="202"/>
-      <c r="AL2" s="203"/>
-      <c r="AM2" s="201" t="s">
+      <c r="AJ2" s="195"/>
+      <c r="AK2" s="195"/>
+      <c r="AL2" s="196"/>
+      <c r="AM2" s="194" t="s">
         <v>659</v>
       </c>
-      <c r="AN2" s="202"/>
-      <c r="AO2" s="202"/>
-      <c r="AP2" s="203"/>
-      <c r="AQ2" s="201" t="s">
+      <c r="AN2" s="195"/>
+      <c r="AO2" s="195"/>
+      <c r="AP2" s="196"/>
+      <c r="AQ2" s="194" t="s">
         <v>660</v>
       </c>
-      <c r="AR2" s="202"/>
-      <c r="AS2" s="202"/>
-      <c r="AT2" s="203"/>
-      <c r="AU2" s="201" t="s">
+      <c r="AR2" s="195"/>
+      <c r="AS2" s="195"/>
+      <c r="AT2" s="196"/>
+      <c r="AU2" s="194" t="s">
         <v>722</v>
       </c>
-      <c r="AV2" s="202"/>
-      <c r="AW2" s="202"/>
-      <c r="AX2" s="203"/>
-      <c r="AY2" s="201" t="s">
+      <c r="AV2" s="195"/>
+      <c r="AW2" s="195"/>
+      <c r="AX2" s="196"/>
+      <c r="AY2" s="194" t="s">
         <v>729</v>
       </c>
-      <c r="AZ2" s="202"/>
-      <c r="BA2" s="202"/>
-      <c r="BB2" s="203"/>
+      <c r="AZ2" s="195"/>
+      <c r="BA2" s="195"/>
+      <c r="BB2" s="196"/>
     </row>
     <row r="3" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
-      <c r="C3" s="198"/>
-      <c r="D3" s="198"/>
-      <c r="E3" s="198"/>
-      <c r="F3" s="200"/>
+      <c r="C3" s="202"/>
+      <c r="D3" s="202"/>
+      <c r="E3" s="202"/>
+      <c r="F3" s="204"/>
       <c r="G3" s="80">
         <v>1</v>
       </c>
@@ -39093,11 +39109,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="O2:R2"/>
     <mergeCell ref="AU2:AX2"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="AY2:BB2"/>
@@ -39109,6 +39120,11 @@
     <mergeCell ref="AM2:AP2"/>
     <mergeCell ref="AQ2:AT2"/>
     <mergeCell ref="S2:V2"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="O2:R2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E84" location="ลูกค้า!A1" display="ลูกค้า!A1"/>
@@ -39299,7 +39315,7 @@
       <c r="A1" s="211" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="197" t="s">
+      <c r="B1" s="201" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="213" t="s">
@@ -39327,7 +39343,7 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="212"/>
-      <c r="B2" s="198"/>
+      <c r="B2" s="202"/>
       <c r="C2" s="1">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
-stock hist. -move up/down productlist -province
</commit_message>
<xml_diff>
--- a/_Doc/Feature.xlsx
+++ b/_Doc/Feature.xlsx
@@ -4,54 +4,54 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="795" windowWidth="19080" windowHeight="6705" tabRatio="884" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="855" windowWidth="19080" windowHeight="6645" tabRatio="884" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="46" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="45" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="46" state="hidden" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="45" state="hidden" r:id="rId2"/>
     <sheet name="UpdateList" sheetId="43" r:id="rId3"/>
     <sheet name="Menu" sheetId="42" r:id="rId4"/>
     <sheet name="TimeLine" sheetId="39" r:id="rId5"/>
     <sheet name="Windows(old)" sheetId="41" state="hidden" r:id="rId6"/>
-    <sheet name="Windows (2)" sheetId="44" r:id="rId7"/>
+    <sheet name="Windows (2)" sheetId="44" state="hidden" r:id="rId7"/>
     <sheet name="Windows" sheetId="38" r:id="rId8"/>
     <sheet name="Web" sheetId="40" r:id="rId9"/>
     <sheet name="Main" sheetId="1" state="hidden" r:id="rId10"/>
-    <sheet name="Admin" sheetId="2" r:id="rId11"/>
-    <sheet name="ลูกค้า" sheetId="3" r:id="rId12"/>
-    <sheet name="เจ้าหนี้" sheetId="4" r:id="rId13"/>
-    <sheet name="สินค้า" sheetId="6" r:id="rId14"/>
-    <sheet name="ราคาขาย" sheetId="5" r:id="rId15"/>
-    <sheet name="เครดิต" sheetId="7" r:id="rId16"/>
-    <sheet name="เสนอราคา" sheetId="8" r:id="rId17"/>
-    <sheet name="จองสินค้า" sheetId="9" r:id="rId18"/>
-    <sheet name="สั่งขาย" sheetId="10" r:id="rId19"/>
-    <sheet name="ส่งของ" sheetId="11" r:id="rId20"/>
-    <sheet name="คืน" sheetId="12" r:id="rId21"/>
-    <sheet name="เพิ่มสินค้า" sheetId="13" r:id="rId22"/>
-    <sheet name="มัดจำ" sheetId="14" r:id="rId23"/>
-    <sheet name="คืนมัดจำ" sheetId="15" r:id="rId24"/>
-    <sheet name="ตั้งลูกหนี้" sheetId="16" r:id="rId25"/>
-    <sheet name="ลดลูกหนี้" sheetId="17" r:id="rId26"/>
-    <sheet name="วางบิล" sheetId="18" r:id="rId27"/>
-    <sheet name="ใบเสร็จ" sheetId="19" r:id="rId28"/>
-    <sheet name="ชำระหนี้ " sheetId="20" r:id="rId29"/>
-    <sheet name="สั่งซื้อ" sheetId="21" r:id="rId30"/>
-    <sheet name="รับสินค้า" sheetId="22" r:id="rId31"/>
-    <sheet name="ตั้งหนี้" sheetId="23" r:id="rId32"/>
-    <sheet name="ส่งคืน" sheetId="24" r:id="rId33"/>
-    <sheet name="ตั้งเจ้าหนี้" sheetId="25" r:id="rId34"/>
-    <sheet name="ลดเจ้าหนี้" sheetId="26" r:id="rId35"/>
-    <sheet name="รับวางบิล" sheetId="27" r:id="rId36"/>
-    <sheet name="เตรียมจ่าย" sheetId="29" r:id="rId37"/>
-    <sheet name="จ่ายหนี้ " sheetId="28" r:id="rId38"/>
-    <sheet name="คลัง" sheetId="30" r:id="rId39"/>
-    <sheet name="บัญชี" sheetId="31" r:id="rId40"/>
-    <sheet name="เช็ค " sheetId="32" r:id="rId41"/>
-    <sheet name="สินทรัพย์ " sheetId="33" r:id="rId42"/>
-    <sheet name="ทดรองจ่าย" sheetId="34" r:id="rId43"/>
-    <sheet name="ขนส่ง" sheetId="35" r:id="rId44"/>
-    <sheet name="MIS" sheetId="36" r:id="rId45"/>
+    <sheet name="Admin" sheetId="2" state="hidden" r:id="rId11"/>
+    <sheet name="ลูกค้า" sheetId="3" state="hidden" r:id="rId12"/>
+    <sheet name="เจ้าหนี้" sheetId="4" state="hidden" r:id="rId13"/>
+    <sheet name="สินค้า" sheetId="6" state="hidden" r:id="rId14"/>
+    <sheet name="ราคาขาย" sheetId="5" state="hidden" r:id="rId15"/>
+    <sheet name="เครดิต" sheetId="7" state="hidden" r:id="rId16"/>
+    <sheet name="เสนอราคา" sheetId="8" state="hidden" r:id="rId17"/>
+    <sheet name="จองสินค้า" sheetId="9" state="hidden" r:id="rId18"/>
+    <sheet name="สั่งขาย" sheetId="10" state="hidden" r:id="rId19"/>
+    <sheet name="ส่งของ" sheetId="11" state="hidden" r:id="rId20"/>
+    <sheet name="คืน" sheetId="12" state="hidden" r:id="rId21"/>
+    <sheet name="เพิ่มสินค้า" sheetId="13" state="hidden" r:id="rId22"/>
+    <sheet name="มัดจำ" sheetId="14" state="hidden" r:id="rId23"/>
+    <sheet name="คืนมัดจำ" sheetId="15" state="hidden" r:id="rId24"/>
+    <sheet name="ตั้งลูกหนี้" sheetId="16" state="hidden" r:id="rId25"/>
+    <sheet name="ลดลูกหนี้" sheetId="17" state="hidden" r:id="rId26"/>
+    <sheet name="วางบิล" sheetId="18" state="hidden" r:id="rId27"/>
+    <sheet name="ใบเสร็จ" sheetId="19" state="hidden" r:id="rId28"/>
+    <sheet name="ชำระหนี้ " sheetId="20" state="hidden" r:id="rId29"/>
+    <sheet name="สั่งซื้อ" sheetId="21" state="hidden" r:id="rId30"/>
+    <sheet name="รับสินค้า" sheetId="22" state="hidden" r:id="rId31"/>
+    <sheet name="ตั้งหนี้" sheetId="23" state="hidden" r:id="rId32"/>
+    <sheet name="ส่งคืน" sheetId="24" state="hidden" r:id="rId33"/>
+    <sheet name="ตั้งเจ้าหนี้" sheetId="25" state="hidden" r:id="rId34"/>
+    <sheet name="ลดเจ้าหนี้" sheetId="26" state="hidden" r:id="rId35"/>
+    <sheet name="รับวางบิล" sheetId="27" state="hidden" r:id="rId36"/>
+    <sheet name="เตรียมจ่าย" sheetId="29" state="hidden" r:id="rId37"/>
+    <sheet name="จ่ายหนี้ " sheetId="28" state="hidden" r:id="rId38"/>
+    <sheet name="คลัง" sheetId="30" state="hidden" r:id="rId39"/>
+    <sheet name="บัญชี" sheetId="31" state="hidden" r:id="rId40"/>
+    <sheet name="เช็ค " sheetId="32" state="hidden" r:id="rId41"/>
+    <sheet name="สินทรัพย์ " sheetId="33" state="hidden" r:id="rId42"/>
+    <sheet name="ทดรองจ่าย" sheetId="34" state="hidden" r:id="rId43"/>
+    <sheet name="ขนส่ง" sheetId="35" state="hidden" r:id="rId44"/>
+    <sheet name="MIS" sheetId="36" state="hidden" r:id="rId45"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Menu!$A$1:$R$57</definedName>
@@ -226,7 +226,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2428" uniqueCount="1704">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2436" uniqueCount="1712">
   <si>
     <t>No.</t>
   </si>
@@ -4788,9 +4788,6 @@
     <t>update Orders  set IsMakePO=0;</t>
   </si>
   <si>
-    <t>set error end</t>
-  </si>
-  <si>
     <t>alter table ProductList add IsMerge int;</t>
   </si>
   <si>
@@ -5011,9 +5008,6 @@
   </si>
   <si>
     <t>เช็ค Stock มีหลายหน่วย</t>
-  </si>
-  <si>
-    <t>menu add pk</t>
   </si>
   <si>
     <t>1.0.0.69</t>
@@ -5410,9 +5404,6 @@
   </si>
   <si>
     <t>ใบเสนอราคาที่กลับมาแก้ไข หมายเหตุแล้วจะไม่แสดงครับ</t>
-  </si>
-  <si>
-    <t>สินค้านี้มี sn เดียวใช่ไหมครับ</t>
   </si>
   <si>
     <t>เบย์ลองแล้วครับ มันคำนวน ที่แถวมันอ่ะครับ อยากให้มันเลือกได้ว่าจะคำนวนแถวหรือจาก cost อ่ะครับ</t>
@@ -5745,6 +5736,39 @@
   </si>
   <si>
     <t>update  ProductList set PriceMain=Price;</t>
+  </si>
+  <si>
+    <t>alter table Province add IsInActive  int ;</t>
+  </si>
+  <si>
+    <t>alter table Province add IsDelete  int ;</t>
+  </si>
+  <si>
+    <t>alter table Province add CreateBy  bigint ;</t>
+  </si>
+  <si>
+    <t>alter table Province add CreateTime  datetime ;</t>
+  </si>
+  <si>
+    <t>alter table Province add ModifiedBy  bigint ;</t>
+  </si>
+  <si>
+    <t>alter table Province add ModifiedTime  datetime ;</t>
+  </si>
+  <si>
+    <t>alter table Province add Remark  nvarchar(100) ;</t>
+  </si>
+  <si>
+    <t>update Province set IsInActive=0;</t>
+  </si>
+  <si>
+    <t>update Province set IsDelete=0;</t>
+  </si>
+  <si>
+    <t>กำหนดราคา  เพิ่มเงื่อนไขการคำนวณให้เลือกใช้ cost เป็นตัวตั้ง หรือใช้ราคานั้นๆ</t>
+  </si>
+  <si>
+    <t>รายการสินค้าสามารถปรับเลื่อนขึ้นลงได้</t>
   </si>
 </sst>
 </file>
@@ -6046,12 +6070,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color rgb="FF2A411F"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="14"/>
       <color theme="1" tint="0.499984740745262"/>
       <name val="Cordia New"/>
@@ -6061,6 +6079,12 @@
       <sz val="9"/>
       <color theme="2" tint="-0.249977111117893"/>
       <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Cordia New"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -6709,27 +6733,17 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -6738,9 +6752,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -6754,6 +6765,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -6788,6 +6811,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -7190,7 +7214,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:B102"/>
   <sheetViews>
-    <sheetView topLeftCell="A82" workbookViewId="0">
+    <sheetView topLeftCell="A79" workbookViewId="0">
       <selection activeCell="B95" sqref="B95"/>
     </sheetView>
   </sheetViews>
@@ -7566,27 +7590,27 @@
     </row>
     <row r="95" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
-        <v>1503</v>
+        <v>1502</v>
       </c>
     </row>
     <row r="99" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B99" s="163" t="s">
-        <v>1504</v>
+        <v>1503</v>
       </c>
     </row>
     <row r="100" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
-        <v>1505</v>
+        <v>1504</v>
       </c>
     </row>
     <row r="101" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
-        <v>1506</v>
+        <v>1505</v>
       </c>
     </row>
     <row r="102" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
-        <v>1507</v>
+        <v>1506</v>
       </c>
     </row>
   </sheetData>
@@ -7618,20 +7642,20 @@
       <c r="B1" s="2"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="201" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="201" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="201" t="s">
+      <c r="A2" s="196" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="196" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="196" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="202"/>
-      <c r="B3" s="202"/>
-      <c r="C3" s="202"/>
+      <c r="A3" s="197"/>
+      <c r="B3" s="197"/>
+      <c r="C3" s="197"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
@@ -8447,7 +8471,7 @@
   <dimension ref="A2:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8726,100 +8750,100 @@
       </c>
     </row>
     <row r="31" spans="2:3" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="B31" s="214" t="s">
+      <c r="B31" s="213" t="s">
         <v>162</v>
       </c>
-      <c r="C31" s="214"/>
+      <c r="C31" s="213"/>
     </row>
     <row r="32" spans="2:3" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="B32" s="214" t="s">
+      <c r="B32" s="213" t="s">
         <v>163</v>
       </c>
-      <c r="C32" s="214"/>
+      <c r="C32" s="213"/>
     </row>
     <row r="33" spans="2:3" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="B33" s="214" t="s">
+      <c r="B33" s="213" t="s">
         <v>164</v>
       </c>
-      <c r="C33" s="214"/>
+      <c r="C33" s="213"/>
     </row>
     <row r="34" spans="2:3" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="B34" s="214" t="s">
+      <c r="B34" s="213" t="s">
         <v>165</v>
       </c>
-      <c r="C34" s="214"/>
+      <c r="C34" s="213"/>
     </row>
     <row r="35" spans="2:3" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="B35" s="214" t="s">
+      <c r="B35" s="213" t="s">
         <v>166</v>
       </c>
-      <c r="C35" s="214"/>
+      <c r="C35" s="213"/>
     </row>
     <row r="36" spans="2:3" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="B36" s="214" t="s">
+      <c r="B36" s="213" t="s">
         <v>167</v>
       </c>
-      <c r="C36" s="214"/>
+      <c r="C36" s="213"/>
     </row>
     <row r="37" spans="2:3" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="B37" s="214" t="s">
+      <c r="B37" s="213" t="s">
         <v>168</v>
       </c>
-      <c r="C37" s="214"/>
+      <c r="C37" s="213"/>
     </row>
     <row r="38" spans="2:3" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="B38" s="214" t="s">
+      <c r="B38" s="213" t="s">
         <v>169</v>
       </c>
-      <c r="C38" s="214"/>
+      <c r="C38" s="213"/>
     </row>
     <row r="39" spans="2:3" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="B39" s="214" t="s">
+      <c r="B39" s="213" t="s">
         <v>170</v>
       </c>
-      <c r="C39" s="214"/>
+      <c r="C39" s="213"/>
     </row>
     <row r="40" spans="2:3" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="B40" s="214" t="s">
+      <c r="B40" s="213" t="s">
         <v>171</v>
       </c>
-      <c r="C40" s="214"/>
+      <c r="C40" s="213"/>
     </row>
     <row r="41" spans="2:3" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="B41" s="214" t="s">
+      <c r="B41" s="213" t="s">
         <v>172</v>
       </c>
-      <c r="C41" s="214"/>
+      <c r="C41" s="213"/>
     </row>
     <row r="42" spans="2:3" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="B42" s="214" t="s">
+      <c r="B42" s="213" t="s">
         <v>173</v>
       </c>
-      <c r="C42" s="214"/>
+      <c r="C42" s="213"/>
     </row>
     <row r="43" spans="2:3" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="B43" s="214" t="s">
+      <c r="B43" s="213" t="s">
         <v>174</v>
       </c>
-      <c r="C43" s="214"/>
+      <c r="C43" s="213"/>
     </row>
     <row r="44" spans="2:3" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="B44" s="214" t="s">
+      <c r="B44" s="213" t="s">
         <v>175</v>
       </c>
-      <c r="C44" s="214"/>
+      <c r="C44" s="213"/>
     </row>
     <row r="45" spans="2:3" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="B45" s="214" t="s">
+      <c r="B45" s="213" t="s">
         <v>176</v>
       </c>
-      <c r="C45" s="214"/>
+      <c r="C45" s="213"/>
     </row>
     <row r="46" spans="2:3" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="B46" s="214" t="s">
+      <c r="B46" s="213" t="s">
         <v>177</v>
       </c>
-      <c r="C46" s="214"/>
+      <c r="C46" s="213"/>
     </row>
     <row r="47" spans="2:3" ht="18.75" x14ac:dyDescent="0.45">
       <c r="B47" s="20" t="s">
@@ -8833,6 +8857,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
     <mergeCell ref="B43:C43"/>
     <mergeCell ref="B44:C44"/>
     <mergeCell ref="B45:C45"/>
@@ -8843,12 +8873,6 @@
     <mergeCell ref="B40:C40"/>
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -8862,7 +8886,9 @@
   </sheetPr>
   <dimension ref="B2:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -8963,7 +8989,7 @@
   <dimension ref="A2:C25"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9277,7 +9303,7 @@
   <dimension ref="B2:B14"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9362,7 +9388,9 @@
   </sheetPr>
   <dimension ref="B2:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -9437,7 +9465,7 @@
   <dimension ref="B2:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9530,7 +9558,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A125"/>
   <sheetViews>
-    <sheetView topLeftCell="A88" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A34" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="A103" sqref="A103"/>
     </sheetView>
   </sheetViews>
@@ -9961,82 +9989,82 @@
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" s="180" t="s">
-        <v>1457</v>
+        <v>1456</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" s="180" t="s">
-        <v>1455</v>
+        <v>1454</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" s="180" t="s">
-        <v>1456</v>
+        <v>1455</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" s="180" t="s">
-        <v>1471</v>
+        <v>1470</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>1472</v>
+        <v>1471</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" s="161" t="s">
-        <v>1560</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" s="167" t="s">
-        <v>1563</v>
+        <v>1561</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" s="180" t="s">
-        <v>1564</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" s="163" t="s">
-        <v>1565</v>
+        <v>1563</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" s="163" t="s">
-        <v>1570</v>
+        <v>1568</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>1589</v>
+        <v>1587</v>
       </c>
     </row>
     <row r="120" spans="1:1" ht="105" x14ac:dyDescent="0.25">
       <c r="A120" s="121" t="s">
-        <v>1590</v>
+        <v>1588</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>1591</v>
+        <v>1589</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>1597</v>
+        <v>1595</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>1596</v>
+        <v>1594</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>1598</v>
+        <v>1596</v>
       </c>
     </row>
   </sheetData>
@@ -10204,7 +10232,9 @@
   </sheetPr>
   <dimension ref="B2:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -10444,7 +10474,7 @@
   <dimension ref="B2:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10484,7 +10514,9 @@
   </sheetPr>
   <dimension ref="B2:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -10524,7 +10556,7 @@
   <dimension ref="B2:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10560,7 +10592,7 @@
   <dimension ref="B2:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10620,7 +10652,9 @@
   </sheetPr>
   <dimension ref="B2:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -10669,7 +10703,9 @@
   </sheetPr>
   <dimension ref="B2:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -10761,10 +10797,10 @@
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
-  <dimension ref="A1:C372"/>
+  <dimension ref="A1:C378"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A342" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C353" sqref="C352:C353"/>
+    <sheetView tabSelected="1" topLeftCell="A369" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B377" sqref="B377"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21.75" x14ac:dyDescent="0.5"/>
@@ -10797,7 +10833,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="B4" s="192" t="s">
+      <c r="B4" s="191" t="s">
         <v>993</v>
       </c>
       <c r="C4" s="153" t="s">
@@ -10805,13 +10841,13 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="B5" s="192"/>
+      <c r="B5" s="191"/>
       <c r="C5" s="151" t="s">
         <v>991</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="B6" s="192"/>
+      <c r="B6" s="191"/>
       <c r="C6" s="151" t="s">
         <v>992</v>
       </c>
@@ -11002,7 +11038,7 @@
       <c r="B37" s="151" t="s">
         <v>1027</v>
       </c>
-      <c r="C37" s="193" t="s">
+      <c r="C37" s="192" t="s">
         <v>1061</v>
       </c>
     </row>
@@ -11010,61 +11046,61 @@
       <c r="B38" s="151" t="s">
         <v>1028</v>
       </c>
-      <c r="C38" s="193"/>
+      <c r="C38" s="192"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B39" s="151" t="s">
         <v>1053</v>
       </c>
-      <c r="C39" s="193"/>
+      <c r="C39" s="192"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B40" s="151" t="s">
         <v>1057</v>
       </c>
-      <c r="C40" s="193"/>
+      <c r="C40" s="192"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B41" s="151" t="s">
         <v>1058</v>
       </c>
-      <c r="C41" s="193"/>
+      <c r="C41" s="192"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B42" s="151" t="s">
         <v>1059</v>
       </c>
-      <c r="C42" s="193"/>
+      <c r="C42" s="192"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B43" s="151" t="s">
         <v>1063</v>
       </c>
-      <c r="C43" s="193"/>
+      <c r="C43" s="192"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B44" s="151" t="s">
         <v>1062</v>
       </c>
-      <c r="C44" s="193"/>
+      <c r="C44" s="192"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="C45" s="193"/>
+      <c r="C45" s="192"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="C46" s="193"/>
+      <c r="C46" s="192"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="C47" s="193"/>
+      <c r="C47" s="192"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="C48" s="193"/>
+      <c r="C48" s="192"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="C49" s="193"/>
+      <c r="C49" s="192"/>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="C50" s="193"/>
+      <c r="C50" s="192"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A51" s="151" t="s">
@@ -11953,7 +11989,7 @@
         <v>1433</v>
       </c>
       <c r="B212" s="151" t="s">
-        <v>1454</v>
+        <v>1453</v>
       </c>
       <c r="C212" s="151" t="s">
         <v>1432</v>
@@ -11961,7 +11997,7 @@
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B213" s="151" t="s">
-        <v>1473</v>
+        <v>1472</v>
       </c>
       <c r="C213" s="151" t="s">
         <v>1435</v>
@@ -11969,7 +12005,7 @@
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B214" s="151" t="s">
-        <v>1459</v>
+        <v>1458</v>
       </c>
       <c r="C214" s="151" t="s">
         <v>1450</v>
@@ -11977,7 +12013,7 @@
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B215" s="151" t="s">
-        <v>1464</v>
+        <v>1463</v>
       </c>
       <c r="C215" s="151" t="s">
         <v>1436</v>
@@ -11985,7 +12021,7 @@
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B216" s="120" t="s">
-        <v>1465</v>
+        <v>1464</v>
       </c>
       <c r="C216" s="151" t="s">
         <v>1442</v>
@@ -11993,7 +12029,7 @@
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B217" s="151" t="s">
-        <v>1469</v>
+        <v>1468</v>
       </c>
       <c r="C217" s="151" t="s">
         <v>1448</v>
@@ -12001,7 +12037,7 @@
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B218" s="151" t="s">
-        <v>1474</v>
+        <v>1473</v>
       </c>
       <c r="C218" s="151" t="s">
         <v>1449</v>
@@ -12009,65 +12045,65 @@
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.5">
       <c r="C219" s="151" t="s">
-        <v>1452</v>
+        <v>1451</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.5">
       <c r="C220" s="151" t="s">
-        <v>1453</v>
+        <v>1452</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.5">
       <c r="C221" s="151" t="s">
-        <v>1458</v>
+        <v>1457</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.5">
       <c r="C222" s="151" t="s">
-        <v>1460</v>
+        <v>1459</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.5">
       <c r="C223" s="151" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.5">
       <c r="C224" s="151" t="s">
-        <v>1462</v>
+        <v>1461</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.5">
       <c r="C225" s="151" t="s">
-        <v>1463</v>
+        <v>1462</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.5">
       <c r="C226" s="151" t="s">
-        <v>1470</v>
+        <v>1469</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.5">
       <c r="C227" s="151" t="s">
-        <v>1475</v>
+        <v>1474</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.5">
       <c r="C228" s="151" t="s">
-        <v>1476</v>
+        <v>1475</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.5">
       <c r="C229" s="151" t="s">
-        <v>1477</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A231" s="151" t="s">
-        <v>1479</v>
+        <v>1478</v>
       </c>
       <c r="B231" s="151" t="s">
-        <v>1478</v>
+        <v>1477</v>
       </c>
       <c r="C231" s="151" t="s">
         <v>1450</v>
@@ -12080,208 +12116,208 @@
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.5">
       <c r="C233" s="151" t="s">
-        <v>1453</v>
+        <v>1452</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.5">
       <c r="C234" s="151" t="s">
-        <v>1463</v>
+        <v>1462</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A235" s="151" t="s">
-        <v>1481</v>
+        <v>1480</v>
       </c>
       <c r="B235" s="151" t="s">
-        <v>1480</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A236" s="151" t="s">
-        <v>1483</v>
+        <v>1482</v>
       </c>
       <c r="B236" s="151" t="s">
-        <v>1482</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A238" s="151" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
       <c r="B238" s="151" t="s">
-        <v>1493</v>
+        <v>1492</v>
       </c>
       <c r="C238" s="151" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B239" s="151" t="s">
-        <v>1494</v>
+        <v>1493</v>
       </c>
       <c r="C239" s="151" t="s">
-        <v>1490</v>
+        <v>1489</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B240" s="151" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
       <c r="C240" s="151" t="s">
-        <v>1491</v>
+        <v>1490</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.5">
       <c r="C241" s="151" t="s">
-        <v>1492</v>
+        <v>1491</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.5">
       <c r="C242" s="151" t="s">
-        <v>1496</v>
+        <v>1495</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A244" s="151" t="s">
-        <v>1498</v>
+        <v>1497</v>
       </c>
       <c r="B244" s="151" t="s">
-        <v>1497</v>
+        <v>1496</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A246" s="151" t="s">
+        <v>1498</v>
+      </c>
+      <c r="B246" s="151" t="s">
+        <v>1501</v>
+      </c>
+      <c r="C246" s="151" t="s">
         <v>1499</v>
-      </c>
-      <c r="B246" s="151" t="s">
-        <v>1502</v>
-      </c>
-      <c r="C246" s="151" t="s">
-        <v>1500</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.5">
       <c r="C247" s="151" t="s">
-        <v>1501</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A249" s="151" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
       <c r="B249" s="151" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
       <c r="C249" s="151" t="s">
-        <v>1515</v>
+        <v>1514</v>
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B250" s="151" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A252" s="151" t="s">
+        <v>1515</v>
+      </c>
+      <c r="B252" s="151" t="s">
         <v>1516</v>
       </c>
-      <c r="B252" s="151" t="s">
-        <v>1517</v>
-      </c>
       <c r="C252" s="151" t="s">
-        <v>1510</v>
+        <v>1509</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B253" s="151" t="s">
-        <v>1518</v>
+        <v>1517</v>
       </c>
       <c r="C253" s="151" t="s">
-        <v>1508</v>
+        <v>1507</v>
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.5">
       <c r="C254" s="151" t="s">
-        <v>1511</v>
+        <v>1510</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.5">
       <c r="C255" s="151" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A257" s="151" t="s">
+        <v>1520</v>
+      </c>
+      <c r="B257" s="151" t="s">
         <v>1521</v>
       </c>
-      <c r="B257" s="151" t="s">
-        <v>1522</v>
-      </c>
       <c r="C257" s="151" t="s">
-        <v>1520</v>
+        <v>1519</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B258" s="151" t="s">
-        <v>1523</v>
+        <v>1522</v>
       </c>
       <c r="C258" s="151" t="s">
-        <v>1519</v>
+        <v>1518</v>
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A260" s="151" t="s">
-        <v>1527</v>
+        <v>1525</v>
       </c>
       <c r="C260" s="151" t="s">
-        <v>1524</v>
+        <v>1523</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A261" s="151" t="s">
-        <v>1528</v>
+        <v>1526</v>
       </c>
       <c r="B261" s="151" t="s">
-        <v>1529</v>
+        <v>1527</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A262" s="151" t="s">
-        <v>1530</v>
+        <v>1528</v>
       </c>
       <c r="B262" s="151" t="s">
-        <v>1531</v>
+        <v>1529</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A263" s="151" t="s">
-        <v>1534</v>
+        <v>1532</v>
       </c>
       <c r="B263" s="151" t="s">
+        <v>1533</v>
+      </c>
+      <c r="C263" s="185" t="s">
         <v>1535</v>
-      </c>
-      <c r="C263" s="185" t="s">
-        <v>1537</v>
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A264" s="151" t="s">
-        <v>1539</v>
+        <v>1537</v>
       </c>
       <c r="B264" s="151" t="s">
-        <v>1538</v>
+        <v>1536</v>
       </c>
       <c r="C264" s="185"/>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B265" s="151" t="s">
-        <v>1540</v>
+        <v>1538</v>
       </c>
       <c r="C265" s="185"/>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B266" s="151" t="s">
-        <v>1541</v>
+        <v>1539</v>
       </c>
       <c r="C266" s="185"/>
     </row>
@@ -12290,45 +12326,45 @@
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A268" s="151" t="s">
-        <v>1571</v>
+        <v>1569</v>
       </c>
       <c r="B268" s="151" t="s">
-        <v>1546</v>
+        <v>1544</v>
       </c>
       <c r="C268" s="185" t="s">
-        <v>1543</v>
+        <v>1541</v>
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B269" s="151" t="s">
-        <v>1574</v>
+        <v>1572</v>
       </c>
       <c r="C269" s="185" t="s">
-        <v>1544</v>
+        <v>1542</v>
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B270" s="151" t="s">
-        <v>1572</v>
+        <v>1570</v>
       </c>
       <c r="C270" s="151" t="s">
-        <v>1545</v>
+        <v>1543</v>
       </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B271" s="151" t="s">
-        <v>1573</v>
+        <v>1571</v>
       </c>
       <c r="C271" s="185"/>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.5">
       <c r="C272" s="185" t="s">
-        <v>1550</v>
+        <v>1548</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.5">
       <c r="C273" s="185" t="s">
-        <v>1554</v>
+        <v>1552</v>
       </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.5">
@@ -12336,344 +12372,344 @@
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.5">
       <c r="C275" s="151" t="s">
-        <v>1561</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="276" spans="1:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="C276" s="185" t="s">
-        <v>1562</v>
+        <v>1560</v>
       </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.5">
       <c r="C277" s="185" t="s">
-        <v>1558</v>
+        <v>1556</v>
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.5">
       <c r="C278" s="151" t="s">
-        <v>1559</v>
+        <v>1557</v>
       </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.5">
       <c r="C279" s="151" t="s">
-        <v>1569</v>
+        <v>1567</v>
       </c>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A281" s="151" t="s">
-        <v>1575</v>
+        <v>1573</v>
       </c>
       <c r="B281" s="151" t="s">
-        <v>1576</v>
+        <v>1574</v>
       </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B282" s="151" t="s">
-        <v>1577</v>
+        <v>1575</v>
       </c>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A284" s="151" t="s">
-        <v>1578</v>
+        <v>1576</v>
       </c>
       <c r="B284" s="151" t="s">
-        <v>1579</v>
+        <v>1577</v>
       </c>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B285" s="151" t="s">
-        <v>1580</v>
+        <v>1578</v>
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A287" s="151" t="s">
-        <v>1581</v>
+        <v>1579</v>
       </c>
       <c r="B287" s="151" t="s">
-        <v>1582</v>
+        <v>1580</v>
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A288" s="151" t="s">
-        <v>1583</v>
+        <v>1581</v>
       </c>
       <c r="B288" s="151" t="s">
-        <v>1584</v>
+        <v>1582</v>
       </c>
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A290" s="151" t="s">
-        <v>1614</v>
+        <v>1612</v>
       </c>
       <c r="B290" s="151" t="s">
-        <v>1587</v>
+        <v>1585</v>
       </c>
       <c r="C290" s="151" t="s">
-        <v>1613</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B291" s="151" t="s">
-        <v>1588</v>
+        <v>1586</v>
       </c>
       <c r="C291" s="151" t="s">
-        <v>1595</v>
+        <v>1593</v>
       </c>
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B292" s="151" t="s">
-        <v>1599</v>
+        <v>1597</v>
       </c>
       <c r="C292" s="151" t="s">
-        <v>1609</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B293" s="151" t="s">
-        <v>1605</v>
+        <v>1603</v>
       </c>
       <c r="C293" s="151" t="s">
-        <v>1610</v>
+        <v>1608</v>
       </c>
     </row>
     <row r="294" spans="1:3" ht="87" x14ac:dyDescent="0.5">
       <c r="B294" s="151" t="s">
-        <v>1606</v>
+        <v>1604</v>
       </c>
       <c r="C294" s="152" t="s">
-        <v>1607</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B295" s="151" t="s">
-        <v>1611</v>
+        <v>1609</v>
       </c>
       <c r="C295" s="151" t="s">
-        <v>1608</v>
+        <v>1606</v>
       </c>
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A297" s="151" t="s">
-        <v>1616</v>
+        <v>1614</v>
       </c>
       <c r="B297" s="151" t="s">
-        <v>1615</v>
+        <v>1613</v>
       </c>
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B298" s="151" t="s">
-        <v>1617</v>
+        <v>1615</v>
       </c>
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B299" s="151" t="s">
-        <v>1621</v>
+        <v>1619</v>
       </c>
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B300" s="151" t="s">
-        <v>1618</v>
+        <v>1616</v>
       </c>
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B301" s="151" t="s">
-        <v>1619</v>
+        <v>1617</v>
       </c>
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B302" s="151" t="s">
-        <v>1620</v>
+        <v>1618</v>
       </c>
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A304" s="151" t="s">
-        <v>1629</v>
+        <v>1627</v>
       </c>
       <c r="B304" s="151" t="s">
-        <v>1622</v>
+        <v>1620</v>
       </c>
     </row>
     <row r="305" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B305" s="151" t="s">
-        <v>1623</v>
+        <v>1621</v>
       </c>
     </row>
     <row r="306" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B306" s="151" t="s">
-        <v>1627</v>
+        <v>1625</v>
       </c>
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B307" s="151" t="s">
-        <v>1628</v>
+        <v>1626</v>
       </c>
     </row>
     <row r="309" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A309" s="151" t="s">
-        <v>1636</v>
+        <v>1634</v>
       </c>
       <c r="B309" s="151" t="s">
-        <v>1632</v>
+        <v>1630</v>
       </c>
       <c r="C309" s="151" t="s">
-        <v>1630</v>
+        <v>1628</v>
       </c>
     </row>
     <row r="310" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B310" s="151" t="s">
-        <v>1633</v>
+        <v>1631</v>
       </c>
       <c r="C310" s="151" t="s">
-        <v>1631</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="311" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B311" s="151" t="s">
-        <v>1634</v>
+        <v>1632</v>
       </c>
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A313" s="151" t="s">
-        <v>1641</v>
+        <v>1639</v>
       </c>
       <c r="B313" s="151" t="s">
-        <v>1635</v>
+        <v>1633</v>
       </c>
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B314" s="151" t="s">
-        <v>1637</v>
+        <v>1635</v>
       </c>
     </row>
     <row r="315" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B315" s="151" t="s">
-        <v>1638</v>
+        <v>1636</v>
       </c>
     </row>
     <row r="316" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B316" s="151" t="s">
-        <v>1639</v>
+        <v>1637</v>
       </c>
     </row>
     <row r="317" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B317" s="151" t="s">
-        <v>1640</v>
+        <v>1638</v>
       </c>
     </row>
     <row r="319" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A319" s="151" t="s">
-        <v>1651</v>
+        <v>1648</v>
       </c>
       <c r="B319" s="151" t="s">
-        <v>1652</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="320" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B320" s="151" t="s">
-        <v>1653</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="321" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B321" s="151" t="s">
-        <v>1654</v>
+        <v>1651</v>
       </c>
     </row>
     <row r="322" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B322" s="151" t="s">
-        <v>1655</v>
+        <v>1652</v>
       </c>
     </row>
     <row r="324" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A324" s="151" t="s">
-        <v>1656</v>
+        <v>1653</v>
       </c>
       <c r="B324" s="151" t="s">
-        <v>1657</v>
+        <v>1654</v>
       </c>
     </row>
     <row r="325" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A325" s="151" t="s">
-        <v>1658</v>
+        <v>1655</v>
       </c>
       <c r="B325" s="151" t="s">
-        <v>1659</v>
+        <v>1656</v>
       </c>
     </row>
     <row r="327" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A327" s="151" t="s">
-        <v>1673</v>
+        <v>1670</v>
       </c>
       <c r="B327" s="151" t="s">
-        <v>1660</v>
+        <v>1657</v>
       </c>
       <c r="C327" s="151" t="s">
-        <v>1669</v>
+        <v>1666</v>
       </c>
     </row>
     <row r="328" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B328" s="151" t="s">
-        <v>1672</v>
+        <v>1669</v>
       </c>
       <c r="C328" s="151" t="s">
-        <v>1670</v>
+        <v>1667</v>
       </c>
     </row>
     <row r="329" spans="1:3" x14ac:dyDescent="0.5">
       <c r="C329" s="185" t="s">
-        <v>1662</v>
+        <v>1659</v>
       </c>
     </row>
     <row r="330" spans="1:3" x14ac:dyDescent="0.5">
       <c r="C330" s="151" t="s">
-        <v>1630</v>
+        <v>1628</v>
       </c>
     </row>
     <row r="331" spans="1:3" x14ac:dyDescent="0.5">
       <c r="C331" s="151" t="s">
-        <v>1631</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="332" spans="1:3" x14ac:dyDescent="0.5">
       <c r="C332" s="185" t="s">
-        <v>1661</v>
+        <v>1658</v>
       </c>
     </row>
     <row r="333" spans="1:3" x14ac:dyDescent="0.5">
       <c r="C333" s="151" t="s">
-        <v>1663</v>
+        <v>1660</v>
       </c>
     </row>
     <row r="334" spans="1:3" x14ac:dyDescent="0.5">
       <c r="C334" s="151" t="s">
-        <v>1664</v>
+        <v>1661</v>
       </c>
     </row>
     <row r="335" spans="1:3" x14ac:dyDescent="0.5">
       <c r="C335" s="151" t="s">
-        <v>1668</v>
+        <v>1665</v>
       </c>
     </row>
     <row r="336" spans="1:3" x14ac:dyDescent="0.5">
       <c r="C336" s="185" t="s">
-        <v>1671</v>
+        <v>1668</v>
       </c>
     </row>
     <row r="337" spans="1:3" ht="87" x14ac:dyDescent="0.5">
       <c r="C337" s="152" t="s">
-        <v>1674</v>
+        <v>1671</v>
       </c>
     </row>
     <row r="338" spans="1:3" ht="108.75" x14ac:dyDescent="0.5">
       <c r="C338" s="152" t="s">
-        <v>1675</v>
+        <v>1672</v>
       </c>
     </row>
     <row r="339" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A339" s="151" t="s">
-        <v>1676</v>
+        <v>1673</v>
       </c>
       <c r="B339" s="151" t="s">
-        <v>1677</v>
+        <v>1674</v>
       </c>
       <c r="C339" s="152"/>
     </row>
@@ -12682,21 +12718,21 @@
     </row>
     <row r="341" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A341" s="151" t="s">
-        <v>1678</v>
+        <v>1675</v>
       </c>
       <c r="B341" s="151" t="s">
-        <v>1682</v>
+        <v>1679</v>
       </c>
       <c r="C341" s="151" t="s">
-        <v>1680</v>
+        <v>1677</v>
       </c>
     </row>
     <row r="342" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B342" s="151" t="s">
-        <v>1683</v>
+        <v>1680</v>
       </c>
       <c r="C342" s="152" t="s">
-        <v>1681</v>
+        <v>1678</v>
       </c>
     </row>
     <row r="343" spans="1:3" x14ac:dyDescent="0.5">
@@ -12704,151 +12740,187 @@
     </row>
     <row r="344" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A344" s="151" t="s">
-        <v>1693</v>
+        <v>1690</v>
       </c>
       <c r="B344" s="151" t="s">
-        <v>1679</v>
+        <v>1676</v>
       </c>
       <c r="C344" s="151" t="s">
-        <v>1684</v>
+        <v>1681</v>
       </c>
     </row>
     <row r="345" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B345" s="151" t="s">
-        <v>1694</v>
+        <v>1691</v>
       </c>
       <c r="C345" s="152" t="s">
-        <v>1685</v>
+        <v>1682</v>
       </c>
     </row>
     <row r="346" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B346" s="151" t="s">
-        <v>1688</v>
+        <v>1685</v>
       </c>
       <c r="C346" s="152" t="s">
-        <v>1686</v>
+        <v>1683</v>
       </c>
     </row>
     <row r="347" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B347" s="151" t="s">
-        <v>1690</v>
+        <v>1687</v>
       </c>
       <c r="C347" s="151" t="s">
-        <v>1687</v>
+        <v>1684</v>
       </c>
     </row>
     <row r="348" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B348" s="151" t="s">
-        <v>1689</v>
+        <v>1686</v>
       </c>
       <c r="C348" s="151" t="s">
-        <v>1699</v>
+        <v>1696</v>
       </c>
     </row>
     <row r="349" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B349" s="151" t="s">
-        <v>1691</v>
+        <v>1688</v>
       </c>
       <c r="C349" s="151" t="s">
-        <v>1700</v>
+        <v>1697</v>
       </c>
     </row>
     <row r="350" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B350" s="151" t="s">
-        <v>1692</v>
-      </c>
-      <c r="C350" s="191" t="s">
+        <v>1689</v>
+      </c>
+      <c r="C350" s="190" t="s">
+        <v>1695</v>
+      </c>
+    </row>
+    <row r="351" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="B351" s="151" t="s">
+        <v>1710</v>
+      </c>
+      <c r="C351" s="185" t="s">
         <v>1698</v>
       </c>
     </row>
-    <row r="351" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="C351" s="185" t="s">
-        <v>1701</v>
-      </c>
-    </row>
     <row r="352" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="B352" s="151" t="s">
+        <v>1711</v>
+      </c>
       <c r="C352" s="152" t="s">
-        <v>1702</v>
+        <v>1699</v>
       </c>
     </row>
     <row r="353" spans="2:3" x14ac:dyDescent="0.5">
       <c r="C353" s="151" t="s">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="354" spans="2:3" x14ac:dyDescent="0.5">
+      <c r="C354" s="151" t="s">
+        <v>1701</v>
+      </c>
+    </row>
+    <row r="355" spans="2:3" x14ac:dyDescent="0.5">
+      <c r="C355" s="151" t="s">
+        <v>1702</v>
+      </c>
+    </row>
+    <row r="356" spans="2:3" x14ac:dyDescent="0.5">
+      <c r="C356" s="151" t="s">
         <v>1703</v>
       </c>
     </row>
     <row r="357" spans="2:3" x14ac:dyDescent="0.5">
-      <c r="B357" s="151" t="s">
-        <v>1525</v>
+      <c r="C357" s="151" t="s">
+        <v>1704</v>
       </c>
     </row>
     <row r="358" spans="2:3" x14ac:dyDescent="0.5">
-      <c r="B358" s="151" t="s">
-        <v>1451</v>
+      <c r="C358" s="151" t="s">
+        <v>1705</v>
       </c>
     </row>
     <row r="359" spans="2:3" x14ac:dyDescent="0.5">
-      <c r="B359" s="151" t="s">
+      <c r="C359" s="151" t="s">
+        <v>1706</v>
+      </c>
+    </row>
+    <row r="360" spans="2:3" x14ac:dyDescent="0.5">
+      <c r="C360" s="151" t="s">
+        <v>1707</v>
+      </c>
+    </row>
+    <row r="361" spans="2:3" x14ac:dyDescent="0.5">
+      <c r="C361" s="151" t="s">
+        <v>1708</v>
+      </c>
+    </row>
+    <row r="362" spans="2:3" x14ac:dyDescent="0.5">
+      <c r="C362" s="151" t="s">
+        <v>1709</v>
+      </c>
+    </row>
+    <row r="366" spans="2:3" x14ac:dyDescent="0.5">
+      <c r="B366" s="151" t="s">
+        <v>1622</v>
+      </c>
+    </row>
+    <row r="367" spans="2:3" x14ac:dyDescent="0.5">
+      <c r="B367" s="215" t="s">
+        <v>1524</v>
+      </c>
+    </row>
+    <row r="368" spans="2:3" x14ac:dyDescent="0.5">
+      <c r="B368" s="215" t="s">
+        <v>1623</v>
+      </c>
+    </row>
+    <row r="369" spans="2:2" ht="87" x14ac:dyDescent="0.5">
+      <c r="B369" s="152" t="s">
         <v>1624</v>
       </c>
     </row>
-    <row r="360" spans="2:3" x14ac:dyDescent="0.5">
-      <c r="B360" s="151" t="s">
-        <v>1526</v>
-      </c>
-    </row>
-    <row r="361" spans="2:3" x14ac:dyDescent="0.5">
-      <c r="B361" s="151" t="s">
-        <v>1625</v>
-      </c>
-    </row>
-    <row r="362" spans="2:3" ht="87" x14ac:dyDescent="0.5">
-      <c r="B362" s="152" t="s">
-        <v>1626</v>
-      </c>
-    </row>
-    <row r="364" spans="2:3" x14ac:dyDescent="0.5">
-      <c r="B364" s="187" t="s">
+    <row r="371" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B371" s="186" t="s">
+        <v>1642</v>
+      </c>
+    </row>
+    <row r="372" spans="2:2" ht="65.25" x14ac:dyDescent="0.5">
+      <c r="B372" s="187" t="s">
+        <v>1640</v>
+      </c>
+    </row>
+    <row r="373" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B373" s="188" t="s">
+        <v>1641</v>
+      </c>
+    </row>
+    <row r="374" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B374" s="189" t="s">
+        <v>1643</v>
+      </c>
+    </row>
+    <row r="375" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B375" s="215" t="s">
         <v>1644</v>
       </c>
     </row>
-    <row r="365" spans="2:3" ht="65.25" x14ac:dyDescent="0.5">
-      <c r="B365" s="188" t="s">
-        <v>1642</v>
-      </c>
-    </row>
-    <row r="366" spans="2:3" x14ac:dyDescent="0.5">
-      <c r="B366" s="189" t="s">
-        <v>1643</v>
-      </c>
-    </row>
-    <row r="367" spans="2:3" x14ac:dyDescent="0.5">
-      <c r="B367" s="190" t="s">
+    <row r="376" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B376" s="151" t="s">
         <v>1645</v>
       </c>
     </row>
-    <row r="368" spans="2:3" x14ac:dyDescent="0.5">
-      <c r="B368" s="186" t="s">
+    <row r="377" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B377" s="186" t="s">
         <v>1646</v>
       </c>
     </row>
-    <row r="369" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B369" s="151" t="s">
+    <row r="378" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B378" s="215" t="s">
         <v>1647</v>
-      </c>
-    </row>
-    <row r="370" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B370" s="151" t="s">
-        <v>1648</v>
-      </c>
-    </row>
-    <row r="371" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B371" s="187" t="s">
-        <v>1649</v>
-      </c>
-    </row>
-    <row r="372" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B372" s="151" t="s">
-        <v>1650</v>
       </c>
     </row>
   </sheetData>
@@ -12868,7 +12940,9 @@
   </sheetPr>
   <dimension ref="B2:B20"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -12983,7 +13057,9 @@
   </sheetPr>
   <dimension ref="B2:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -13022,7 +13098,9 @@
   </sheetPr>
   <dimension ref="B2:B26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -13167,7 +13245,7 @@
   <dimension ref="B2:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13238,7 +13316,7 @@
   <dimension ref="B2:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13278,9 +13356,7 @@
   </sheetPr>
   <dimension ref="B2:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -13477,9 +13553,7 @@
   </sheetPr>
   <dimension ref="B2:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -13569,9 +13643,7 @@
   </sheetPr>
   <dimension ref="A2:B49"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
-    </sheetView>
+    <sheetView topLeftCell="A37" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -13759,7 +13831,7 @@
       </c>
     </row>
     <row r="39" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="215" t="s">
+      <c r="A39" s="214" t="s">
         <v>927</v>
       </c>
       <c r="B39" s="19" t="s">
@@ -13767,19 +13839,19 @@
       </c>
     </row>
     <row r="40" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="215"/>
+      <c r="A40" s="214"/>
       <c r="B40" s="19" t="s">
         <v>613</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A41" s="215"/>
+      <c r="A41" s="214"/>
       <c r="B41" s="19" t="s">
         <v>614</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="A42" s="215" t="s">
+      <c r="A42" s="214" t="s">
         <v>927</v>
       </c>
       <c r="B42" s="19" t="s">
@@ -13787,13 +13859,13 @@
       </c>
     </row>
     <row r="43" spans="1:2" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="A43" s="215"/>
+      <c r="A43" s="214"/>
       <c r="B43" s="19" t="s">
         <v>616</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="A44" s="215"/>
+      <c r="A44" s="214"/>
       <c r="B44" s="19" t="s">
         <v>617</v>
       </c>
@@ -18216,7 +18288,7 @@
         <v>1121</v>
       </c>
       <c r="G77" s="120" t="s">
-        <v>1542</v>
+        <v>1540</v>
       </c>
       <c r="H77" s="121" t="b">
         <v>1</v>
@@ -18780,13 +18852,13 @@
         <v>817</v>
       </c>
       <c r="E87" s="120" t="s">
-        <v>1468</v>
+        <v>1467</v>
       </c>
       <c r="F87" s="120" t="s">
+        <v>1465</v>
+      </c>
+      <c r="G87" s="120" t="s">
         <v>1466</v>
-      </c>
-      <c r="G87" s="120" t="s">
-        <v>1467</v>
       </c>
       <c r="H87" s="121" t="b">
         <v>1</v>
@@ -18837,13 +18909,13 @@
         <v>902</v>
       </c>
       <c r="E88" s="120" t="s">
+        <v>1484</v>
+      </c>
+      <c r="F88" s="120" t="s">
+        <v>1486</v>
+      </c>
+      <c r="G88" s="120" t="s">
         <v>1485</v>
-      </c>
-      <c r="F88" s="120" t="s">
-        <v>1487</v>
-      </c>
-      <c r="G88" s="120" t="s">
-        <v>1486</v>
       </c>
       <c r="H88" s="121" t="b">
         <v>1</v>
@@ -18894,13 +18966,13 @@
         <v>131</v>
       </c>
       <c r="E89" s="120" t="s">
-        <v>1532</v>
+        <v>1530</v>
       </c>
       <c r="F89" s="120" t="s">
-        <v>1536</v>
+        <v>1534</v>
       </c>
       <c r="G89" s="120" t="s">
-        <v>1533</v>
+        <v>1531</v>
       </c>
       <c r="H89" s="121" t="b">
         <v>1</v>
@@ -18951,13 +19023,13 @@
         <v>779</v>
       </c>
       <c r="E90" s="120" t="s">
+        <v>1545</v>
+      </c>
+      <c r="F90" s="120" t="s">
+        <v>1546</v>
+      </c>
+      <c r="G90" s="120" t="s">
         <v>1547</v>
-      </c>
-      <c r="F90" s="120" t="s">
-        <v>1548</v>
-      </c>
-      <c r="G90" s="120" t="s">
-        <v>1549</v>
       </c>
       <c r="H90" s="121" t="b">
         <v>1</v>
@@ -19008,13 +19080,13 @@
         <v>779</v>
       </c>
       <c r="E91" s="120" t="s">
+        <v>1549</v>
+      </c>
+      <c r="F91" s="120" t="s">
+        <v>1550</v>
+      </c>
+      <c r="G91" s="120" t="s">
         <v>1551</v>
-      </c>
-      <c r="F91" s="120" t="s">
-        <v>1552</v>
-      </c>
-      <c r="G91" s="120" t="s">
-        <v>1553</v>
       </c>
       <c r="H91" s="121" t="b">
         <v>1</v>
@@ -19065,13 +19137,13 @@
         <v>779</v>
       </c>
       <c r="E92" s="120" t="s">
+        <v>1553</v>
+      </c>
+      <c r="F92" s="120" t="s">
         <v>1555</v>
       </c>
-      <c r="F92" s="120" t="s">
-        <v>1557</v>
-      </c>
       <c r="G92" s="120" t="s">
-        <v>1556</v>
+        <v>1554</v>
       </c>
       <c r="H92" s="121" t="b">
         <v>1</v>
@@ -19122,13 +19194,13 @@
         <v>779</v>
       </c>
       <c r="E93" s="120" t="s">
+        <v>1564</v>
+      </c>
+      <c r="F93" s="120" t="s">
+        <v>1565</v>
+      </c>
+      <c r="G93" s="120" t="s">
         <v>1566</v>
-      </c>
-      <c r="F93" s="120" t="s">
-        <v>1567</v>
-      </c>
-      <c r="G93" s="120" t="s">
-        <v>1568</v>
       </c>
       <c r="H93" s="121" t="b">
         <v>1</v>
@@ -19179,13 +19251,13 @@
         <v>817</v>
       </c>
       <c r="E94" s="120" t="s">
-        <v>1585</v>
+        <v>1583</v>
       </c>
       <c r="F94" s="120" t="s">
-        <v>1612</v>
+        <v>1610</v>
       </c>
       <c r="G94" s="120" t="s">
-        <v>1586</v>
+        <v>1584</v>
       </c>
       <c r="H94" s="121" t="b">
         <v>1</v>
@@ -19236,13 +19308,13 @@
         <v>837</v>
       </c>
       <c r="E95" s="120" t="s">
+        <v>1590</v>
+      </c>
+      <c r="F95" s="120" t="s">
         <v>1592</v>
       </c>
-      <c r="F95" s="120" t="s">
-        <v>1594</v>
-      </c>
       <c r="G95" s="120" t="s">
-        <v>1593</v>
+        <v>1591</v>
       </c>
       <c r="H95" s="121" t="b">
         <v>1</v>
@@ -19293,13 +19365,13 @@
         <v>779</v>
       </c>
       <c r="E96" s="120" t="s">
-        <v>1600</v>
+        <v>1598</v>
       </c>
       <c r="F96" s="120" t="s">
-        <v>1597</v>
+        <v>1595</v>
       </c>
       <c r="G96" s="120" t="s">
-        <v>1601</v>
+        <v>1599</v>
       </c>
       <c r="H96" s="121" t="b">
         <v>1</v>
@@ -19350,13 +19422,13 @@
         <v>779</v>
       </c>
       <c r="E97" s="120" t="s">
-        <v>1604</v>
+        <v>1602</v>
       </c>
       <c r="F97" s="120" t="s">
-        <v>1602</v>
+        <v>1600</v>
       </c>
       <c r="G97" s="120" t="s">
-        <v>1603</v>
+        <v>1601</v>
       </c>
       <c r="H97" s="121" t="b">
         <v>1</v>
@@ -19407,13 +19479,13 @@
         <v>817</v>
       </c>
       <c r="E98" s="120" t="s">
-        <v>1666</v>
+        <v>1663</v>
       </c>
       <c r="F98" s="120" t="s">
-        <v>1665</v>
+        <v>1662</v>
       </c>
       <c r="G98" s="120" t="s">
-        <v>1667</v>
+        <v>1664</v>
       </c>
       <c r="H98" s="121" t="b">
         <v>1</v>
@@ -19464,49 +19536,49 @@
         <v>837</v>
       </c>
       <c r="E99" s="120" t="s">
-        <v>1696</v>
+        <v>1693</v>
       </c>
       <c r="F99" s="120" t="s">
+        <v>1692</v>
+      </c>
+      <c r="G99" s="120" t="s">
+        <v>1694</v>
+      </c>
+      <c r="H99" s="121" t="b">
+        <v>1</v>
+      </c>
+      <c r="I99" s="121" t="b">
+        <v>1</v>
+      </c>
+      <c r="J99" s="121" t="b">
+        <v>1</v>
+      </c>
+      <c r="K99" s="121" t="b">
+        <v>1</v>
+      </c>
+      <c r="L99" s="121" t="b">
+        <v>1</v>
+      </c>
+      <c r="M99" s="121" t="b">
+        <v>0</v>
+      </c>
+      <c r="N99" s="121" t="b">
+        <v>0</v>
+      </c>
+      <c r="O99" s="121" t="b">
+        <v>0</v>
+      </c>
+      <c r="P99" s="121" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q99" s="121" t="b">
+        <v>0</v>
+      </c>
+      <c r="R99" s="121" t="b">
+        <v>0</v>
+      </c>
+      <c r="S99" s="190" t="s">
         <v>1695</v>
-      </c>
-      <c r="G99" s="120" t="s">
-        <v>1697</v>
-      </c>
-      <c r="H99" s="121" t="b">
-        <v>1</v>
-      </c>
-      <c r="I99" s="121" t="b">
-        <v>1</v>
-      </c>
-      <c r="J99" s="121" t="b">
-        <v>1</v>
-      </c>
-      <c r="K99" s="121" t="b">
-        <v>1</v>
-      </c>
-      <c r="L99" s="121" t="b">
-        <v>1</v>
-      </c>
-      <c r="M99" s="121" t="b">
-        <v>0</v>
-      </c>
-      <c r="N99" s="121" t="b">
-        <v>0</v>
-      </c>
-      <c r="O99" s="121" t="b">
-        <v>0</v>
-      </c>
-      <c r="P99" s="121" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q99" s="121" t="b">
-        <v>0</v>
-      </c>
-      <c r="R99" s="121" t="b">
-        <v>0</v>
-      </c>
-      <c r="S99" s="191" t="s">
-        <v>1698</v>
       </c>
     </row>
   </sheetData>
@@ -19786,9 +19858,7 @@
   </sheetPr>
   <dimension ref="B2:B37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P30" sqref="P30"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -19979,9 +20049,7 @@
   </sheetPr>
   <dimension ref="B2:B20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -20281,8 +20349,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:N24"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E16" activeCellId="3" sqref="E9 E12 E15 E16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21016,7 +21084,7 @@
         <v>40000</v>
       </c>
       <c r="F16" s="175" t="s">
-        <v>1484</v>
+        <v>1483</v>
       </c>
       <c r="G16" s="48"/>
       <c r="H16" s="49" t="s">
@@ -21462,97 +21530,97 @@
     </row>
     <row r="2" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
-      <c r="B2" s="201" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="201" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="201" t="s">
+      <c r="B2" s="196" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="196" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="196" t="s">
         <v>130</v>
       </c>
-      <c r="E2" s="203" t="s">
+      <c r="E2" s="198" t="s">
         <v>723</v>
       </c>
-      <c r="F2" s="197" t="s">
+      <c r="F2" s="193" t="s">
         <v>651</v>
       </c>
-      <c r="G2" s="198"/>
-      <c r="H2" s="198"/>
-      <c r="I2" s="199"/>
-      <c r="J2" s="197" t="s">
+      <c r="G2" s="194"/>
+      <c r="H2" s="194"/>
+      <c r="I2" s="195"/>
+      <c r="J2" s="193" t="s">
         <v>652</v>
       </c>
-      <c r="K2" s="198"/>
-      <c r="L2" s="198"/>
-      <c r="M2" s="199"/>
-      <c r="N2" s="197" t="s">
+      <c r="K2" s="194"/>
+      <c r="L2" s="194"/>
+      <c r="M2" s="195"/>
+      <c r="N2" s="193" t="s">
         <v>653</v>
       </c>
-      <c r="O2" s="198"/>
-      <c r="P2" s="198"/>
-      <c r="Q2" s="199"/>
-      <c r="R2" s="197" t="s">
+      <c r="O2" s="194"/>
+      <c r="P2" s="194"/>
+      <c r="Q2" s="195"/>
+      <c r="R2" s="193" t="s">
         <v>654</v>
       </c>
-      <c r="S2" s="198"/>
-      <c r="T2" s="198"/>
-      <c r="U2" s="200"/>
-      <c r="V2" s="197" t="s">
+      <c r="S2" s="194"/>
+      <c r="T2" s="194"/>
+      <c r="U2" s="203"/>
+      <c r="V2" s="193" t="s">
         <v>655</v>
       </c>
-      <c r="W2" s="198"/>
-      <c r="X2" s="198"/>
-      <c r="Y2" s="200"/>
-      <c r="Z2" s="194" t="s">
+      <c r="W2" s="194"/>
+      <c r="X2" s="194"/>
+      <c r="Y2" s="203"/>
+      <c r="Z2" s="200" t="s">
         <v>656</v>
       </c>
-      <c r="AA2" s="195"/>
-      <c r="AB2" s="195"/>
-      <c r="AC2" s="196"/>
-      <c r="AD2" s="194" t="s">
+      <c r="AA2" s="201"/>
+      <c r="AB2" s="201"/>
+      <c r="AC2" s="202"/>
+      <c r="AD2" s="200" t="s">
         <v>657</v>
       </c>
-      <c r="AE2" s="195"/>
-      <c r="AF2" s="195"/>
-      <c r="AG2" s="196"/>
-      <c r="AH2" s="194" t="s">
+      <c r="AE2" s="201"/>
+      <c r="AF2" s="201"/>
+      <c r="AG2" s="202"/>
+      <c r="AH2" s="200" t="s">
         <v>658</v>
       </c>
-      <c r="AI2" s="195"/>
-      <c r="AJ2" s="195"/>
-      <c r="AK2" s="196"/>
-      <c r="AL2" s="194" t="s">
+      <c r="AI2" s="201"/>
+      <c r="AJ2" s="201"/>
+      <c r="AK2" s="202"/>
+      <c r="AL2" s="200" t="s">
         <v>659</v>
       </c>
-      <c r="AM2" s="195"/>
-      <c r="AN2" s="195"/>
-      <c r="AO2" s="196"/>
-      <c r="AP2" s="194" t="s">
+      <c r="AM2" s="201"/>
+      <c r="AN2" s="201"/>
+      <c r="AO2" s="202"/>
+      <c r="AP2" s="200" t="s">
         <v>660</v>
       </c>
-      <c r="AQ2" s="195"/>
-      <c r="AR2" s="195"/>
-      <c r="AS2" s="196"/>
-      <c r="AT2" s="194" t="s">
+      <c r="AQ2" s="201"/>
+      <c r="AR2" s="201"/>
+      <c r="AS2" s="202"/>
+      <c r="AT2" s="200" t="s">
         <v>722</v>
       </c>
-      <c r="AU2" s="195"/>
-      <c r="AV2" s="195"/>
-      <c r="AW2" s="196"/>
-      <c r="AX2" s="194" t="s">
+      <c r="AU2" s="201"/>
+      <c r="AV2" s="201"/>
+      <c r="AW2" s="202"/>
+      <c r="AX2" s="200" t="s">
         <v>729</v>
       </c>
-      <c r="AY2" s="195"/>
-      <c r="AZ2" s="195"/>
-      <c r="BA2" s="196"/>
+      <c r="AY2" s="201"/>
+      <c r="AZ2" s="201"/>
+      <c r="BA2" s="202"/>
     </row>
     <row r="3" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
-      <c r="B3" s="202"/>
-      <c r="C3" s="202"/>
-      <c r="D3" s="202"/>
-      <c r="E3" s="204"/>
+      <c r="B3" s="197"/>
+      <c r="C3" s="197"/>
+      <c r="D3" s="197"/>
+      <c r="E3" s="199"/>
       <c r="F3" s="80">
         <v>1</v>
       </c>
@@ -26706,12 +26774,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:I2"/>
     <mergeCell ref="AL2:AO2"/>
     <mergeCell ref="AP2:AS2"/>
     <mergeCell ref="AT2:AW2"/>
@@ -26722,6 +26784,12 @@
     <mergeCell ref="Z2:AC2"/>
     <mergeCell ref="AD2:AG2"/>
     <mergeCell ref="AH2:AK2"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:I2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D84" location="ลูกค้า!A1" display="ลูกค้า!A1"/>
@@ -27239,86 +27307,86 @@
     <row r="2" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
-      <c r="C2" s="201" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="201" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="201" t="s">
+      <c r="C2" s="196" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="196" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="196" t="s">
         <v>130</v>
       </c>
-      <c r="F2" s="203" t="s">
+      <c r="F2" s="198" t="s">
         <v>723</v>
       </c>
-      <c r="G2" s="205" t="s">
+      <c r="G2" s="204" t="s">
         <v>660</v>
       </c>
-      <c r="H2" s="206"/>
-      <c r="I2" s="206"/>
-      <c r="J2" s="208"/>
-      <c r="K2" s="205" t="s">
+      <c r="H2" s="205"/>
+      <c r="I2" s="205"/>
+      <c r="J2" s="207"/>
+      <c r="K2" s="204" t="s">
         <v>722</v>
       </c>
-      <c r="L2" s="206"/>
-      <c r="M2" s="206"/>
-      <c r="N2" s="207"/>
-      <c r="O2" s="205" t="s">
+      <c r="L2" s="205"/>
+      <c r="M2" s="205"/>
+      <c r="N2" s="206"/>
+      <c r="O2" s="204" t="s">
         <v>729</v>
       </c>
-      <c r="P2" s="206"/>
-      <c r="Q2" s="206"/>
-      <c r="R2" s="207"/>
-      <c r="S2" s="205" t="s">
+      <c r="P2" s="205"/>
+      <c r="Q2" s="205"/>
+      <c r="R2" s="206"/>
+      <c r="S2" s="204" t="s">
         <v>651</v>
       </c>
-      <c r="T2" s="206"/>
-      <c r="U2" s="206"/>
-      <c r="V2" s="207"/>
-      <c r="W2" s="205" t="s">
+      <c r="T2" s="205"/>
+      <c r="U2" s="205"/>
+      <c r="V2" s="206"/>
+      <c r="W2" s="204" t="s">
         <v>730</v>
       </c>
-      <c r="X2" s="206"/>
-      <c r="Y2" s="206"/>
-      <c r="Z2" s="207"/>
-      <c r="AA2" s="205" t="s">
+      <c r="X2" s="205"/>
+      <c r="Y2" s="205"/>
+      <c r="Z2" s="206"/>
+      <c r="AA2" s="204" t="s">
         <v>653</v>
       </c>
-      <c r="AB2" s="206"/>
-      <c r="AC2" s="206"/>
-      <c r="AD2" s="207"/>
-      <c r="AE2" s="205" t="s">
+      <c r="AB2" s="205"/>
+      <c r="AC2" s="205"/>
+      <c r="AD2" s="206"/>
+      <c r="AE2" s="204" t="s">
         <v>731</v>
       </c>
-      <c r="AF2" s="206"/>
-      <c r="AG2" s="206"/>
-      <c r="AH2" s="207"/>
-      <c r="AI2" s="205" t="s">
+      <c r="AF2" s="205"/>
+      <c r="AG2" s="205"/>
+      <c r="AH2" s="206"/>
+      <c r="AI2" s="204" t="s">
         <v>655</v>
       </c>
-      <c r="AJ2" s="206"/>
-      <c r="AK2" s="206"/>
-      <c r="AL2" s="207"/>
-      <c r="AM2" s="205" t="s">
+      <c r="AJ2" s="205"/>
+      <c r="AK2" s="205"/>
+      <c r="AL2" s="206"/>
+      <c r="AM2" s="204" t="s">
         <v>656</v>
       </c>
-      <c r="AN2" s="206"/>
-      <c r="AO2" s="206"/>
-      <c r="AP2" s="207"/>
-      <c r="AQ2" s="205" t="s">
+      <c r="AN2" s="205"/>
+      <c r="AO2" s="205"/>
+      <c r="AP2" s="206"/>
+      <c r="AQ2" s="204" t="s">
         <v>657</v>
       </c>
-      <c r="AR2" s="206"/>
-      <c r="AS2" s="206"/>
-      <c r="AT2" s="207"/>
+      <c r="AR2" s="205"/>
+      <c r="AS2" s="205"/>
+      <c r="AT2" s="206"/>
     </row>
     <row r="3" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
-      <c r="C3" s="202"/>
-      <c r="D3" s="202"/>
-      <c r="E3" s="202"/>
-      <c r="F3" s="204"/>
+      <c r="C3" s="197"/>
+      <c r="D3" s="197"/>
+      <c r="E3" s="197"/>
+      <c r="F3" s="199"/>
       <c r="G3" s="80">
         <v>1</v>
       </c>
@@ -33114,11 +33182,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="AE2:AH2"/>
-    <mergeCell ref="AI2:AL2"/>
-    <mergeCell ref="AM2:AP2"/>
-    <mergeCell ref="AQ2:AT2"/>
-    <mergeCell ref="AA2:AD2"/>
     <mergeCell ref="K2:N2"/>
     <mergeCell ref="O2:R2"/>
     <mergeCell ref="S2:V2"/>
@@ -33128,6 +33191,11 @@
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="G2:J2"/>
+    <mergeCell ref="AE2:AH2"/>
+    <mergeCell ref="AI2:AL2"/>
+    <mergeCell ref="AM2:AP2"/>
+    <mergeCell ref="AQ2:AT2"/>
+    <mergeCell ref="AA2:AD2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E84" location="ลูกค้า!A1" display="ลูกค้า!A1"/>
@@ -33605,98 +33673,98 @@
     <row r="2" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
-      <c r="C2" s="201" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="201" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="201" t="s">
+      <c r="C2" s="196" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="196" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="196" t="s">
         <v>130</v>
       </c>
-      <c r="F2" s="203" t="s">
+      <c r="F2" s="198" t="s">
         <v>723</v>
       </c>
-      <c r="G2" s="197" t="s">
+      <c r="G2" s="193" t="s">
         <v>651</v>
       </c>
-      <c r="H2" s="198"/>
-      <c r="I2" s="198"/>
-      <c r="J2" s="199"/>
-      <c r="K2" s="197" t="s">
+      <c r="H2" s="194"/>
+      <c r="I2" s="194"/>
+      <c r="J2" s="195"/>
+      <c r="K2" s="193" t="s">
         <v>652</v>
       </c>
-      <c r="L2" s="198"/>
-      <c r="M2" s="198"/>
-      <c r="N2" s="199"/>
-      <c r="O2" s="197" t="s">
+      <c r="L2" s="194"/>
+      <c r="M2" s="194"/>
+      <c r="N2" s="195"/>
+      <c r="O2" s="193" t="s">
         <v>653</v>
       </c>
-      <c r="P2" s="198"/>
-      <c r="Q2" s="198"/>
-      <c r="R2" s="199"/>
-      <c r="S2" s="197" t="s">
+      <c r="P2" s="194"/>
+      <c r="Q2" s="194"/>
+      <c r="R2" s="195"/>
+      <c r="S2" s="193" t="s">
         <v>654</v>
       </c>
-      <c r="T2" s="198"/>
-      <c r="U2" s="198"/>
-      <c r="V2" s="200"/>
-      <c r="W2" s="197" t="s">
+      <c r="T2" s="194"/>
+      <c r="U2" s="194"/>
+      <c r="V2" s="203"/>
+      <c r="W2" s="193" t="s">
         <v>655</v>
       </c>
-      <c r="X2" s="198"/>
-      <c r="Y2" s="198"/>
-      <c r="Z2" s="200"/>
-      <c r="AA2" s="194" t="s">
+      <c r="X2" s="194"/>
+      <c r="Y2" s="194"/>
+      <c r="Z2" s="203"/>
+      <c r="AA2" s="200" t="s">
         <v>656</v>
       </c>
-      <c r="AB2" s="195"/>
-      <c r="AC2" s="195"/>
-      <c r="AD2" s="196"/>
-      <c r="AE2" s="194" t="s">
+      <c r="AB2" s="201"/>
+      <c r="AC2" s="201"/>
+      <c r="AD2" s="202"/>
+      <c r="AE2" s="200" t="s">
         <v>657</v>
       </c>
-      <c r="AF2" s="195"/>
-      <c r="AG2" s="195"/>
-      <c r="AH2" s="196"/>
-      <c r="AI2" s="194" t="s">
+      <c r="AF2" s="201"/>
+      <c r="AG2" s="201"/>
+      <c r="AH2" s="202"/>
+      <c r="AI2" s="200" t="s">
         <v>658</v>
       </c>
-      <c r="AJ2" s="195"/>
-      <c r="AK2" s="195"/>
-      <c r="AL2" s="196"/>
-      <c r="AM2" s="194" t="s">
+      <c r="AJ2" s="201"/>
+      <c r="AK2" s="201"/>
+      <c r="AL2" s="202"/>
+      <c r="AM2" s="200" t="s">
         <v>659</v>
       </c>
-      <c r="AN2" s="195"/>
-      <c r="AO2" s="195"/>
-      <c r="AP2" s="196"/>
-      <c r="AQ2" s="194" t="s">
+      <c r="AN2" s="201"/>
+      <c r="AO2" s="201"/>
+      <c r="AP2" s="202"/>
+      <c r="AQ2" s="200" t="s">
         <v>660</v>
       </c>
-      <c r="AR2" s="195"/>
-      <c r="AS2" s="195"/>
-      <c r="AT2" s="196"/>
-      <c r="AU2" s="194" t="s">
+      <c r="AR2" s="201"/>
+      <c r="AS2" s="201"/>
+      <c r="AT2" s="202"/>
+      <c r="AU2" s="200" t="s">
         <v>722</v>
       </c>
-      <c r="AV2" s="195"/>
-      <c r="AW2" s="195"/>
-      <c r="AX2" s="196"/>
-      <c r="AY2" s="194" t="s">
+      <c r="AV2" s="201"/>
+      <c r="AW2" s="201"/>
+      <c r="AX2" s="202"/>
+      <c r="AY2" s="200" t="s">
         <v>729</v>
       </c>
-      <c r="AZ2" s="195"/>
-      <c r="BA2" s="195"/>
-      <c r="BB2" s="196"/>
+      <c r="AZ2" s="201"/>
+      <c r="BA2" s="201"/>
+      <c r="BB2" s="202"/>
     </row>
     <row r="3" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
-      <c r="C3" s="202"/>
-      <c r="D3" s="202"/>
-      <c r="E3" s="202"/>
-      <c r="F3" s="204"/>
+      <c r="C3" s="197"/>
+      <c r="D3" s="197"/>
+      <c r="E3" s="197"/>
+      <c r="F3" s="199"/>
       <c r="G3" s="80">
         <v>1</v>
       </c>
@@ -39109,6 +39177,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="O2:R2"/>
     <mergeCell ref="AU2:AX2"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="AY2:BB2"/>
@@ -39120,11 +39193,6 @@
     <mergeCell ref="AM2:AP2"/>
     <mergeCell ref="AQ2:AT2"/>
     <mergeCell ref="S2:V2"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="O2:R2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E84" location="ลูกค้า!A1" display="ลูกค้า!A1"/>
@@ -39312,38 +39380,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="211" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="201" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="213" t="s">
+      <c r="A1" s="210" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="196" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="212" t="s">
         <v>651</v>
       </c>
-      <c r="D1" s="213"/>
-      <c r="E1" s="213"/>
-      <c r="F1" s="210"/>
-      <c r="G1" s="213" t="s">
+      <c r="D1" s="212"/>
+      <c r="E1" s="212"/>
+      <c r="F1" s="209"/>
+      <c r="G1" s="212" t="s">
         <v>730</v>
       </c>
-      <c r="H1" s="213"/>
-      <c r="I1" s="213"/>
-      <c r="J1" s="210"/>
-      <c r="K1" s="213" t="s">
+      <c r="H1" s="212"/>
+      <c r="I1" s="212"/>
+      <c r="J1" s="209"/>
+      <c r="K1" s="212" t="s">
         <v>653</v>
       </c>
-      <c r="L1" s="213"/>
-      <c r="M1" s="213"/>
-      <c r="N1" s="210"/>
-      <c r="O1" s="209" t="s">
+      <c r="L1" s="212"/>
+      <c r="M1" s="212"/>
+      <c r="N1" s="209"/>
+      <c r="O1" s="208" t="s">
         <v>731</v>
       </c>
-      <c r="P1" s="210"/>
+      <c r="P1" s="209"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="212"/>
-      <c r="B2" s="202"/>
+      <c r="A2" s="211"/>
+      <c r="B2" s="197"/>
       <c r="C2" s="1">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
bill total panel @Office
</commit_message>
<xml_diff>
--- a/_Doc/Feature.xlsx
+++ b/_Doc/Feature.xlsx
@@ -56,7 +56,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Menu!$A$1:$R$57</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -226,7 +226,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2540" uniqueCount="1811">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2541" uniqueCount="1811">
   <si>
     <t>No.</t>
   </si>
@@ -6096,7 +6096,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="48" x14ac:knownFonts="1">
     <font>
@@ -6721,7 +6721,7 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
@@ -6805,20 +6805,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="1" fillId="6" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
@@ -6986,11 +6986,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="43" fontId="29" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="43" fontId="14" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -7080,15 +7080,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -7096,9 +7087,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -7112,6 +7100,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -8019,20 +8019,20 @@
       <c r="B1" s="2"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="203" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="203" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="203" t="s">
+      <c r="A2" s="199" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="199" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="199" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="204"/>
-      <c r="B3" s="204"/>
-      <c r="C3" s="204"/>
+      <c r="A3" s="200"/>
+      <c r="B3" s="200"/>
+      <c r="C3" s="200"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
@@ -9234,6 +9234,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
     <mergeCell ref="B43:C43"/>
     <mergeCell ref="B44:C44"/>
     <mergeCell ref="B45:C45"/>
@@ -9244,12 +9250,6 @@
     <mergeCell ref="B40:C40"/>
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -11176,8 +11176,8 @@
   </sheetPr>
   <dimension ref="A1:C469"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A419" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C425" sqref="C425"/>
+    <sheetView tabSelected="1" topLeftCell="A422" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B429" sqref="B429"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21.75" x14ac:dyDescent="0.5"/>
@@ -13658,6 +13658,9 @@
       <c r="C427" s="185"/>
     </row>
     <row r="428" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="B428" s="151" t="s">
+        <v>1806</v>
+      </c>
       <c r="C428" s="185"/>
     </row>
     <row r="429" spans="1:3" x14ac:dyDescent="0.5">
@@ -22556,97 +22559,97 @@
     </row>
     <row r="2" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
-      <c r="B2" s="203" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="203" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="203" t="s">
+      <c r="B2" s="199" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="199" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="199" t="s">
         <v>130</v>
       </c>
-      <c r="E2" s="205" t="s">
+      <c r="E2" s="201" t="s">
         <v>723</v>
       </c>
-      <c r="F2" s="199" t="s">
+      <c r="F2" s="196" t="s">
         <v>651</v>
       </c>
-      <c r="G2" s="200"/>
-      <c r="H2" s="200"/>
-      <c r="I2" s="201"/>
-      <c r="J2" s="199" t="s">
+      <c r="G2" s="197"/>
+      <c r="H2" s="197"/>
+      <c r="I2" s="198"/>
+      <c r="J2" s="196" t="s">
         <v>652</v>
       </c>
-      <c r="K2" s="200"/>
-      <c r="L2" s="200"/>
-      <c r="M2" s="201"/>
-      <c r="N2" s="199" t="s">
+      <c r="K2" s="197"/>
+      <c r="L2" s="197"/>
+      <c r="M2" s="198"/>
+      <c r="N2" s="196" t="s">
         <v>653</v>
       </c>
-      <c r="O2" s="200"/>
-      <c r="P2" s="200"/>
-      <c r="Q2" s="201"/>
-      <c r="R2" s="199" t="s">
+      <c r="O2" s="197"/>
+      <c r="P2" s="197"/>
+      <c r="Q2" s="198"/>
+      <c r="R2" s="196" t="s">
         <v>654</v>
       </c>
-      <c r="S2" s="200"/>
-      <c r="T2" s="200"/>
-      <c r="U2" s="202"/>
-      <c r="V2" s="199" t="s">
+      <c r="S2" s="197"/>
+      <c r="T2" s="197"/>
+      <c r="U2" s="206"/>
+      <c r="V2" s="196" t="s">
         <v>655</v>
       </c>
-      <c r="W2" s="200"/>
-      <c r="X2" s="200"/>
-      <c r="Y2" s="202"/>
-      <c r="Z2" s="196" t="s">
+      <c r="W2" s="197"/>
+      <c r="X2" s="197"/>
+      <c r="Y2" s="206"/>
+      <c r="Z2" s="203" t="s">
         <v>656</v>
       </c>
-      <c r="AA2" s="197"/>
-      <c r="AB2" s="197"/>
-      <c r="AC2" s="198"/>
-      <c r="AD2" s="196" t="s">
+      <c r="AA2" s="204"/>
+      <c r="AB2" s="204"/>
+      <c r="AC2" s="205"/>
+      <c r="AD2" s="203" t="s">
         <v>657</v>
       </c>
-      <c r="AE2" s="197"/>
-      <c r="AF2" s="197"/>
-      <c r="AG2" s="198"/>
-      <c r="AH2" s="196" t="s">
+      <c r="AE2" s="204"/>
+      <c r="AF2" s="204"/>
+      <c r="AG2" s="205"/>
+      <c r="AH2" s="203" t="s">
         <v>658</v>
       </c>
-      <c r="AI2" s="197"/>
-      <c r="AJ2" s="197"/>
-      <c r="AK2" s="198"/>
-      <c r="AL2" s="196" t="s">
+      <c r="AI2" s="204"/>
+      <c r="AJ2" s="204"/>
+      <c r="AK2" s="205"/>
+      <c r="AL2" s="203" t="s">
         <v>659</v>
       </c>
-      <c r="AM2" s="197"/>
-      <c r="AN2" s="197"/>
-      <c r="AO2" s="198"/>
-      <c r="AP2" s="196" t="s">
+      <c r="AM2" s="204"/>
+      <c r="AN2" s="204"/>
+      <c r="AO2" s="205"/>
+      <c r="AP2" s="203" t="s">
         <v>660</v>
       </c>
-      <c r="AQ2" s="197"/>
-      <c r="AR2" s="197"/>
-      <c r="AS2" s="198"/>
-      <c r="AT2" s="196" t="s">
+      <c r="AQ2" s="204"/>
+      <c r="AR2" s="204"/>
+      <c r="AS2" s="205"/>
+      <c r="AT2" s="203" t="s">
         <v>722</v>
       </c>
-      <c r="AU2" s="197"/>
-      <c r="AV2" s="197"/>
-      <c r="AW2" s="198"/>
-      <c r="AX2" s="196" t="s">
+      <c r="AU2" s="204"/>
+      <c r="AV2" s="204"/>
+      <c r="AW2" s="205"/>
+      <c r="AX2" s="203" t="s">
         <v>729</v>
       </c>
-      <c r="AY2" s="197"/>
-      <c r="AZ2" s="197"/>
-      <c r="BA2" s="198"/>
+      <c r="AY2" s="204"/>
+      <c r="AZ2" s="204"/>
+      <c r="BA2" s="205"/>
     </row>
     <row r="3" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
-      <c r="B3" s="204"/>
-      <c r="C3" s="204"/>
-      <c r="D3" s="204"/>
-      <c r="E3" s="206"/>
+      <c r="B3" s="200"/>
+      <c r="C3" s="200"/>
+      <c r="D3" s="200"/>
+      <c r="E3" s="202"/>
       <c r="F3" s="80">
         <v>1</v>
       </c>
@@ -27800,12 +27803,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:I2"/>
     <mergeCell ref="AL2:AO2"/>
     <mergeCell ref="AP2:AS2"/>
     <mergeCell ref="AT2:AW2"/>
@@ -27816,6 +27813,12 @@
     <mergeCell ref="Z2:AC2"/>
     <mergeCell ref="AD2:AG2"/>
     <mergeCell ref="AH2:AK2"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:I2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D84" location="ลูกค้า!A1" display="ลูกค้า!A1"/>
@@ -28333,16 +28336,16 @@
     <row r="2" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
-      <c r="C2" s="203" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="203" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="203" t="s">
+      <c r="C2" s="199" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="199" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="199" t="s">
         <v>130</v>
       </c>
-      <c r="F2" s="205" t="s">
+      <c r="F2" s="201" t="s">
         <v>723</v>
       </c>
       <c r="G2" s="207" t="s">
@@ -28409,10 +28412,10 @@
     <row r="3" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
-      <c r="C3" s="204"/>
-      <c r="D3" s="204"/>
-      <c r="E3" s="204"/>
-      <c r="F3" s="206"/>
+      <c r="C3" s="200"/>
+      <c r="D3" s="200"/>
+      <c r="E3" s="200"/>
+      <c r="F3" s="202"/>
       <c r="G3" s="80">
         <v>1</v>
       </c>
@@ -34208,11 +34211,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="AE2:AH2"/>
-    <mergeCell ref="AI2:AL2"/>
-    <mergeCell ref="AM2:AP2"/>
-    <mergeCell ref="AQ2:AT2"/>
-    <mergeCell ref="AA2:AD2"/>
     <mergeCell ref="K2:N2"/>
     <mergeCell ref="O2:R2"/>
     <mergeCell ref="S2:V2"/>
@@ -34222,6 +34220,11 @@
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="G2:J2"/>
+    <mergeCell ref="AE2:AH2"/>
+    <mergeCell ref="AI2:AL2"/>
+    <mergeCell ref="AM2:AP2"/>
+    <mergeCell ref="AQ2:AT2"/>
+    <mergeCell ref="AA2:AD2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E84" location="ลูกค้า!A1" display="ลูกค้า!A1"/>
@@ -34699,98 +34702,98 @@
     <row r="2" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
-      <c r="C2" s="203" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="203" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="203" t="s">
+      <c r="C2" s="199" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="199" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="199" t="s">
         <v>130</v>
       </c>
-      <c r="F2" s="205" t="s">
+      <c r="F2" s="201" t="s">
         <v>723</v>
       </c>
-      <c r="G2" s="199" t="s">
+      <c r="G2" s="196" t="s">
         <v>651</v>
       </c>
-      <c r="H2" s="200"/>
-      <c r="I2" s="200"/>
-      <c r="J2" s="201"/>
-      <c r="K2" s="199" t="s">
+      <c r="H2" s="197"/>
+      <c r="I2" s="197"/>
+      <c r="J2" s="198"/>
+      <c r="K2" s="196" t="s">
         <v>652</v>
       </c>
-      <c r="L2" s="200"/>
-      <c r="M2" s="200"/>
-      <c r="N2" s="201"/>
-      <c r="O2" s="199" t="s">
+      <c r="L2" s="197"/>
+      <c r="M2" s="197"/>
+      <c r="N2" s="198"/>
+      <c r="O2" s="196" t="s">
         <v>653</v>
       </c>
-      <c r="P2" s="200"/>
-      <c r="Q2" s="200"/>
-      <c r="R2" s="201"/>
-      <c r="S2" s="199" t="s">
+      <c r="P2" s="197"/>
+      <c r="Q2" s="197"/>
+      <c r="R2" s="198"/>
+      <c r="S2" s="196" t="s">
         <v>654</v>
       </c>
-      <c r="T2" s="200"/>
-      <c r="U2" s="200"/>
-      <c r="V2" s="202"/>
-      <c r="W2" s="199" t="s">
+      <c r="T2" s="197"/>
+      <c r="U2" s="197"/>
+      <c r="V2" s="206"/>
+      <c r="W2" s="196" t="s">
         <v>655</v>
       </c>
-      <c r="X2" s="200"/>
-      <c r="Y2" s="200"/>
-      <c r="Z2" s="202"/>
-      <c r="AA2" s="196" t="s">
+      <c r="X2" s="197"/>
+      <c r="Y2" s="197"/>
+      <c r="Z2" s="206"/>
+      <c r="AA2" s="203" t="s">
         <v>656</v>
       </c>
-      <c r="AB2" s="197"/>
-      <c r="AC2" s="197"/>
-      <c r="AD2" s="198"/>
-      <c r="AE2" s="196" t="s">
+      <c r="AB2" s="204"/>
+      <c r="AC2" s="204"/>
+      <c r="AD2" s="205"/>
+      <c r="AE2" s="203" t="s">
         <v>657</v>
       </c>
-      <c r="AF2" s="197"/>
-      <c r="AG2" s="197"/>
-      <c r="AH2" s="198"/>
-      <c r="AI2" s="196" t="s">
+      <c r="AF2" s="204"/>
+      <c r="AG2" s="204"/>
+      <c r="AH2" s="205"/>
+      <c r="AI2" s="203" t="s">
         <v>658</v>
       </c>
-      <c r="AJ2" s="197"/>
-      <c r="AK2" s="197"/>
-      <c r="AL2" s="198"/>
-      <c r="AM2" s="196" t="s">
+      <c r="AJ2" s="204"/>
+      <c r="AK2" s="204"/>
+      <c r="AL2" s="205"/>
+      <c r="AM2" s="203" t="s">
         <v>659</v>
       </c>
-      <c r="AN2" s="197"/>
-      <c r="AO2" s="197"/>
-      <c r="AP2" s="198"/>
-      <c r="AQ2" s="196" t="s">
+      <c r="AN2" s="204"/>
+      <c r="AO2" s="204"/>
+      <c r="AP2" s="205"/>
+      <c r="AQ2" s="203" t="s">
         <v>660</v>
       </c>
-      <c r="AR2" s="197"/>
-      <c r="AS2" s="197"/>
-      <c r="AT2" s="198"/>
-      <c r="AU2" s="196" t="s">
+      <c r="AR2" s="204"/>
+      <c r="AS2" s="204"/>
+      <c r="AT2" s="205"/>
+      <c r="AU2" s="203" t="s">
         <v>722</v>
       </c>
-      <c r="AV2" s="197"/>
-      <c r="AW2" s="197"/>
-      <c r="AX2" s="198"/>
-      <c r="AY2" s="196" t="s">
+      <c r="AV2" s="204"/>
+      <c r="AW2" s="204"/>
+      <c r="AX2" s="205"/>
+      <c r="AY2" s="203" t="s">
         <v>729</v>
       </c>
-      <c r="AZ2" s="197"/>
-      <c r="BA2" s="197"/>
-      <c r="BB2" s="198"/>
+      <c r="AZ2" s="204"/>
+      <c r="BA2" s="204"/>
+      <c r="BB2" s="205"/>
     </row>
     <row r="3" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
-      <c r="C3" s="204"/>
-      <c r="D3" s="204"/>
-      <c r="E3" s="204"/>
-      <c r="F3" s="206"/>
+      <c r="C3" s="200"/>
+      <c r="D3" s="200"/>
+      <c r="E3" s="200"/>
+      <c r="F3" s="202"/>
       <c r="G3" s="80">
         <v>1</v>
       </c>
@@ -40203,6 +40206,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="O2:R2"/>
     <mergeCell ref="AU2:AX2"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="AY2:BB2"/>
@@ -40214,11 +40222,6 @@
     <mergeCell ref="AM2:AP2"/>
     <mergeCell ref="AQ2:AT2"/>
     <mergeCell ref="S2:V2"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="O2:R2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E84" location="ลูกค้า!A1" display="ลูกค้า!A1"/>
@@ -40409,7 +40412,7 @@
       <c r="A1" s="213" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="203" t="s">
+      <c r="B1" s="199" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="215" t="s">
@@ -40437,7 +40440,7 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="214"/>
-      <c r="B2" s="204"/>
+      <c r="B2" s="200"/>
       <c r="C2" s="1">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
ref order step 1 2 3 @Office
</commit_message>
<xml_diff>
--- a/_Doc/Feature.xlsx
+++ b/_Doc/Feature.xlsx
@@ -56,7 +56,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Menu!$A$1:$R$57</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -226,7 +226,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2544" uniqueCount="1814">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2545" uniqueCount="1815">
   <si>
     <t>No.</t>
   </si>
@@ -6099,13 +6099,16 @@
   <si>
     <t xml:space="preserve"> update ProductList set ProductListUnitRef2=0,ProductListUnitRef3=0;</t>
   </si>
+  <si>
+    <t>1.0.1.04</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="48" x14ac:knownFonts="1">
     <font>
@@ -6730,7 +6733,7 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
@@ -6814,20 +6817,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="1" fillId="6" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
@@ -6995,11 +6998,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="43" fontId="29" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="43" fontId="14" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -7089,6 +7092,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -7096,6 +7108,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -7109,18 +7124,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -8028,20 +8031,20 @@
       <c r="B1" s="2"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="199" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="199" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="199" t="s">
+      <c r="A2" s="203" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="203" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="203" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="200"/>
-      <c r="B3" s="200"/>
-      <c r="C3" s="200"/>
+      <c r="A3" s="204"/>
+      <c r="B3" s="204"/>
+      <c r="C3" s="204"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
@@ -9243,12 +9246,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
     <mergeCell ref="B43:C43"/>
     <mergeCell ref="B44:C44"/>
     <mergeCell ref="B45:C45"/>
@@ -9259,6 +9256,12 @@
     <mergeCell ref="B40:C40"/>
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -11186,7 +11189,7 @@
   <dimension ref="A1:C475"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A422" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C430" sqref="C430:C432"/>
+      <selection activeCell="B431" sqref="B431"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21.75" x14ac:dyDescent="0.5"/>
@@ -13676,6 +13679,9 @@
       <c r="C429" s="185"/>
     </row>
     <row r="430" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A430" s="151" t="s">
+        <v>1814</v>
+      </c>
       <c r="C430" s="185" t="s">
         <v>1811</v>
       </c>
@@ -22592,97 +22598,97 @@
     </row>
     <row r="2" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
-      <c r="B2" s="199" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="199" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="199" t="s">
+      <c r="B2" s="203" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="203" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="203" t="s">
         <v>130</v>
       </c>
-      <c r="E2" s="201" t="s">
+      <c r="E2" s="205" t="s">
         <v>723</v>
       </c>
-      <c r="F2" s="196" t="s">
+      <c r="F2" s="199" t="s">
         <v>651</v>
       </c>
-      <c r="G2" s="197"/>
-      <c r="H2" s="197"/>
-      <c r="I2" s="198"/>
-      <c r="J2" s="196" t="s">
+      <c r="G2" s="200"/>
+      <c r="H2" s="200"/>
+      <c r="I2" s="201"/>
+      <c r="J2" s="199" t="s">
         <v>652</v>
       </c>
-      <c r="K2" s="197"/>
-      <c r="L2" s="197"/>
-      <c r="M2" s="198"/>
-      <c r="N2" s="196" t="s">
+      <c r="K2" s="200"/>
+      <c r="L2" s="200"/>
+      <c r="M2" s="201"/>
+      <c r="N2" s="199" t="s">
         <v>653</v>
       </c>
-      <c r="O2" s="197"/>
-      <c r="P2" s="197"/>
-      <c r="Q2" s="198"/>
-      <c r="R2" s="196" t="s">
+      <c r="O2" s="200"/>
+      <c r="P2" s="200"/>
+      <c r="Q2" s="201"/>
+      <c r="R2" s="199" t="s">
         <v>654</v>
       </c>
-      <c r="S2" s="197"/>
-      <c r="T2" s="197"/>
-      <c r="U2" s="206"/>
-      <c r="V2" s="196" t="s">
+      <c r="S2" s="200"/>
+      <c r="T2" s="200"/>
+      <c r="U2" s="202"/>
+      <c r="V2" s="199" t="s">
         <v>655</v>
       </c>
-      <c r="W2" s="197"/>
-      <c r="X2" s="197"/>
-      <c r="Y2" s="206"/>
-      <c r="Z2" s="203" t="s">
+      <c r="W2" s="200"/>
+      <c r="X2" s="200"/>
+      <c r="Y2" s="202"/>
+      <c r="Z2" s="196" t="s">
         <v>656</v>
       </c>
-      <c r="AA2" s="204"/>
-      <c r="AB2" s="204"/>
-      <c r="AC2" s="205"/>
-      <c r="AD2" s="203" t="s">
+      <c r="AA2" s="197"/>
+      <c r="AB2" s="197"/>
+      <c r="AC2" s="198"/>
+      <c r="AD2" s="196" t="s">
         <v>657</v>
       </c>
-      <c r="AE2" s="204"/>
-      <c r="AF2" s="204"/>
-      <c r="AG2" s="205"/>
-      <c r="AH2" s="203" t="s">
+      <c r="AE2" s="197"/>
+      <c r="AF2" s="197"/>
+      <c r="AG2" s="198"/>
+      <c r="AH2" s="196" t="s">
         <v>658</v>
       </c>
-      <c r="AI2" s="204"/>
-      <c r="AJ2" s="204"/>
-      <c r="AK2" s="205"/>
-      <c r="AL2" s="203" t="s">
+      <c r="AI2" s="197"/>
+      <c r="AJ2" s="197"/>
+      <c r="AK2" s="198"/>
+      <c r="AL2" s="196" t="s">
         <v>659</v>
       </c>
-      <c r="AM2" s="204"/>
-      <c r="AN2" s="204"/>
-      <c r="AO2" s="205"/>
-      <c r="AP2" s="203" t="s">
+      <c r="AM2" s="197"/>
+      <c r="AN2" s="197"/>
+      <c r="AO2" s="198"/>
+      <c r="AP2" s="196" t="s">
         <v>660</v>
       </c>
-      <c r="AQ2" s="204"/>
-      <c r="AR2" s="204"/>
-      <c r="AS2" s="205"/>
-      <c r="AT2" s="203" t="s">
+      <c r="AQ2" s="197"/>
+      <c r="AR2" s="197"/>
+      <c r="AS2" s="198"/>
+      <c r="AT2" s="196" t="s">
         <v>722</v>
       </c>
-      <c r="AU2" s="204"/>
-      <c r="AV2" s="204"/>
-      <c r="AW2" s="205"/>
-      <c r="AX2" s="203" t="s">
+      <c r="AU2" s="197"/>
+      <c r="AV2" s="197"/>
+      <c r="AW2" s="198"/>
+      <c r="AX2" s="196" t="s">
         <v>729</v>
       </c>
-      <c r="AY2" s="204"/>
-      <c r="AZ2" s="204"/>
-      <c r="BA2" s="205"/>
+      <c r="AY2" s="197"/>
+      <c r="AZ2" s="197"/>
+      <c r="BA2" s="198"/>
     </row>
     <row r="3" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
-      <c r="B3" s="200"/>
-      <c r="C3" s="200"/>
-      <c r="D3" s="200"/>
-      <c r="E3" s="202"/>
+      <c r="B3" s="204"/>
+      <c r="C3" s="204"/>
+      <c r="D3" s="204"/>
+      <c r="E3" s="206"/>
       <c r="F3" s="80">
         <v>1</v>
       </c>
@@ -27836,6 +27842,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:I2"/>
     <mergeCell ref="AL2:AO2"/>
     <mergeCell ref="AP2:AS2"/>
     <mergeCell ref="AT2:AW2"/>
@@ -27846,12 +27858,6 @@
     <mergeCell ref="Z2:AC2"/>
     <mergeCell ref="AD2:AG2"/>
     <mergeCell ref="AH2:AK2"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:I2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D84" location="ลูกค้า!A1" display="ลูกค้า!A1"/>
@@ -28369,16 +28375,16 @@
     <row r="2" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
-      <c r="C2" s="199" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="199" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="199" t="s">
+      <c r="C2" s="203" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="203" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="203" t="s">
         <v>130</v>
       </c>
-      <c r="F2" s="201" t="s">
+      <c r="F2" s="205" t="s">
         <v>723</v>
       </c>
       <c r="G2" s="207" t="s">
@@ -28445,10 +28451,10 @@
     <row r="3" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
-      <c r="C3" s="200"/>
-      <c r="D3" s="200"/>
-      <c r="E3" s="200"/>
-      <c r="F3" s="202"/>
+      <c r="C3" s="204"/>
+      <c r="D3" s="204"/>
+      <c r="E3" s="204"/>
+      <c r="F3" s="206"/>
       <c r="G3" s="80">
         <v>1</v>
       </c>
@@ -34244,6 +34250,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="AE2:AH2"/>
+    <mergeCell ref="AI2:AL2"/>
+    <mergeCell ref="AM2:AP2"/>
+    <mergeCell ref="AQ2:AT2"/>
+    <mergeCell ref="AA2:AD2"/>
     <mergeCell ref="K2:N2"/>
     <mergeCell ref="O2:R2"/>
     <mergeCell ref="S2:V2"/>
@@ -34253,11 +34264,6 @@
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="G2:J2"/>
-    <mergeCell ref="AE2:AH2"/>
-    <mergeCell ref="AI2:AL2"/>
-    <mergeCell ref="AM2:AP2"/>
-    <mergeCell ref="AQ2:AT2"/>
-    <mergeCell ref="AA2:AD2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E84" location="ลูกค้า!A1" display="ลูกค้า!A1"/>
@@ -34735,98 +34741,98 @@
     <row r="2" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
-      <c r="C2" s="199" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="199" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="199" t="s">
+      <c r="C2" s="203" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="203" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="203" t="s">
         <v>130</v>
       </c>
-      <c r="F2" s="201" t="s">
+      <c r="F2" s="205" t="s">
         <v>723</v>
       </c>
-      <c r="G2" s="196" t="s">
+      <c r="G2" s="199" t="s">
         <v>651</v>
       </c>
-      <c r="H2" s="197"/>
-      <c r="I2" s="197"/>
-      <c r="J2" s="198"/>
-      <c r="K2" s="196" t="s">
+      <c r="H2" s="200"/>
+      <c r="I2" s="200"/>
+      <c r="J2" s="201"/>
+      <c r="K2" s="199" t="s">
         <v>652</v>
       </c>
-      <c r="L2" s="197"/>
-      <c r="M2" s="197"/>
-      <c r="N2" s="198"/>
-      <c r="O2" s="196" t="s">
+      <c r="L2" s="200"/>
+      <c r="M2" s="200"/>
+      <c r="N2" s="201"/>
+      <c r="O2" s="199" t="s">
         <v>653</v>
       </c>
-      <c r="P2" s="197"/>
-      <c r="Q2" s="197"/>
-      <c r="R2" s="198"/>
-      <c r="S2" s="196" t="s">
+      <c r="P2" s="200"/>
+      <c r="Q2" s="200"/>
+      <c r="R2" s="201"/>
+      <c r="S2" s="199" t="s">
         <v>654</v>
       </c>
-      <c r="T2" s="197"/>
-      <c r="U2" s="197"/>
-      <c r="V2" s="206"/>
-      <c r="W2" s="196" t="s">
+      <c r="T2" s="200"/>
+      <c r="U2" s="200"/>
+      <c r="V2" s="202"/>
+      <c r="W2" s="199" t="s">
         <v>655</v>
       </c>
-      <c r="X2" s="197"/>
-      <c r="Y2" s="197"/>
-      <c r="Z2" s="206"/>
-      <c r="AA2" s="203" t="s">
+      <c r="X2" s="200"/>
+      <c r="Y2" s="200"/>
+      <c r="Z2" s="202"/>
+      <c r="AA2" s="196" t="s">
         <v>656</v>
       </c>
-      <c r="AB2" s="204"/>
-      <c r="AC2" s="204"/>
-      <c r="AD2" s="205"/>
-      <c r="AE2" s="203" t="s">
+      <c r="AB2" s="197"/>
+      <c r="AC2" s="197"/>
+      <c r="AD2" s="198"/>
+      <c r="AE2" s="196" t="s">
         <v>657</v>
       </c>
-      <c r="AF2" s="204"/>
-      <c r="AG2" s="204"/>
-      <c r="AH2" s="205"/>
-      <c r="AI2" s="203" t="s">
+      <c r="AF2" s="197"/>
+      <c r="AG2" s="197"/>
+      <c r="AH2" s="198"/>
+      <c r="AI2" s="196" t="s">
         <v>658</v>
       </c>
-      <c r="AJ2" s="204"/>
-      <c r="AK2" s="204"/>
-      <c r="AL2" s="205"/>
-      <c r="AM2" s="203" t="s">
+      <c r="AJ2" s="197"/>
+      <c r="AK2" s="197"/>
+      <c r="AL2" s="198"/>
+      <c r="AM2" s="196" t="s">
         <v>659</v>
       </c>
-      <c r="AN2" s="204"/>
-      <c r="AO2" s="204"/>
-      <c r="AP2" s="205"/>
-      <c r="AQ2" s="203" t="s">
+      <c r="AN2" s="197"/>
+      <c r="AO2" s="197"/>
+      <c r="AP2" s="198"/>
+      <c r="AQ2" s="196" t="s">
         <v>660</v>
       </c>
-      <c r="AR2" s="204"/>
-      <c r="AS2" s="204"/>
-      <c r="AT2" s="205"/>
-      <c r="AU2" s="203" t="s">
+      <c r="AR2" s="197"/>
+      <c r="AS2" s="197"/>
+      <c r="AT2" s="198"/>
+      <c r="AU2" s="196" t="s">
         <v>722</v>
       </c>
-      <c r="AV2" s="204"/>
-      <c r="AW2" s="204"/>
-      <c r="AX2" s="205"/>
-      <c r="AY2" s="203" t="s">
+      <c r="AV2" s="197"/>
+      <c r="AW2" s="197"/>
+      <c r="AX2" s="198"/>
+      <c r="AY2" s="196" t="s">
         <v>729</v>
       </c>
-      <c r="AZ2" s="204"/>
-      <c r="BA2" s="204"/>
-      <c r="BB2" s="205"/>
+      <c r="AZ2" s="197"/>
+      <c r="BA2" s="197"/>
+      <c r="BB2" s="198"/>
     </row>
     <row r="3" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
-      <c r="C3" s="200"/>
-      <c r="D3" s="200"/>
-      <c r="E3" s="200"/>
-      <c r="F3" s="202"/>
+      <c r="C3" s="204"/>
+      <c r="D3" s="204"/>
+      <c r="E3" s="204"/>
+      <c r="F3" s="206"/>
       <c r="G3" s="80">
         <v>1</v>
       </c>
@@ -40239,11 +40245,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="O2:R2"/>
     <mergeCell ref="AU2:AX2"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="AY2:BB2"/>
@@ -40255,6 +40256,11 @@
     <mergeCell ref="AM2:AP2"/>
     <mergeCell ref="AQ2:AT2"/>
     <mergeCell ref="S2:V2"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="O2:R2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E84" location="ลูกค้า!A1" display="ลูกค้า!A1"/>
@@ -40445,7 +40451,7 @@
       <c r="A1" s="213" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="199" t="s">
+      <c r="B1" s="203" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="215" t="s">
@@ -40473,7 +40479,7 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="214"/>
-      <c r="B2" s="200"/>
+      <c r="B2" s="204"/>
       <c r="C2" s="1">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
fixed ref order @office
</commit_message>
<xml_diff>
--- a/_Doc/Feature.xlsx
+++ b/_Doc/Feature.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="1095" windowWidth="19080" windowHeight="6405" tabRatio="884" activeTab="45"/>
+    <workbookView xWindow="120" yWindow="1095" windowWidth="19080" windowHeight="6405" tabRatio="884" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="46" r:id="rId1"/>
@@ -57,7 +57,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Menu!$A$1:$R$57</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -227,7 +227,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2560" uniqueCount="1823">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2558" uniqueCount="1823">
   <si>
     <t>No.</t>
   </si>
@@ -6098,9 +6098,6 @@
     <t xml:space="preserve"> alter table ProductList add ProductListUnitRef3  bigint;</t>
   </si>
   <si>
-    <t xml:space="preserve"> update ProductList set ProductListUnitRef2=0,ProductListUnitRef3=0;</t>
-  </si>
-  <si>
     <t>1.0.1.04</t>
   </si>
   <si>
@@ -6110,12 +6107,6 @@
     <t>pro</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
     <t>prolistid</t>
   </si>
   <si>
@@ -6126,6 +6117,15 @@
   </si>
   <si>
     <t>ref</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> alter table ProductList add ProductListUnitRef1  bigint;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> update ProductList set ProductListUnitRef1=0, ProductListUnitRef2=0,ProductListUnitRef3=0;</t>
+  </si>
+  <si>
+    <t>7023</t>
   </si>
 </sst>
 </file>
@@ -6133,7 +6133,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="48" x14ac:knownFonts="1">
     <font>
@@ -6758,13 +6758,13 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="222">
+  <cellXfs count="221">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -6842,20 +6842,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="1" fillId="6" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
@@ -7023,11 +7023,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="43" fontId="29" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="43" fontId="14" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -7111,11 +7111,24 @@
     <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -7124,6 +7137,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -7137,18 +7153,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -7182,11 +7186,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -8064,20 +8063,20 @@
       <c r="B1" s="2"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="199" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="199" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="199" t="s">
+      <c r="A2" s="205" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="205" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="205" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="200"/>
-      <c r="B3" s="200"/>
-      <c r="C3" s="200"/>
+      <c r="A3" s="206"/>
+      <c r="B3" s="206"/>
+      <c r="C3" s="206"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
@@ -9172,100 +9171,100 @@
       </c>
     </row>
     <row r="31" spans="2:3" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="B31" s="216" t="s">
+      <c r="B31" s="218" t="s">
         <v>162</v>
       </c>
-      <c r="C31" s="216"/>
+      <c r="C31" s="218"/>
     </row>
     <row r="32" spans="2:3" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="B32" s="216" t="s">
+      <c r="B32" s="218" t="s">
         <v>163</v>
       </c>
-      <c r="C32" s="216"/>
+      <c r="C32" s="218"/>
     </row>
     <row r="33" spans="2:3" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="B33" s="216" t="s">
+      <c r="B33" s="218" t="s">
         <v>164</v>
       </c>
-      <c r="C33" s="216"/>
+      <c r="C33" s="218"/>
     </row>
     <row r="34" spans="2:3" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="B34" s="216" t="s">
+      <c r="B34" s="218" t="s">
         <v>165</v>
       </c>
-      <c r="C34" s="216"/>
+      <c r="C34" s="218"/>
     </row>
     <row r="35" spans="2:3" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="B35" s="216" t="s">
+      <c r="B35" s="218" t="s">
         <v>166</v>
       </c>
-      <c r="C35" s="216"/>
+      <c r="C35" s="218"/>
     </row>
     <row r="36" spans="2:3" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="B36" s="216" t="s">
+      <c r="B36" s="218" t="s">
         <v>167</v>
       </c>
-      <c r="C36" s="216"/>
+      <c r="C36" s="218"/>
     </row>
     <row r="37" spans="2:3" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="B37" s="216" t="s">
+      <c r="B37" s="218" t="s">
         <v>168</v>
       </c>
-      <c r="C37" s="216"/>
+      <c r="C37" s="218"/>
     </row>
     <row r="38" spans="2:3" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="B38" s="216" t="s">
+      <c r="B38" s="218" t="s">
         <v>169</v>
       </c>
-      <c r="C38" s="216"/>
+      <c r="C38" s="218"/>
     </row>
     <row r="39" spans="2:3" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="B39" s="216" t="s">
+      <c r="B39" s="218" t="s">
         <v>170</v>
       </c>
-      <c r="C39" s="216"/>
+      <c r="C39" s="218"/>
     </row>
     <row r="40" spans="2:3" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="B40" s="216" t="s">
+      <c r="B40" s="218" t="s">
         <v>171</v>
       </c>
-      <c r="C40" s="216"/>
+      <c r="C40" s="218"/>
     </row>
     <row r="41" spans="2:3" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="B41" s="216" t="s">
+      <c r="B41" s="218" t="s">
         <v>172</v>
       </c>
-      <c r="C41" s="216"/>
+      <c r="C41" s="218"/>
     </row>
     <row r="42" spans="2:3" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="B42" s="216" t="s">
+      <c r="B42" s="218" t="s">
         <v>173</v>
       </c>
-      <c r="C42" s="216"/>
+      <c r="C42" s="218"/>
     </row>
     <row r="43" spans="2:3" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="B43" s="216" t="s">
+      <c r="B43" s="218" t="s">
         <v>174</v>
       </c>
-      <c r="C43" s="216"/>
+      <c r="C43" s="218"/>
     </row>
     <row r="44" spans="2:3" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="B44" s="216" t="s">
+      <c r="B44" s="218" t="s">
         <v>175</v>
       </c>
-      <c r="C44" s="216"/>
+      <c r="C44" s="218"/>
     </row>
     <row r="45" spans="2:3" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="B45" s="216" t="s">
+      <c r="B45" s="218" t="s">
         <v>176</v>
       </c>
-      <c r="C45" s="216"/>
+      <c r="C45" s="218"/>
     </row>
     <row r="46" spans="2:3" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="B46" s="216" t="s">
+      <c r="B46" s="218" t="s">
         <v>177</v>
       </c>
-      <c r="C46" s="216"/>
+      <c r="C46" s="218"/>
     </row>
     <row r="47" spans="2:3" ht="18.75" x14ac:dyDescent="0.45">
       <c r="B47" s="20" t="s">
@@ -9279,12 +9278,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
     <mergeCell ref="B43:C43"/>
     <mergeCell ref="B44:C44"/>
     <mergeCell ref="B45:C45"/>
@@ -9295,6 +9288,12 @@
     <mergeCell ref="B40:C40"/>
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -11221,8 +11220,8 @@
   </sheetPr>
   <dimension ref="A1:C475"/>
   <sheetViews>
-    <sheetView topLeftCell="A446" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B431" sqref="B431"/>
+    <sheetView tabSelected="1" topLeftCell="A446" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B439" sqref="B439"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21.75" x14ac:dyDescent="0.5"/>
@@ -11255,7 +11254,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="B4" s="194" t="s">
+      <c r="B4" s="196" t="s">
         <v>993</v>
       </c>
       <c r="C4" s="153" t="s">
@@ -11263,13 +11262,13 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="B5" s="194"/>
+      <c r="B5" s="196"/>
       <c r="C5" s="151" t="s">
         <v>991</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="B6" s="194"/>
+      <c r="B6" s="196"/>
       <c r="C6" s="151" t="s">
         <v>992</v>
       </c>
@@ -11460,7 +11459,7 @@
       <c r="B37" s="151" t="s">
         <v>1027</v>
       </c>
-      <c r="C37" s="195" t="s">
+      <c r="C37" s="197" t="s">
         <v>1061</v>
       </c>
     </row>
@@ -11468,61 +11467,61 @@
       <c r="B38" s="151" t="s">
         <v>1028</v>
       </c>
-      <c r="C38" s="195"/>
+      <c r="C38" s="197"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B39" s="151" t="s">
         <v>1053</v>
       </c>
-      <c r="C39" s="195"/>
+      <c r="C39" s="197"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B40" s="151" t="s">
         <v>1057</v>
       </c>
-      <c r="C40" s="195"/>
+      <c r="C40" s="197"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B41" s="151" t="s">
         <v>1058</v>
       </c>
-      <c r="C41" s="195"/>
+      <c r="C41" s="197"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B42" s="151" t="s">
         <v>1059</v>
       </c>
-      <c r="C42" s="195"/>
+      <c r="C42" s="197"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B43" s="151" t="s">
         <v>1063</v>
       </c>
-      <c r="C43" s="195"/>
+      <c r="C43" s="197"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B44" s="151" t="s">
         <v>1062</v>
       </c>
-      <c r="C44" s="195"/>
+      <c r="C44" s="197"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="C45" s="195"/>
+      <c r="C45" s="197"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="C46" s="195"/>
+      <c r="C46" s="197"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="C47" s="195"/>
+      <c r="C47" s="197"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="C48" s="195"/>
+      <c r="C48" s="197"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="C49" s="195"/>
+      <c r="C49" s="197"/>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="C50" s="195"/>
+      <c r="C50" s="197"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A51" s="151" t="s">
@@ -13709,11 +13708,13 @@
       <c r="C428" s="185"/>
     </row>
     <row r="429" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="C429" s="185"/>
+      <c r="C429" s="185" t="s">
+        <v>1820</v>
+      </c>
     </row>
     <row r="430" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A430" s="151" t="s">
-        <v>1814</v>
+        <v>1813</v>
       </c>
       <c r="C430" s="185" t="s">
         <v>1811</v>
@@ -13726,7 +13727,7 @@
     </row>
     <row r="432" spans="1:3" x14ac:dyDescent="0.5">
       <c r="C432" s="185" t="s">
-        <v>1813</v>
+        <v>1821</v>
       </c>
     </row>
     <row r="433" spans="1:3" x14ac:dyDescent="0.5">
@@ -14818,7 +14819,7 @@
       </c>
     </row>
     <row r="39" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="217" t="s">
+      <c r="A39" s="219" t="s">
         <v>927</v>
       </c>
       <c r="B39" s="19" t="s">
@@ -14826,19 +14827,19 @@
       </c>
     </row>
     <row r="40" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="217"/>
+      <c r="A40" s="219"/>
       <c r="B40" s="19" t="s">
         <v>613</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A41" s="217"/>
+      <c r="A41" s="219"/>
       <c r="B41" s="19" t="s">
         <v>614</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="A42" s="217" t="s">
+      <c r="A42" s="219" t="s">
         <v>927</v>
       </c>
       <c r="B42" s="19" t="s">
@@ -14846,13 +14847,13 @@
       </c>
     </row>
     <row r="43" spans="1:2" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="A43" s="217"/>
+      <c r="A43" s="219"/>
       <c r="B43" s="19" t="s">
         <v>616</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="A44" s="217"/>
+      <c r="A44" s="219"/>
       <c r="B44" s="19" t="s">
         <v>617</v>
       </c>
@@ -21450,86 +21451,86 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.28515625" style="120" customWidth="1"/>
     <col min="2" max="2" width="5.28515625" customWidth="1"/>
-    <col min="4" max="4" width="7.140625" customWidth="1"/>
-    <col min="5" max="5" width="5.42578125" style="120" customWidth="1"/>
-    <col min="6" max="6" width="8.140625" style="12" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" style="120" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" style="12" customWidth="1"/>
     <col min="8" max="8" width="9.140625" style="120"/>
     <col min="10" max="11" width="9.140625" style="120"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="120" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="219"/>
-      <c r="B1" s="219" t="s">
+      <c r="A1" s="194"/>
+      <c r="B1" s="194" t="s">
+        <v>1814</v>
+      </c>
+      <c r="C1" s="194" t="s">
         <v>1815</v>
       </c>
-      <c r="C1" s="219" t="s">
+      <c r="D1" s="194" t="s">
         <v>1816</v>
       </c>
-      <c r="D1" s="219" t="s">
+      <c r="E1" s="194" t="s">
+        <v>1818</v>
+      </c>
+      <c r="F1" s="195" t="s">
+        <v>1817</v>
+      </c>
+      <c r="G1" s="220">
+        <v>1</v>
+      </c>
+      <c r="H1" s="220"/>
+      <c r="I1" s="220">
+        <v>2</v>
+      </c>
+      <c r="J1" s="220"/>
+      <c r="K1" s="220">
+        <v>3</v>
+      </c>
+      <c r="L1" s="220"/>
+    </row>
+    <row r="2" spans="1:12" s="120" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="194"/>
+      <c r="B2" s="194"/>
+      <c r="C2" s="194"/>
+      <c r="D2" s="194"/>
+      <c r="E2" s="194"/>
+      <c r="F2" s="195"/>
+      <c r="G2" s="195" t="s">
         <v>1819</v>
       </c>
-      <c r="E1" s="219" t="s">
-        <v>1821</v>
-      </c>
-      <c r="F1" s="220" t="s">
-        <v>1820</v>
-      </c>
-      <c r="G1" s="221">
-        <v>1</v>
-      </c>
-      <c r="H1" s="221"/>
-      <c r="I1" s="221">
-        <v>2</v>
-      </c>
-      <c r="J1" s="221"/>
-      <c r="K1" s="221">
-        <v>3</v>
-      </c>
-      <c r="L1" s="221"/>
-    </row>
-    <row r="2" spans="1:12" s="120" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="219"/>
-      <c r="B2" s="219"/>
-      <c r="C2" s="219"/>
-      <c r="D2" s="219"/>
-      <c r="E2" s="219"/>
-      <c r="F2" s="220"/>
-      <c r="G2" s="220" t="s">
-        <v>1822</v>
-      </c>
-      <c r="H2" s="220" t="s">
-        <v>1821</v>
-      </c>
-      <c r="I2" s="220" t="s">
-        <v>1822</v>
-      </c>
-      <c r="J2" s="220" t="s">
-        <v>1821</v>
-      </c>
-      <c r="K2" s="220" t="s">
-        <v>1822</v>
-      </c>
-      <c r="L2" s="220" t="s">
-        <v>1821</v>
+      <c r="H2" s="195" t="s">
+        <v>1818</v>
+      </c>
+      <c r="I2" s="195" t="s">
+        <v>1819</v>
+      </c>
+      <c r="J2" s="195" t="s">
+        <v>1818</v>
+      </c>
+      <c r="K2" s="195" t="s">
+        <v>1819</v>
+      </c>
+      <c r="L2" s="195" t="s">
+        <v>1818</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>33</v>
       </c>
-      <c r="C3" t="s">
-        <v>1817</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
+      <c r="C3" s="55">
+        <v>7023</v>
+      </c>
+      <c r="D3" s="120">
+        <v>112729</v>
       </c>
       <c r="E3" s="120">
         <v>2</v>
@@ -21538,13 +21539,13 @@
         <v>5</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>112729</v>
       </c>
       <c r="H3" s="120">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I3">
-        <v>3</v>
+        <v>112731</v>
       </c>
       <c r="J3" s="120">
         <v>1</v>
@@ -21554,11 +21555,11 @@
       <c r="B4">
         <v>33</v>
       </c>
-      <c r="C4" s="218" t="s">
-        <v>1818</v>
+      <c r="C4" s="55">
+        <v>7022</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>112728</v>
       </c>
       <c r="E4" s="120">
         <v>2</v>
@@ -21566,14 +21567,14 @@
       <c r="F4" s="12">
         <v>6</v>
       </c>
-      <c r="G4">
-        <v>2</v>
+      <c r="G4" s="120">
+        <v>112728</v>
       </c>
       <c r="H4" s="120">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I4">
-        <v>4</v>
+        <v>112730</v>
       </c>
       <c r="J4" s="120">
         <v>1</v>
@@ -21583,11 +21584,11 @@
       <c r="B5">
         <v>34</v>
       </c>
-      <c r="C5" t="s">
-        <v>1817</v>
+      <c r="C5" s="55">
+        <v>7022</v>
       </c>
       <c r="D5">
-        <v>3</v>
+        <v>112730</v>
       </c>
       <c r="E5" s="120">
         <v>1</v>
@@ -21597,11 +21598,11 @@
       <c r="B6">
         <v>34</v>
       </c>
-      <c r="C6" s="218" t="s">
-        <v>1818</v>
+      <c r="C6" s="55" t="s">
+        <v>1822</v>
       </c>
       <c r="D6">
-        <v>4</v>
+        <v>112731</v>
       </c>
       <c r="E6" s="120">
         <v>1</v>
@@ -21614,7 +21615,7 @@
     <mergeCell ref="K1:L1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -22803,97 +22804,97 @@
     </row>
     <row r="2" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
-      <c r="B2" s="199" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="199" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="199" t="s">
+      <c r="B2" s="205" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="205" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="205" t="s">
         <v>130</v>
       </c>
-      <c r="E2" s="201" t="s">
+      <c r="E2" s="207" t="s">
         <v>723</v>
       </c>
-      <c r="F2" s="196" t="s">
+      <c r="F2" s="201" t="s">
         <v>651</v>
       </c>
-      <c r="G2" s="197"/>
-      <c r="H2" s="197"/>
-      <c r="I2" s="198"/>
-      <c r="J2" s="196" t="s">
+      <c r="G2" s="202"/>
+      <c r="H2" s="202"/>
+      <c r="I2" s="203"/>
+      <c r="J2" s="201" t="s">
         <v>652</v>
       </c>
-      <c r="K2" s="197"/>
-      <c r="L2" s="197"/>
-      <c r="M2" s="198"/>
-      <c r="N2" s="196" t="s">
+      <c r="K2" s="202"/>
+      <c r="L2" s="202"/>
+      <c r="M2" s="203"/>
+      <c r="N2" s="201" t="s">
         <v>653</v>
       </c>
-      <c r="O2" s="197"/>
-      <c r="P2" s="197"/>
-      <c r="Q2" s="198"/>
-      <c r="R2" s="196" t="s">
+      <c r="O2" s="202"/>
+      <c r="P2" s="202"/>
+      <c r="Q2" s="203"/>
+      <c r="R2" s="201" t="s">
         <v>654</v>
       </c>
-      <c r="S2" s="197"/>
-      <c r="T2" s="197"/>
-      <c r="U2" s="206"/>
-      <c r="V2" s="196" t="s">
+      <c r="S2" s="202"/>
+      <c r="T2" s="202"/>
+      <c r="U2" s="204"/>
+      <c r="V2" s="201" t="s">
         <v>655</v>
       </c>
-      <c r="W2" s="197"/>
-      <c r="X2" s="197"/>
-      <c r="Y2" s="206"/>
-      <c r="Z2" s="203" t="s">
+      <c r="W2" s="202"/>
+      <c r="X2" s="202"/>
+      <c r="Y2" s="204"/>
+      <c r="Z2" s="198" t="s">
         <v>656</v>
       </c>
-      <c r="AA2" s="204"/>
-      <c r="AB2" s="204"/>
-      <c r="AC2" s="205"/>
-      <c r="AD2" s="203" t="s">
+      <c r="AA2" s="199"/>
+      <c r="AB2" s="199"/>
+      <c r="AC2" s="200"/>
+      <c r="AD2" s="198" t="s">
         <v>657</v>
       </c>
-      <c r="AE2" s="204"/>
-      <c r="AF2" s="204"/>
-      <c r="AG2" s="205"/>
-      <c r="AH2" s="203" t="s">
+      <c r="AE2" s="199"/>
+      <c r="AF2" s="199"/>
+      <c r="AG2" s="200"/>
+      <c r="AH2" s="198" t="s">
         <v>658</v>
       </c>
-      <c r="AI2" s="204"/>
-      <c r="AJ2" s="204"/>
-      <c r="AK2" s="205"/>
-      <c r="AL2" s="203" t="s">
+      <c r="AI2" s="199"/>
+      <c r="AJ2" s="199"/>
+      <c r="AK2" s="200"/>
+      <c r="AL2" s="198" t="s">
         <v>659</v>
       </c>
-      <c r="AM2" s="204"/>
-      <c r="AN2" s="204"/>
-      <c r="AO2" s="205"/>
-      <c r="AP2" s="203" t="s">
+      <c r="AM2" s="199"/>
+      <c r="AN2" s="199"/>
+      <c r="AO2" s="200"/>
+      <c r="AP2" s="198" t="s">
         <v>660</v>
       </c>
-      <c r="AQ2" s="204"/>
-      <c r="AR2" s="204"/>
-      <c r="AS2" s="205"/>
-      <c r="AT2" s="203" t="s">
+      <c r="AQ2" s="199"/>
+      <c r="AR2" s="199"/>
+      <c r="AS2" s="200"/>
+      <c r="AT2" s="198" t="s">
         <v>722</v>
       </c>
-      <c r="AU2" s="204"/>
-      <c r="AV2" s="204"/>
-      <c r="AW2" s="205"/>
-      <c r="AX2" s="203" t="s">
+      <c r="AU2" s="199"/>
+      <c r="AV2" s="199"/>
+      <c r="AW2" s="200"/>
+      <c r="AX2" s="198" t="s">
         <v>729</v>
       </c>
-      <c r="AY2" s="204"/>
-      <c r="AZ2" s="204"/>
-      <c r="BA2" s="205"/>
+      <c r="AY2" s="199"/>
+      <c r="AZ2" s="199"/>
+      <c r="BA2" s="200"/>
     </row>
     <row r="3" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
-      <c r="B3" s="200"/>
-      <c r="C3" s="200"/>
-      <c r="D3" s="200"/>
-      <c r="E3" s="202"/>
+      <c r="B3" s="206"/>
+      <c r="C3" s="206"/>
+      <c r="D3" s="206"/>
+      <c r="E3" s="208"/>
       <c r="F3" s="80">
         <v>1</v>
       </c>
@@ -28047,6 +28048,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:I2"/>
     <mergeCell ref="AL2:AO2"/>
     <mergeCell ref="AP2:AS2"/>
     <mergeCell ref="AT2:AW2"/>
@@ -28057,12 +28064,6 @@
     <mergeCell ref="Z2:AC2"/>
     <mergeCell ref="AD2:AG2"/>
     <mergeCell ref="AH2:AK2"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:I2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D84" location="ลูกค้า!A1" display="ลูกค้า!A1"/>
@@ -28580,86 +28581,86 @@
     <row r="2" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
-      <c r="C2" s="199" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="199" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="199" t="s">
+      <c r="C2" s="205" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="205" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="205" t="s">
         <v>130</v>
       </c>
-      <c r="F2" s="201" t="s">
+      <c r="F2" s="207" t="s">
         <v>723</v>
       </c>
-      <c r="G2" s="207" t="s">
+      <c r="G2" s="209" t="s">
         <v>660</v>
       </c>
-      <c r="H2" s="208"/>
-      <c r="I2" s="208"/>
-      <c r="J2" s="210"/>
-      <c r="K2" s="207" t="s">
+      <c r="H2" s="210"/>
+      <c r="I2" s="210"/>
+      <c r="J2" s="212"/>
+      <c r="K2" s="209" t="s">
         <v>722</v>
       </c>
-      <c r="L2" s="208"/>
-      <c r="M2" s="208"/>
-      <c r="N2" s="209"/>
-      <c r="O2" s="207" t="s">
+      <c r="L2" s="210"/>
+      <c r="M2" s="210"/>
+      <c r="N2" s="211"/>
+      <c r="O2" s="209" t="s">
         <v>729</v>
       </c>
-      <c r="P2" s="208"/>
-      <c r="Q2" s="208"/>
-      <c r="R2" s="209"/>
-      <c r="S2" s="207" t="s">
+      <c r="P2" s="210"/>
+      <c r="Q2" s="210"/>
+      <c r="R2" s="211"/>
+      <c r="S2" s="209" t="s">
         <v>651</v>
       </c>
-      <c r="T2" s="208"/>
-      <c r="U2" s="208"/>
-      <c r="V2" s="209"/>
-      <c r="W2" s="207" t="s">
+      <c r="T2" s="210"/>
+      <c r="U2" s="210"/>
+      <c r="V2" s="211"/>
+      <c r="W2" s="209" t="s">
         <v>730</v>
       </c>
-      <c r="X2" s="208"/>
-      <c r="Y2" s="208"/>
-      <c r="Z2" s="209"/>
-      <c r="AA2" s="207" t="s">
+      <c r="X2" s="210"/>
+      <c r="Y2" s="210"/>
+      <c r="Z2" s="211"/>
+      <c r="AA2" s="209" t="s">
         <v>653</v>
       </c>
-      <c r="AB2" s="208"/>
-      <c r="AC2" s="208"/>
-      <c r="AD2" s="209"/>
-      <c r="AE2" s="207" t="s">
+      <c r="AB2" s="210"/>
+      <c r="AC2" s="210"/>
+      <c r="AD2" s="211"/>
+      <c r="AE2" s="209" t="s">
         <v>731</v>
       </c>
-      <c r="AF2" s="208"/>
-      <c r="AG2" s="208"/>
-      <c r="AH2" s="209"/>
-      <c r="AI2" s="207" t="s">
+      <c r="AF2" s="210"/>
+      <c r="AG2" s="210"/>
+      <c r="AH2" s="211"/>
+      <c r="AI2" s="209" t="s">
         <v>655</v>
       </c>
-      <c r="AJ2" s="208"/>
-      <c r="AK2" s="208"/>
-      <c r="AL2" s="209"/>
-      <c r="AM2" s="207" t="s">
+      <c r="AJ2" s="210"/>
+      <c r="AK2" s="210"/>
+      <c r="AL2" s="211"/>
+      <c r="AM2" s="209" t="s">
         <v>656</v>
       </c>
-      <c r="AN2" s="208"/>
-      <c r="AO2" s="208"/>
-      <c r="AP2" s="209"/>
-      <c r="AQ2" s="207" t="s">
+      <c r="AN2" s="210"/>
+      <c r="AO2" s="210"/>
+      <c r="AP2" s="211"/>
+      <c r="AQ2" s="209" t="s">
         <v>657</v>
       </c>
-      <c r="AR2" s="208"/>
-      <c r="AS2" s="208"/>
-      <c r="AT2" s="209"/>
+      <c r="AR2" s="210"/>
+      <c r="AS2" s="210"/>
+      <c r="AT2" s="211"/>
     </row>
     <row r="3" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
-      <c r="C3" s="200"/>
-      <c r="D3" s="200"/>
-      <c r="E3" s="200"/>
-      <c r="F3" s="202"/>
+      <c r="C3" s="206"/>
+      <c r="D3" s="206"/>
+      <c r="E3" s="206"/>
+      <c r="F3" s="208"/>
       <c r="G3" s="80">
         <v>1</v>
       </c>
@@ -34455,6 +34456,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="AE2:AH2"/>
+    <mergeCell ref="AI2:AL2"/>
+    <mergeCell ref="AM2:AP2"/>
+    <mergeCell ref="AQ2:AT2"/>
+    <mergeCell ref="AA2:AD2"/>
     <mergeCell ref="K2:N2"/>
     <mergeCell ref="O2:R2"/>
     <mergeCell ref="S2:V2"/>
@@ -34464,11 +34470,6 @@
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="G2:J2"/>
-    <mergeCell ref="AE2:AH2"/>
-    <mergeCell ref="AI2:AL2"/>
-    <mergeCell ref="AM2:AP2"/>
-    <mergeCell ref="AQ2:AT2"/>
-    <mergeCell ref="AA2:AD2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E84" location="ลูกค้า!A1" display="ลูกค้า!A1"/>
@@ -34946,98 +34947,98 @@
     <row r="2" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
-      <c r="C2" s="199" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="199" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="199" t="s">
+      <c r="C2" s="205" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="205" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="205" t="s">
         <v>130</v>
       </c>
-      <c r="F2" s="201" t="s">
+      <c r="F2" s="207" t="s">
         <v>723</v>
       </c>
-      <c r="G2" s="196" t="s">
+      <c r="G2" s="201" t="s">
         <v>651</v>
       </c>
-      <c r="H2" s="197"/>
-      <c r="I2" s="197"/>
-      <c r="J2" s="198"/>
-      <c r="K2" s="196" t="s">
+      <c r="H2" s="202"/>
+      <c r="I2" s="202"/>
+      <c r="J2" s="203"/>
+      <c r="K2" s="201" t="s">
         <v>652</v>
       </c>
-      <c r="L2" s="197"/>
-      <c r="M2" s="197"/>
-      <c r="N2" s="198"/>
-      <c r="O2" s="196" t="s">
+      <c r="L2" s="202"/>
+      <c r="M2" s="202"/>
+      <c r="N2" s="203"/>
+      <c r="O2" s="201" t="s">
         <v>653</v>
       </c>
-      <c r="P2" s="197"/>
-      <c r="Q2" s="197"/>
-      <c r="R2" s="198"/>
-      <c r="S2" s="196" t="s">
+      <c r="P2" s="202"/>
+      <c r="Q2" s="202"/>
+      <c r="R2" s="203"/>
+      <c r="S2" s="201" t="s">
         <v>654</v>
       </c>
-      <c r="T2" s="197"/>
-      <c r="U2" s="197"/>
-      <c r="V2" s="206"/>
-      <c r="W2" s="196" t="s">
+      <c r="T2" s="202"/>
+      <c r="U2" s="202"/>
+      <c r="V2" s="204"/>
+      <c r="W2" s="201" t="s">
         <v>655</v>
       </c>
-      <c r="X2" s="197"/>
-      <c r="Y2" s="197"/>
-      <c r="Z2" s="206"/>
-      <c r="AA2" s="203" t="s">
+      <c r="X2" s="202"/>
+      <c r="Y2" s="202"/>
+      <c r="Z2" s="204"/>
+      <c r="AA2" s="198" t="s">
         <v>656</v>
       </c>
-      <c r="AB2" s="204"/>
-      <c r="AC2" s="204"/>
-      <c r="AD2" s="205"/>
-      <c r="AE2" s="203" t="s">
+      <c r="AB2" s="199"/>
+      <c r="AC2" s="199"/>
+      <c r="AD2" s="200"/>
+      <c r="AE2" s="198" t="s">
         <v>657</v>
       </c>
-      <c r="AF2" s="204"/>
-      <c r="AG2" s="204"/>
-      <c r="AH2" s="205"/>
-      <c r="AI2" s="203" t="s">
+      <c r="AF2" s="199"/>
+      <c r="AG2" s="199"/>
+      <c r="AH2" s="200"/>
+      <c r="AI2" s="198" t="s">
         <v>658</v>
       </c>
-      <c r="AJ2" s="204"/>
-      <c r="AK2" s="204"/>
-      <c r="AL2" s="205"/>
-      <c r="AM2" s="203" t="s">
+      <c r="AJ2" s="199"/>
+      <c r="AK2" s="199"/>
+      <c r="AL2" s="200"/>
+      <c r="AM2" s="198" t="s">
         <v>659</v>
       </c>
-      <c r="AN2" s="204"/>
-      <c r="AO2" s="204"/>
-      <c r="AP2" s="205"/>
-      <c r="AQ2" s="203" t="s">
+      <c r="AN2" s="199"/>
+      <c r="AO2" s="199"/>
+      <c r="AP2" s="200"/>
+      <c r="AQ2" s="198" t="s">
         <v>660</v>
       </c>
-      <c r="AR2" s="204"/>
-      <c r="AS2" s="204"/>
-      <c r="AT2" s="205"/>
-      <c r="AU2" s="203" t="s">
+      <c r="AR2" s="199"/>
+      <c r="AS2" s="199"/>
+      <c r="AT2" s="200"/>
+      <c r="AU2" s="198" t="s">
         <v>722</v>
       </c>
-      <c r="AV2" s="204"/>
-      <c r="AW2" s="204"/>
-      <c r="AX2" s="205"/>
-      <c r="AY2" s="203" t="s">
+      <c r="AV2" s="199"/>
+      <c r="AW2" s="199"/>
+      <c r="AX2" s="200"/>
+      <c r="AY2" s="198" t="s">
         <v>729</v>
       </c>
-      <c r="AZ2" s="204"/>
-      <c r="BA2" s="204"/>
-      <c r="BB2" s="205"/>
+      <c r="AZ2" s="199"/>
+      <c r="BA2" s="199"/>
+      <c r="BB2" s="200"/>
     </row>
     <row r="3" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
-      <c r="C3" s="200"/>
-      <c r="D3" s="200"/>
-      <c r="E3" s="200"/>
-      <c r="F3" s="202"/>
+      <c r="C3" s="206"/>
+      <c r="D3" s="206"/>
+      <c r="E3" s="206"/>
+      <c r="F3" s="208"/>
       <c r="G3" s="80">
         <v>1</v>
       </c>
@@ -40450,11 +40451,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="O2:R2"/>
     <mergeCell ref="AU2:AX2"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="AY2:BB2"/>
@@ -40466,6 +40462,11 @@
     <mergeCell ref="AM2:AP2"/>
     <mergeCell ref="AQ2:AT2"/>
     <mergeCell ref="S2:V2"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="O2:R2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E84" location="ลูกค้า!A1" display="ลูกค้า!A1"/>
@@ -40653,38 +40654,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="213" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="199" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="215" t="s">
+      <c r="A1" s="215" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="205" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="217" t="s">
         <v>651</v>
       </c>
-      <c r="D1" s="215"/>
-      <c r="E1" s="215"/>
-      <c r="F1" s="212"/>
-      <c r="G1" s="215" t="s">
+      <c r="D1" s="217"/>
+      <c r="E1" s="217"/>
+      <c r="F1" s="214"/>
+      <c r="G1" s="217" t="s">
         <v>730</v>
       </c>
-      <c r="H1" s="215"/>
-      <c r="I1" s="215"/>
-      <c r="J1" s="212"/>
-      <c r="K1" s="215" t="s">
+      <c r="H1" s="217"/>
+      <c r="I1" s="217"/>
+      <c r="J1" s="214"/>
+      <c r="K1" s="217" t="s">
         <v>653</v>
       </c>
-      <c r="L1" s="215"/>
-      <c r="M1" s="215"/>
-      <c r="N1" s="212"/>
-      <c r="O1" s="211" t="s">
+      <c r="L1" s="217"/>
+      <c r="M1" s="217"/>
+      <c r="N1" s="214"/>
+      <c r="O1" s="213" t="s">
         <v>731</v>
       </c>
-      <c r="P1" s="212"/>
+      <c r="P1" s="214"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="214"/>
-      <c r="B2" s="200"/>
+      <c r="A2" s="216"/>
+      <c r="B2" s="206"/>
       <c r="C2" s="1">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
ref to po edit wrong
</commit_message>
<xml_diff>
--- a/_Doc/Feature.xlsx
+++ b/_Doc/Feature.xlsx
@@ -57,7 +57,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Menu!$A$1:$R$57</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -227,7 +227,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2561" uniqueCount="1826">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2564" uniqueCount="1829">
   <si>
     <t>No.</t>
   </si>
@@ -6136,13 +6136,22 @@
   <si>
     <t xml:space="preserve"> update note set seq=noteid;</t>
   </si>
+  <si>
+    <t>เพิ่มหมายเหตุ เพื่อพิมพ์ในเอกสารต่อท้ายรายการสินค้า</t>
+  </si>
+  <si>
+    <t>แก้ไขใบสั่งซื้อ แล้วใบสั่งจองกลับมาสถานะผิด</t>
+  </si>
+  <si>
+    <t>1.0.1.05</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="48" x14ac:knownFonts="1">
     <font>
@@ -6767,7 +6776,7 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
@@ -6851,20 +6860,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="6" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="1" fillId="6" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
@@ -7032,11 +7041,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="29" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="14" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -7130,6 +7139,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -7137,6 +7155,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -7150,18 +7171,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -8072,20 +8081,20 @@
       <c r="B1" s="2"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="201" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="201" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="201" t="s">
+      <c r="A2" s="205" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="205" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="205" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="202"/>
-      <c r="B3" s="202"/>
-      <c r="C3" s="202"/>
+      <c r="A3" s="206"/>
+      <c r="B3" s="206"/>
+      <c r="C3" s="206"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
@@ -9287,12 +9296,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
     <mergeCell ref="B43:C43"/>
     <mergeCell ref="B44:C44"/>
     <mergeCell ref="B45:C45"/>
@@ -9303,6 +9306,12 @@
     <mergeCell ref="B40:C40"/>
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -11230,7 +11239,7 @@
   <dimension ref="A1:C476"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A422" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C432" sqref="C432"/>
+      <selection activeCell="C434" sqref="C434:C435"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21.75" x14ac:dyDescent="0.5"/>
@@ -13746,11 +13755,20 @@
       <c r="C433" s="185"/>
     </row>
     <row r="434" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A434" s="151" t="s">
+        <v>1828</v>
+      </c>
+      <c r="B434" s="151" t="s">
+        <v>1826</v>
+      </c>
       <c r="C434" s="185" t="s">
         <v>1824</v>
       </c>
     </row>
     <row r="435" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="B435" s="151" t="s">
+        <v>1827</v>
+      </c>
       <c r="C435" s="185" t="s">
         <v>1825</v>
       </c>
@@ -22823,97 +22841,97 @@
     </row>
     <row r="2" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
-      <c r="B2" s="201" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="201" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="201" t="s">
+      <c r="B2" s="205" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="205" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="205" t="s">
         <v>130</v>
       </c>
-      <c r="E2" s="203" t="s">
+      <c r="E2" s="207" t="s">
         <v>723</v>
       </c>
-      <c r="F2" s="198" t="s">
+      <c r="F2" s="201" t="s">
         <v>651</v>
       </c>
-      <c r="G2" s="199"/>
-      <c r="H2" s="199"/>
-      <c r="I2" s="200"/>
-      <c r="J2" s="198" t="s">
+      <c r="G2" s="202"/>
+      <c r="H2" s="202"/>
+      <c r="I2" s="203"/>
+      <c r="J2" s="201" t="s">
         <v>652</v>
       </c>
-      <c r="K2" s="199"/>
-      <c r="L2" s="199"/>
-      <c r="M2" s="200"/>
-      <c r="N2" s="198" t="s">
+      <c r="K2" s="202"/>
+      <c r="L2" s="202"/>
+      <c r="M2" s="203"/>
+      <c r="N2" s="201" t="s">
         <v>653</v>
       </c>
-      <c r="O2" s="199"/>
-      <c r="P2" s="199"/>
-      <c r="Q2" s="200"/>
-      <c r="R2" s="198" t="s">
+      <c r="O2" s="202"/>
+      <c r="P2" s="202"/>
+      <c r="Q2" s="203"/>
+      <c r="R2" s="201" t="s">
         <v>654</v>
       </c>
-      <c r="S2" s="199"/>
-      <c r="T2" s="199"/>
-      <c r="U2" s="208"/>
-      <c r="V2" s="198" t="s">
+      <c r="S2" s="202"/>
+      <c r="T2" s="202"/>
+      <c r="U2" s="204"/>
+      <c r="V2" s="201" t="s">
         <v>655</v>
       </c>
-      <c r="W2" s="199"/>
-      <c r="X2" s="199"/>
-      <c r="Y2" s="208"/>
-      <c r="Z2" s="205" t="s">
+      <c r="W2" s="202"/>
+      <c r="X2" s="202"/>
+      <c r="Y2" s="204"/>
+      <c r="Z2" s="198" t="s">
         <v>656</v>
       </c>
-      <c r="AA2" s="206"/>
-      <c r="AB2" s="206"/>
-      <c r="AC2" s="207"/>
-      <c r="AD2" s="205" t="s">
+      <c r="AA2" s="199"/>
+      <c r="AB2" s="199"/>
+      <c r="AC2" s="200"/>
+      <c r="AD2" s="198" t="s">
         <v>657</v>
       </c>
-      <c r="AE2" s="206"/>
-      <c r="AF2" s="206"/>
-      <c r="AG2" s="207"/>
-      <c r="AH2" s="205" t="s">
+      <c r="AE2" s="199"/>
+      <c r="AF2" s="199"/>
+      <c r="AG2" s="200"/>
+      <c r="AH2" s="198" t="s">
         <v>658</v>
       </c>
-      <c r="AI2" s="206"/>
-      <c r="AJ2" s="206"/>
-      <c r="AK2" s="207"/>
-      <c r="AL2" s="205" t="s">
+      <c r="AI2" s="199"/>
+      <c r="AJ2" s="199"/>
+      <c r="AK2" s="200"/>
+      <c r="AL2" s="198" t="s">
         <v>659</v>
       </c>
-      <c r="AM2" s="206"/>
-      <c r="AN2" s="206"/>
-      <c r="AO2" s="207"/>
-      <c r="AP2" s="205" t="s">
+      <c r="AM2" s="199"/>
+      <c r="AN2" s="199"/>
+      <c r="AO2" s="200"/>
+      <c r="AP2" s="198" t="s">
         <v>660</v>
       </c>
-      <c r="AQ2" s="206"/>
-      <c r="AR2" s="206"/>
-      <c r="AS2" s="207"/>
-      <c r="AT2" s="205" t="s">
+      <c r="AQ2" s="199"/>
+      <c r="AR2" s="199"/>
+      <c r="AS2" s="200"/>
+      <c r="AT2" s="198" t="s">
         <v>722</v>
       </c>
-      <c r="AU2" s="206"/>
-      <c r="AV2" s="206"/>
-      <c r="AW2" s="207"/>
-      <c r="AX2" s="205" t="s">
+      <c r="AU2" s="199"/>
+      <c r="AV2" s="199"/>
+      <c r="AW2" s="200"/>
+      <c r="AX2" s="198" t="s">
         <v>729</v>
       </c>
-      <c r="AY2" s="206"/>
-      <c r="AZ2" s="206"/>
-      <c r="BA2" s="207"/>
+      <c r="AY2" s="199"/>
+      <c r="AZ2" s="199"/>
+      <c r="BA2" s="200"/>
     </row>
     <row r="3" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
-      <c r="B3" s="202"/>
-      <c r="C3" s="202"/>
-      <c r="D3" s="202"/>
-      <c r="E3" s="204"/>
+      <c r="B3" s="206"/>
+      <c r="C3" s="206"/>
+      <c r="D3" s="206"/>
+      <c r="E3" s="208"/>
       <c r="F3" s="80">
         <v>1</v>
       </c>
@@ -28067,6 +28085,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:I2"/>
     <mergeCell ref="AL2:AO2"/>
     <mergeCell ref="AP2:AS2"/>
     <mergeCell ref="AT2:AW2"/>
@@ -28077,12 +28101,6 @@
     <mergeCell ref="Z2:AC2"/>
     <mergeCell ref="AD2:AG2"/>
     <mergeCell ref="AH2:AK2"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:I2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D84" location="ลูกค้า!A1" display="ลูกค้า!A1"/>
@@ -28600,16 +28618,16 @@
     <row r="2" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
-      <c r="C2" s="201" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="201" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="201" t="s">
+      <c r="C2" s="205" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="205" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="205" t="s">
         <v>130</v>
       </c>
-      <c r="F2" s="203" t="s">
+      <c r="F2" s="207" t="s">
         <v>723</v>
       </c>
       <c r="G2" s="209" t="s">
@@ -28676,10 +28694,10 @@
     <row r="3" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
-      <c r="C3" s="202"/>
-      <c r="D3" s="202"/>
-      <c r="E3" s="202"/>
-      <c r="F3" s="204"/>
+      <c r="C3" s="206"/>
+      <c r="D3" s="206"/>
+      <c r="E3" s="206"/>
+      <c r="F3" s="208"/>
       <c r="G3" s="80">
         <v>1</v>
       </c>
@@ -34475,6 +34493,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="AE2:AH2"/>
+    <mergeCell ref="AI2:AL2"/>
+    <mergeCell ref="AM2:AP2"/>
+    <mergeCell ref="AQ2:AT2"/>
+    <mergeCell ref="AA2:AD2"/>
     <mergeCell ref="K2:N2"/>
     <mergeCell ref="O2:R2"/>
     <mergeCell ref="S2:V2"/>
@@ -34484,11 +34507,6 @@
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="G2:J2"/>
-    <mergeCell ref="AE2:AH2"/>
-    <mergeCell ref="AI2:AL2"/>
-    <mergeCell ref="AM2:AP2"/>
-    <mergeCell ref="AQ2:AT2"/>
-    <mergeCell ref="AA2:AD2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E84" location="ลูกค้า!A1" display="ลูกค้า!A1"/>
@@ -34966,98 +34984,98 @@
     <row r="2" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
-      <c r="C2" s="201" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="201" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="201" t="s">
+      <c r="C2" s="205" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="205" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="205" t="s">
         <v>130</v>
       </c>
-      <c r="F2" s="203" t="s">
+      <c r="F2" s="207" t="s">
         <v>723</v>
       </c>
-      <c r="G2" s="198" t="s">
+      <c r="G2" s="201" t="s">
         <v>651</v>
       </c>
-      <c r="H2" s="199"/>
-      <c r="I2" s="199"/>
-      <c r="J2" s="200"/>
-      <c r="K2" s="198" t="s">
+      <c r="H2" s="202"/>
+      <c r="I2" s="202"/>
+      <c r="J2" s="203"/>
+      <c r="K2" s="201" t="s">
         <v>652</v>
       </c>
-      <c r="L2" s="199"/>
-      <c r="M2" s="199"/>
-      <c r="N2" s="200"/>
-      <c r="O2" s="198" t="s">
+      <c r="L2" s="202"/>
+      <c r="M2" s="202"/>
+      <c r="N2" s="203"/>
+      <c r="O2" s="201" t="s">
         <v>653</v>
       </c>
-      <c r="P2" s="199"/>
-      <c r="Q2" s="199"/>
-      <c r="R2" s="200"/>
-      <c r="S2" s="198" t="s">
+      <c r="P2" s="202"/>
+      <c r="Q2" s="202"/>
+      <c r="R2" s="203"/>
+      <c r="S2" s="201" t="s">
         <v>654</v>
       </c>
-      <c r="T2" s="199"/>
-      <c r="U2" s="199"/>
-      <c r="V2" s="208"/>
-      <c r="W2" s="198" t="s">
+      <c r="T2" s="202"/>
+      <c r="U2" s="202"/>
+      <c r="V2" s="204"/>
+      <c r="W2" s="201" t="s">
         <v>655</v>
       </c>
-      <c r="X2" s="199"/>
-      <c r="Y2" s="199"/>
-      <c r="Z2" s="208"/>
-      <c r="AA2" s="205" t="s">
+      <c r="X2" s="202"/>
+      <c r="Y2" s="202"/>
+      <c r="Z2" s="204"/>
+      <c r="AA2" s="198" t="s">
         <v>656</v>
       </c>
-      <c r="AB2" s="206"/>
-      <c r="AC2" s="206"/>
-      <c r="AD2" s="207"/>
-      <c r="AE2" s="205" t="s">
+      <c r="AB2" s="199"/>
+      <c r="AC2" s="199"/>
+      <c r="AD2" s="200"/>
+      <c r="AE2" s="198" t="s">
         <v>657</v>
       </c>
-      <c r="AF2" s="206"/>
-      <c r="AG2" s="206"/>
-      <c r="AH2" s="207"/>
-      <c r="AI2" s="205" t="s">
+      <c r="AF2" s="199"/>
+      <c r="AG2" s="199"/>
+      <c r="AH2" s="200"/>
+      <c r="AI2" s="198" t="s">
         <v>658</v>
       </c>
-      <c r="AJ2" s="206"/>
-      <c r="AK2" s="206"/>
-      <c r="AL2" s="207"/>
-      <c r="AM2" s="205" t="s">
+      <c r="AJ2" s="199"/>
+      <c r="AK2" s="199"/>
+      <c r="AL2" s="200"/>
+      <c r="AM2" s="198" t="s">
         <v>659</v>
       </c>
-      <c r="AN2" s="206"/>
-      <c r="AO2" s="206"/>
-      <c r="AP2" s="207"/>
-      <c r="AQ2" s="205" t="s">
+      <c r="AN2" s="199"/>
+      <c r="AO2" s="199"/>
+      <c r="AP2" s="200"/>
+      <c r="AQ2" s="198" t="s">
         <v>660</v>
       </c>
-      <c r="AR2" s="206"/>
-      <c r="AS2" s="206"/>
-      <c r="AT2" s="207"/>
-      <c r="AU2" s="205" t="s">
+      <c r="AR2" s="199"/>
+      <c r="AS2" s="199"/>
+      <c r="AT2" s="200"/>
+      <c r="AU2" s="198" t="s">
         <v>722</v>
       </c>
-      <c r="AV2" s="206"/>
-      <c r="AW2" s="206"/>
-      <c r="AX2" s="207"/>
-      <c r="AY2" s="205" t="s">
+      <c r="AV2" s="199"/>
+      <c r="AW2" s="199"/>
+      <c r="AX2" s="200"/>
+      <c r="AY2" s="198" t="s">
         <v>729</v>
       </c>
-      <c r="AZ2" s="206"/>
-      <c r="BA2" s="206"/>
-      <c r="BB2" s="207"/>
+      <c r="AZ2" s="199"/>
+      <c r="BA2" s="199"/>
+      <c r="BB2" s="200"/>
     </row>
     <row r="3" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
-      <c r="C3" s="202"/>
-      <c r="D3" s="202"/>
-      <c r="E3" s="202"/>
-      <c r="F3" s="204"/>
+      <c r="C3" s="206"/>
+      <c r="D3" s="206"/>
+      <c r="E3" s="206"/>
+      <c r="F3" s="208"/>
       <c r="G3" s="80">
         <v>1</v>
       </c>
@@ -40470,11 +40488,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="O2:R2"/>
     <mergeCell ref="AU2:AX2"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="AY2:BB2"/>
@@ -40486,6 +40499,11 @@
     <mergeCell ref="AM2:AP2"/>
     <mergeCell ref="AQ2:AT2"/>
     <mergeCell ref="S2:V2"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="O2:R2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E84" location="ลูกค้า!A1" display="ลูกค้า!A1"/>
@@ -40676,7 +40694,7 @@
       <c r="A1" s="215" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="201" t="s">
+      <c r="B1" s="205" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="217" t="s">
@@ -40704,7 +40722,7 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="216"/>
-      <c r="B2" s="202"/>
+      <c r="B2" s="206"/>
       <c r="C2" s="1">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
sell hist. report can not select product
</commit_message>
<xml_diff>
--- a/_Doc/Feature.xlsx
+++ b/_Doc/Feature.xlsx
@@ -57,7 +57,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Menu!$A$1:$R$57</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -227,7 +227,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2564" uniqueCount="1829">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2566" uniqueCount="1831">
   <si>
     <t>No.</t>
   </si>
@@ -6145,13 +6145,19 @@
   <si>
     <t>1.0.1.05</t>
   </si>
+  <si>
+    <t>1.0.1.06</t>
+  </si>
+  <si>
+    <t>หน้าประวัติขายเลือกสินค้าไม่ได้</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="48" x14ac:knownFonts="1">
     <font>
@@ -6776,7 +6782,7 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
@@ -6860,20 +6866,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="1" fillId="6" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
@@ -7041,11 +7047,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="43" fontId="29" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="43" fontId="14" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -7317,13 +7323,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>95251</xdr:colOff>
-      <xdr:row>468</xdr:row>
+      <xdr:row>470</xdr:row>
       <xdr:rowOff>143542</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>160787</xdr:colOff>
-      <xdr:row>477</xdr:row>
+      <xdr:row>479</xdr:row>
       <xdr:rowOff>210818</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -7343,6 +7349,82 @@
         <a:xfrm>
           <a:off x="7229476" y="136084342"/>
           <a:ext cx="7475986" cy="5591776"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2709334</xdr:colOff>
+      <xdr:row>436</xdr:row>
+      <xdr:rowOff>21167</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>530858</xdr:colOff>
+      <xdr:row>450</xdr:row>
+      <xdr:rowOff>273595</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7863417" y="130270250"/>
+          <a:ext cx="3409524" cy="4104762"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2614084</xdr:colOff>
+      <xdr:row>451</xdr:row>
+      <xdr:rowOff>21167</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>502275</xdr:colOff>
+      <xdr:row>463</xdr:row>
+      <xdr:rowOff>309643</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7768167" y="134397750"/>
+          <a:ext cx="3476191" cy="3590476"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -11236,10 +11318,10 @@
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
-  <dimension ref="A1:C476"/>
+  <dimension ref="A1:C478"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A422" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C434" sqref="C434:C435"/>
+    <sheetView tabSelected="1" topLeftCell="A446" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I455" sqref="I455"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21.75" x14ac:dyDescent="0.5"/>
@@ -13777,173 +13859,185 @@
       <c r="C436" s="185"/>
     </row>
     <row r="437" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="B437" s="192" t="s">
-        <v>1721</v>
+      <c r="A437" s="151" t="s">
+        <v>1829</v>
+      </c>
+      <c r="B437" s="151" t="s">
+        <v>1830</v>
       </c>
       <c r="C437" s="185"/>
     </row>
     <row r="438" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="B438" s="192" t="s">
-        <v>1722</v>
-      </c>
       <c r="C438" s="185"/>
     </row>
     <row r="439" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B439" s="192" t="s">
-        <v>1723</v>
+        <v>1721</v>
       </c>
       <c r="C439" s="185"/>
     </row>
     <row r="440" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="B440" s="151" t="s">
-        <v>1724</v>
+      <c r="B440" s="192" t="s">
+        <v>1722</v>
       </c>
       <c r="C440" s="185"/>
     </row>
     <row r="441" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B441" s="192" t="s">
+        <v>1723</v>
+      </c>
+      <c r="C441" s="185"/>
+    </row>
+    <row r="442" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="B442" s="151" t="s">
+        <v>1724</v>
+      </c>
+      <c r="C442" s="185"/>
+    </row>
+    <row r="443" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="B443" s="192" t="s">
         <v>1733</v>
-      </c>
-      <c r="C441" s="185"/>
-    </row>
-    <row r="442" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="B442" s="192" t="s">
-        <v>1725</v>
-      </c>
-      <c r="C442" s="185"/>
-    </row>
-    <row r="443" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="B443" s="151" t="s">
-        <v>1726</v>
       </c>
       <c r="C443" s="185"/>
     </row>
     <row r="444" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B444" s="192" t="s">
+        <v>1725</v>
+      </c>
+      <c r="C444" s="185"/>
+    </row>
+    <row r="445" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="B445" s="151" t="s">
+        <v>1726</v>
+      </c>
+      <c r="C445" s="185"/>
+    </row>
+    <row r="446" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="B446" s="192" t="s">
         <v>1731</v>
       </c>
-      <c r="C444" s="185"/>
-    </row>
-    <row r="445" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="C445" s="185"/>
-    </row>
-    <row r="446" spans="1:3" x14ac:dyDescent="0.5">
       <c r="C446" s="185"/>
     </row>
     <row r="447" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A447" s="151" t="s">
+      <c r="C447" s="185"/>
+    </row>
+    <row r="448" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="C448" s="185"/>
+    </row>
+    <row r="449" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A449" s="151" t="s">
         <v>1732</v>
       </c>
-      <c r="B447" s="151" t="s">
+      <c r="B449" s="151" t="s">
         <v>1727</v>
       </c>
-      <c r="C447" s="185"/>
-    </row>
-    <row r="448" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="B448" s="192" t="s">
+      <c r="C449" s="185"/>
+    </row>
+    <row r="450" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="B450" s="192" t="s">
         <v>1728</v>
       </c>
-      <c r="C448" s="185"/>
-    </row>
-    <row r="449" spans="2:3" x14ac:dyDescent="0.5">
-      <c r="B449" s="192" t="s">
+      <c r="C450" s="185"/>
+    </row>
+    <row r="451" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="B451" s="192" t="s">
         <v>1729</v>
       </c>
-      <c r="C449" s="185"/>
-    </row>
-    <row r="450" spans="2:3" x14ac:dyDescent="0.5">
-      <c r="B450" s="192" t="s">
+      <c r="C451" s="185"/>
+    </row>
+    <row r="452" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="B452" s="192" t="s">
         <v>1730</v>
       </c>
-      <c r="C450" s="185"/>
-    </row>
-    <row r="451" spans="2:3" x14ac:dyDescent="0.5">
-      <c r="C451" s="185"/>
-    </row>
-    <row r="452" spans="2:3" x14ac:dyDescent="0.5">
       <c r="C452" s="185"/>
     </row>
-    <row r="453" spans="2:3" x14ac:dyDescent="0.5">
+    <row r="453" spans="1:3" x14ac:dyDescent="0.5">
       <c r="C453" s="185"/>
     </row>
-    <row r="454" spans="2:3" x14ac:dyDescent="0.5">
+    <row r="454" spans="1:3" x14ac:dyDescent="0.5">
       <c r="C454" s="185"/>
     </row>
-    <row r="455" spans="2:3" x14ac:dyDescent="0.5">
+    <row r="455" spans="1:3" x14ac:dyDescent="0.5">
       <c r="C455" s="185"/>
     </row>
-    <row r="459" spans="2:3" x14ac:dyDescent="0.5">
-      <c r="B459" s="151" t="s">
+    <row r="456" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="C456" s="185"/>
+    </row>
+    <row r="457" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="C457" s="185"/>
+    </row>
+    <row r="461" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="B461" s="151" t="s">
         <v>1622</v>
       </c>
     </row>
-    <row r="460" spans="2:3" x14ac:dyDescent="0.5">
-      <c r="B460" s="191" t="s">
+    <row r="462" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="B462" s="191" t="s">
         <v>1524</v>
       </c>
     </row>
-    <row r="461" spans="2:3" x14ac:dyDescent="0.5">
-      <c r="B461" s="191" t="s">
+    <row r="463" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="B463" s="191" t="s">
         <v>1623</v>
       </c>
     </row>
-    <row r="462" spans="2:3" ht="87" x14ac:dyDescent="0.5">
-      <c r="B462" s="152" t="s">
+    <row r="464" spans="1:3" ht="87" x14ac:dyDescent="0.5">
+      <c r="B464" s="152" t="s">
         <v>1624</v>
       </c>
     </row>
-    <row r="464" spans="2:3" x14ac:dyDescent="0.5">
-      <c r="B464" s="186" t="s">
+    <row r="466" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B466" s="186" t="s">
         <v>1642</v>
       </c>
     </row>
-    <row r="465" spans="2:2" ht="65.25" x14ac:dyDescent="0.5">
-      <c r="B465" s="187" t="s">
+    <row r="467" spans="2:2" ht="65.25" x14ac:dyDescent="0.5">
+      <c r="B467" s="187" t="s">
         <v>1640</v>
       </c>
     </row>
-    <row r="466" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B466" s="188" t="s">
+    <row r="468" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B468" s="188" t="s">
         <v>1641</v>
       </c>
     </row>
-    <row r="467" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B467" s="189" t="s">
+    <row r="469" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B469" s="189" t="s">
         <v>1643</v>
       </c>
     </row>
-    <row r="468" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B468" s="191" t="s">
+    <row r="470" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B470" s="191" t="s">
         <v>1644</v>
       </c>
     </row>
-    <row r="469" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B469" s="151" t="s">
+    <row r="471" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B471" s="151" t="s">
         <v>1645</v>
       </c>
     </row>
-    <row r="470" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B470" s="186" t="s">
+    <row r="472" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B472" s="186" t="s">
         <v>1646</v>
       </c>
     </row>
-    <row r="471" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B471" s="191" t="s">
+    <row r="473" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B473" s="191" t="s">
         <v>1647</v>
       </c>
     </row>
-    <row r="474" spans="2:2" ht="108.75" x14ac:dyDescent="0.5">
-      <c r="B474" s="152" t="s">
+    <row r="476" spans="2:2" ht="108.75" x14ac:dyDescent="0.5">
+      <c r="B476" s="152" t="s">
         <v>1792</v>
       </c>
     </row>
-    <row r="475" spans="2:2" ht="108.75" x14ac:dyDescent="0.5">
-      <c r="B475" s="152" t="s">
+    <row r="477" spans="2:2" ht="108.75" x14ac:dyDescent="0.5">
+      <c r="B477" s="152" t="s">
         <v>1793</v>
       </c>
     </row>
-    <row r="476" spans="2:2" ht="87" x14ac:dyDescent="0.5">
-      <c r="B476" s="152" t="s">
+    <row r="478" spans="2:2" ht="87" x14ac:dyDescent="0.5">
+      <c r="B478" s="152" t="s">
         <v>1791</v>
       </c>
     </row>

</xml_diff>

<commit_message>
* V.1.0.1.18 @Office *ส่งแล้ว
</commit_message>
<xml_diff>
--- a/_Doc/Feature.xlsx
+++ b/_Doc/Feature.xlsx
@@ -228,7 +228,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2683" uniqueCount="1938">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2682" uniqueCount="1937">
   <si>
     <t>No.</t>
   </si>
@@ -6576,9 +6576,6 @@
   </si>
   <si>
     <t>INSERT INTO  [Menu]([MenuID],[ShowMode],[System],[Module],[MenuName],[MenuDisplay],[TableName],[IsVisible],[IsEnable],[IsAdd],[IsEdit],[IsDelete],[IsPrint],[IsImport],[IsCreateQuick],[IsCopy],[IsAssign],[IsConvert]) VALUES (104,3,'อนุมัติเอกสาร','อนุมัติเอกสาร' ,'NotifyBar','ข้อความแจ้งเตือน' ,'Notify',1 ,1 ,0,0,0,0,0,0,0,0,0);</t>
-  </si>
-  <si>
-    <t>V.1.0.1.19</t>
   </si>
   <si>
     <t>Stockin preview รายการไม่แสดง SN</t>
@@ -7577,15 +7574,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -7593,9 +7581,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -7609,6 +7594,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -8598,7 +8595,7 @@
       <c r="A1" s="215" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="205" t="s">
+      <c r="B1" s="201" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="217" t="s">
@@ -8626,7 +8623,7 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="216"/>
-      <c r="B2" s="206"/>
+      <c r="B2" s="202"/>
       <c r="C2" s="1">
         <v>1</v>
       </c>
@@ -9319,20 +9316,20 @@
       <c r="B1" s="2"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="205" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="205" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="205" t="s">
+      <c r="A2" s="201" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="201" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="201" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="206"/>
-      <c r="B3" s="206"/>
-      <c r="C3" s="206"/>
+      <c r="A3" s="202"/>
+      <c r="B3" s="202"/>
+      <c r="C3" s="202"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
@@ -10534,6 +10531,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
     <mergeCell ref="B43:C43"/>
     <mergeCell ref="B44:C44"/>
     <mergeCell ref="B45:C45"/>
@@ -10544,12 +10547,6 @@
     <mergeCell ref="B40:C40"/>
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -12378,10 +12375,10 @@
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
-  <dimension ref="A1:C521"/>
+  <dimension ref="A1:C522"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A470" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A480" sqref="A480"/>
+    <sheetView tabSelected="1" topLeftCell="A476" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B482" sqref="B482"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21.75" x14ac:dyDescent="0.5"/>
@@ -15177,99 +15174,93 @@
         <v>1934</v>
       </c>
     </row>
-    <row r="480" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A480" s="151" t="s">
+    <row r="479" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="B479" s="151" t="s">
         <v>1936</v>
       </c>
-      <c r="B480" s="151" t="s">
-        <v>1937</v>
-      </c>
-    </row>
-    <row r="481" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="B481" s="120"/>
     </row>
     <row r="482" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="B482" s="192" t="s">
-        <v>1721</v>
-      </c>
-      <c r="C482" s="185"/>
+      <c r="B482" s="120"/>
     </row>
     <row r="483" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B483" s="192" t="s">
-        <v>1722</v>
+        <v>1721</v>
       </c>
       <c r="C483" s="185"/>
     </row>
     <row r="484" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B484" s="192" t="s">
+        <v>1722</v>
+      </c>
+      <c r="C484" s="185"/>
+    </row>
+    <row r="485" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="B485" s="192" t="s">
         <v>1723</v>
       </c>
-      <c r="C484" s="185"/>
-    </row>
-    <row r="485" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="B485" s="151" t="s">
+      <c r="C485" s="185"/>
+    </row>
+    <row r="486" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="B486" s="151" t="s">
         <v>1724</v>
-      </c>
-      <c r="C485" s="185"/>
-    </row>
-    <row r="486" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="B486" s="192" t="s">
-        <v>1733</v>
       </c>
       <c r="C486" s="185"/>
     </row>
     <row r="487" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B487" s="192" t="s">
+        <v>1733</v>
+      </c>
+      <c r="C487" s="185"/>
+    </row>
+    <row r="488" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="B488" s="192" t="s">
         <v>1725</v>
       </c>
-      <c r="C487" s="185"/>
-    </row>
-    <row r="488" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="B488" s="151" t="s">
+      <c r="C488" s="185"/>
+    </row>
+    <row r="489" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="B489" s="151" t="s">
         <v>1726</v>
       </c>
-      <c r="C488" s="185"/>
-    </row>
-    <row r="489" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="B489" s="192" t="s">
+      <c r="C489" s="185"/>
+    </row>
+    <row r="490" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="B490" s="192" t="s">
         <v>1731</v>
       </c>
-      <c r="C489" s="185"/>
-    </row>
-    <row r="490" spans="1:3" x14ac:dyDescent="0.5">
       <c r="C490" s="185"/>
     </row>
     <row r="491" spans="1:3" x14ac:dyDescent="0.5">
       <c r="C491" s="185"/>
     </row>
     <row r="492" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A492" s="151" t="s">
+      <c r="C492" s="185"/>
+    </row>
+    <row r="493" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A493" s="151" t="s">
         <v>1732</v>
       </c>
-      <c r="B492" s="151" t="s">
+      <c r="B493" s="151" t="s">
         <v>1727</v>
-      </c>
-      <c r="C492" s="185"/>
-    </row>
-    <row r="493" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="B493" s="192" t="s">
-        <v>1728</v>
       </c>
       <c r="C493" s="185"/>
     </row>
     <row r="494" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B494" s="192" t="s">
-        <v>1729</v>
+        <v>1728</v>
       </c>
       <c r="C494" s="185"/>
     </row>
     <row r="495" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B495" s="192" t="s">
+        <v>1729</v>
+      </c>
+      <c r="C495" s="185"/>
+    </row>
+    <row r="496" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="B496" s="192" t="s">
         <v>1730</v>
       </c>
-      <c r="C495" s="185"/>
-    </row>
-    <row r="496" spans="1:3" x14ac:dyDescent="0.5">
       <c r="C496" s="185"/>
     </row>
     <row r="497" spans="2:3" x14ac:dyDescent="0.5">
@@ -15284,78 +15275,81 @@
     <row r="500" spans="2:3" x14ac:dyDescent="0.5">
       <c r="C500" s="185"/>
     </row>
-    <row r="504" spans="2:3" x14ac:dyDescent="0.5">
-      <c r="B504" s="151" t="s">
+    <row r="501" spans="2:3" x14ac:dyDescent="0.5">
+      <c r="C501" s="185"/>
+    </row>
+    <row r="505" spans="2:3" x14ac:dyDescent="0.5">
+      <c r="B505" s="151" t="s">
         <v>1622</v>
-      </c>
-    </row>
-    <row r="505" spans="2:3" x14ac:dyDescent="0.5">
-      <c r="B505" s="191" t="s">
-        <v>1524</v>
       </c>
     </row>
     <row r="506" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B506" s="191" t="s">
+        <v>1524</v>
+      </c>
+    </row>
+    <row r="507" spans="2:3" x14ac:dyDescent="0.5">
+      <c r="B507" s="191" t="s">
         <v>1623</v>
       </c>
     </row>
-    <row r="507" spans="2:3" ht="87" x14ac:dyDescent="0.5">
-      <c r="B507" s="152" t="s">
+    <row r="508" spans="2:3" ht="87" x14ac:dyDescent="0.5">
+      <c r="B508" s="152" t="s">
         <v>1624</v>
       </c>
     </row>
-    <row r="509" spans="2:3" x14ac:dyDescent="0.5">
-      <c r="B509" s="186" t="s">
+    <row r="510" spans="2:3" x14ac:dyDescent="0.5">
+      <c r="B510" s="186" t="s">
         <v>1642</v>
       </c>
     </row>
-    <row r="510" spans="2:3" ht="65.25" x14ac:dyDescent="0.5">
-      <c r="B510" s="187" t="s">
+    <row r="511" spans="2:3" ht="65.25" x14ac:dyDescent="0.5">
+      <c r="B511" s="187" t="s">
         <v>1640</v>
       </c>
     </row>
-    <row r="511" spans="2:3" x14ac:dyDescent="0.5">
-      <c r="B511" s="188" t="s">
+    <row r="512" spans="2:3" x14ac:dyDescent="0.5">
+      <c r="B512" s="188" t="s">
         <v>1641</v>
       </c>
     </row>
-    <row r="512" spans="2:3" x14ac:dyDescent="0.5">
-      <c r="B512" s="189" t="s">
+    <row r="513" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B513" s="189" t="s">
         <v>1643</v>
       </c>
     </row>
-    <row r="513" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B513" s="191" t="s">
+    <row r="514" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B514" s="191" t="s">
         <v>1644</v>
       </c>
     </row>
-    <row r="514" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B514" s="151" t="s">
+    <row r="515" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B515" s="151" t="s">
         <v>1645</v>
       </c>
     </row>
-    <row r="515" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B515" s="186" t="s">
+    <row r="516" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B516" s="186" t="s">
         <v>1646</v>
       </c>
     </row>
-    <row r="516" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B516" s="191" t="s">
+    <row r="517" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B517" s="191" t="s">
         <v>1647</v>
-      </c>
-    </row>
-    <row r="519" spans="2:2" ht="108.75" x14ac:dyDescent="0.5">
-      <c r="B519" s="152" t="s">
-        <v>1792</v>
       </c>
     </row>
     <row r="520" spans="2:2" ht="108.75" x14ac:dyDescent="0.5">
       <c r="B520" s="152" t="s">
+        <v>1792</v>
+      </c>
+    </row>
+    <row r="521" spans="2:2" ht="108.75" x14ac:dyDescent="0.5">
+      <c r="B521" s="152" t="s">
         <v>1793</v>
       </c>
     </row>
-    <row r="521" spans="2:2" ht="87" x14ac:dyDescent="0.5">
-      <c r="B521" s="152" t="s">
+    <row r="522" spans="2:2" ht="87" x14ac:dyDescent="0.5">
+      <c r="B522" s="152" t="s">
         <v>1791</v>
       </c>
     </row>
@@ -25217,97 +25211,97 @@
     </row>
     <row r="2" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
-      <c r="B2" s="205" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="205" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="205" t="s">
+      <c r="B2" s="201" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="201" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="201" t="s">
         <v>130</v>
       </c>
-      <c r="E2" s="207" t="s">
+      <c r="E2" s="203" t="s">
         <v>723</v>
       </c>
-      <c r="F2" s="201" t="s">
+      <c r="F2" s="198" t="s">
         <v>651</v>
       </c>
-      <c r="G2" s="202"/>
-      <c r="H2" s="202"/>
-      <c r="I2" s="203"/>
-      <c r="J2" s="201" t="s">
+      <c r="G2" s="199"/>
+      <c r="H2" s="199"/>
+      <c r="I2" s="200"/>
+      <c r="J2" s="198" t="s">
         <v>652</v>
       </c>
-      <c r="K2" s="202"/>
-      <c r="L2" s="202"/>
-      <c r="M2" s="203"/>
-      <c r="N2" s="201" t="s">
+      <c r="K2" s="199"/>
+      <c r="L2" s="199"/>
+      <c r="M2" s="200"/>
+      <c r="N2" s="198" t="s">
         <v>653</v>
       </c>
-      <c r="O2" s="202"/>
-      <c r="P2" s="202"/>
-      <c r="Q2" s="203"/>
-      <c r="R2" s="201" t="s">
+      <c r="O2" s="199"/>
+      <c r="P2" s="199"/>
+      <c r="Q2" s="200"/>
+      <c r="R2" s="198" t="s">
         <v>654</v>
       </c>
-      <c r="S2" s="202"/>
-      <c r="T2" s="202"/>
-      <c r="U2" s="204"/>
-      <c r="V2" s="201" t="s">
+      <c r="S2" s="199"/>
+      <c r="T2" s="199"/>
+      <c r="U2" s="208"/>
+      <c r="V2" s="198" t="s">
         <v>655</v>
       </c>
-      <c r="W2" s="202"/>
-      <c r="X2" s="202"/>
-      <c r="Y2" s="204"/>
-      <c r="Z2" s="198" t="s">
+      <c r="W2" s="199"/>
+      <c r="X2" s="199"/>
+      <c r="Y2" s="208"/>
+      <c r="Z2" s="205" t="s">
         <v>656</v>
       </c>
-      <c r="AA2" s="199"/>
-      <c r="AB2" s="199"/>
-      <c r="AC2" s="200"/>
-      <c r="AD2" s="198" t="s">
+      <c r="AA2" s="206"/>
+      <c r="AB2" s="206"/>
+      <c r="AC2" s="207"/>
+      <c r="AD2" s="205" t="s">
         <v>657</v>
       </c>
-      <c r="AE2" s="199"/>
-      <c r="AF2" s="199"/>
-      <c r="AG2" s="200"/>
-      <c r="AH2" s="198" t="s">
+      <c r="AE2" s="206"/>
+      <c r="AF2" s="206"/>
+      <c r="AG2" s="207"/>
+      <c r="AH2" s="205" t="s">
         <v>658</v>
       </c>
-      <c r="AI2" s="199"/>
-      <c r="AJ2" s="199"/>
-      <c r="AK2" s="200"/>
-      <c r="AL2" s="198" t="s">
+      <c r="AI2" s="206"/>
+      <c r="AJ2" s="206"/>
+      <c r="AK2" s="207"/>
+      <c r="AL2" s="205" t="s">
         <v>659</v>
       </c>
-      <c r="AM2" s="199"/>
-      <c r="AN2" s="199"/>
-      <c r="AO2" s="200"/>
-      <c r="AP2" s="198" t="s">
+      <c r="AM2" s="206"/>
+      <c r="AN2" s="206"/>
+      <c r="AO2" s="207"/>
+      <c r="AP2" s="205" t="s">
         <v>660</v>
       </c>
-      <c r="AQ2" s="199"/>
-      <c r="AR2" s="199"/>
-      <c r="AS2" s="200"/>
-      <c r="AT2" s="198" t="s">
+      <c r="AQ2" s="206"/>
+      <c r="AR2" s="206"/>
+      <c r="AS2" s="207"/>
+      <c r="AT2" s="205" t="s">
         <v>722</v>
       </c>
-      <c r="AU2" s="199"/>
-      <c r="AV2" s="199"/>
-      <c r="AW2" s="200"/>
-      <c r="AX2" s="198" t="s">
+      <c r="AU2" s="206"/>
+      <c r="AV2" s="206"/>
+      <c r="AW2" s="207"/>
+      <c r="AX2" s="205" t="s">
         <v>729</v>
       </c>
-      <c r="AY2" s="199"/>
-      <c r="AZ2" s="199"/>
-      <c r="BA2" s="200"/>
+      <c r="AY2" s="206"/>
+      <c r="AZ2" s="206"/>
+      <c r="BA2" s="207"/>
     </row>
     <row r="3" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
-      <c r="B3" s="206"/>
-      <c r="C3" s="206"/>
-      <c r="D3" s="206"/>
-      <c r="E3" s="208"/>
+      <c r="B3" s="202"/>
+      <c r="C3" s="202"/>
+      <c r="D3" s="202"/>
+      <c r="E3" s="204"/>
       <c r="F3" s="80">
         <v>1</v>
       </c>
@@ -30461,12 +30455,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:I2"/>
     <mergeCell ref="AL2:AO2"/>
     <mergeCell ref="AP2:AS2"/>
     <mergeCell ref="AT2:AW2"/>
@@ -30477,6 +30465,12 @@
     <mergeCell ref="Z2:AC2"/>
     <mergeCell ref="AD2:AG2"/>
     <mergeCell ref="AH2:AK2"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:I2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D84" location="ลูกค้า!A1" display="ลูกค้า!A1"/>
@@ -30994,16 +30988,16 @@
     <row r="2" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
-      <c r="C2" s="205" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="205" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="205" t="s">
+      <c r="C2" s="201" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="201" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="201" t="s">
         <v>130</v>
       </c>
-      <c r="F2" s="207" t="s">
+      <c r="F2" s="203" t="s">
         <v>723</v>
       </c>
       <c r="G2" s="209" t="s">
@@ -31070,10 +31064,10 @@
     <row r="3" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
-      <c r="C3" s="206"/>
-      <c r="D3" s="206"/>
-      <c r="E3" s="206"/>
-      <c r="F3" s="208"/>
+      <c r="C3" s="202"/>
+      <c r="D3" s="202"/>
+      <c r="E3" s="202"/>
+      <c r="F3" s="204"/>
       <c r="G3" s="80">
         <v>1</v>
       </c>
@@ -36869,11 +36863,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="AE2:AH2"/>
-    <mergeCell ref="AI2:AL2"/>
-    <mergeCell ref="AM2:AP2"/>
-    <mergeCell ref="AQ2:AT2"/>
-    <mergeCell ref="AA2:AD2"/>
     <mergeCell ref="K2:N2"/>
     <mergeCell ref="O2:R2"/>
     <mergeCell ref="S2:V2"/>
@@ -36883,6 +36872,11 @@
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="G2:J2"/>
+    <mergeCell ref="AE2:AH2"/>
+    <mergeCell ref="AI2:AL2"/>
+    <mergeCell ref="AM2:AP2"/>
+    <mergeCell ref="AQ2:AT2"/>
+    <mergeCell ref="AA2:AD2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E84" location="ลูกค้า!A1" display="ลูกค้า!A1"/>
@@ -37360,98 +37354,98 @@
     <row r="2" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
-      <c r="C2" s="205" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="205" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="205" t="s">
+      <c r="C2" s="201" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="201" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="201" t="s">
         <v>130</v>
       </c>
-      <c r="F2" s="207" t="s">
+      <c r="F2" s="203" t="s">
         <v>723</v>
       </c>
-      <c r="G2" s="201" t="s">
+      <c r="G2" s="198" t="s">
         <v>651</v>
       </c>
-      <c r="H2" s="202"/>
-      <c r="I2" s="202"/>
-      <c r="J2" s="203"/>
-      <c r="K2" s="201" t="s">
+      <c r="H2" s="199"/>
+      <c r="I2" s="199"/>
+      <c r="J2" s="200"/>
+      <c r="K2" s="198" t="s">
         <v>652</v>
       </c>
-      <c r="L2" s="202"/>
-      <c r="M2" s="202"/>
-      <c r="N2" s="203"/>
-      <c r="O2" s="201" t="s">
+      <c r="L2" s="199"/>
+      <c r="M2" s="199"/>
+      <c r="N2" s="200"/>
+      <c r="O2" s="198" t="s">
         <v>653</v>
       </c>
-      <c r="P2" s="202"/>
-      <c r="Q2" s="202"/>
-      <c r="R2" s="203"/>
-      <c r="S2" s="201" t="s">
+      <c r="P2" s="199"/>
+      <c r="Q2" s="199"/>
+      <c r="R2" s="200"/>
+      <c r="S2" s="198" t="s">
         <v>654</v>
       </c>
-      <c r="T2" s="202"/>
-      <c r="U2" s="202"/>
-      <c r="V2" s="204"/>
-      <c r="W2" s="201" t="s">
+      <c r="T2" s="199"/>
+      <c r="U2" s="199"/>
+      <c r="V2" s="208"/>
+      <c r="W2" s="198" t="s">
         <v>655</v>
       </c>
-      <c r="X2" s="202"/>
-      <c r="Y2" s="202"/>
-      <c r="Z2" s="204"/>
-      <c r="AA2" s="198" t="s">
+      <c r="X2" s="199"/>
+      <c r="Y2" s="199"/>
+      <c r="Z2" s="208"/>
+      <c r="AA2" s="205" t="s">
         <v>656</v>
       </c>
-      <c r="AB2" s="199"/>
-      <c r="AC2" s="199"/>
-      <c r="AD2" s="200"/>
-      <c r="AE2" s="198" t="s">
+      <c r="AB2" s="206"/>
+      <c r="AC2" s="206"/>
+      <c r="AD2" s="207"/>
+      <c r="AE2" s="205" t="s">
         <v>657</v>
       </c>
-      <c r="AF2" s="199"/>
-      <c r="AG2" s="199"/>
-      <c r="AH2" s="200"/>
-      <c r="AI2" s="198" t="s">
+      <c r="AF2" s="206"/>
+      <c r="AG2" s="206"/>
+      <c r="AH2" s="207"/>
+      <c r="AI2" s="205" t="s">
         <v>658</v>
       </c>
-      <c r="AJ2" s="199"/>
-      <c r="AK2" s="199"/>
-      <c r="AL2" s="200"/>
-      <c r="AM2" s="198" t="s">
+      <c r="AJ2" s="206"/>
+      <c r="AK2" s="206"/>
+      <c r="AL2" s="207"/>
+      <c r="AM2" s="205" t="s">
         <v>659</v>
       </c>
-      <c r="AN2" s="199"/>
-      <c r="AO2" s="199"/>
-      <c r="AP2" s="200"/>
-      <c r="AQ2" s="198" t="s">
+      <c r="AN2" s="206"/>
+      <c r="AO2" s="206"/>
+      <c r="AP2" s="207"/>
+      <c r="AQ2" s="205" t="s">
         <v>660</v>
       </c>
-      <c r="AR2" s="199"/>
-      <c r="AS2" s="199"/>
-      <c r="AT2" s="200"/>
-      <c r="AU2" s="198" t="s">
+      <c r="AR2" s="206"/>
+      <c r="AS2" s="206"/>
+      <c r="AT2" s="207"/>
+      <c r="AU2" s="205" t="s">
         <v>722</v>
       </c>
-      <c r="AV2" s="199"/>
-      <c r="AW2" s="199"/>
-      <c r="AX2" s="200"/>
-      <c r="AY2" s="198" t="s">
+      <c r="AV2" s="206"/>
+      <c r="AW2" s="206"/>
+      <c r="AX2" s="207"/>
+      <c r="AY2" s="205" t="s">
         <v>729</v>
       </c>
-      <c r="AZ2" s="199"/>
-      <c r="BA2" s="199"/>
-      <c r="BB2" s="200"/>
+      <c r="AZ2" s="206"/>
+      <c r="BA2" s="206"/>
+      <c r="BB2" s="207"/>
     </row>
     <row r="3" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
-      <c r="C3" s="206"/>
-      <c r="D3" s="206"/>
-      <c r="E3" s="206"/>
-      <c r="F3" s="208"/>
+      <c r="C3" s="202"/>
+      <c r="D3" s="202"/>
+      <c r="E3" s="202"/>
+      <c r="F3" s="204"/>
       <c r="G3" s="80">
         <v>1</v>
       </c>
@@ -42864,6 +42858,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="O2:R2"/>
     <mergeCell ref="AU2:AX2"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="AY2:BB2"/>
@@ -42875,11 +42874,6 @@
     <mergeCell ref="AM2:AP2"/>
     <mergeCell ref="AQ2:AT2"/>
     <mergeCell ref="S2:V2"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="O2:R2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E84" location="ลูกค้า!A1" display="ลูกค้า!A1"/>

</xml_diff>

<commit_message>
* * V.1.0.1.19 @Home ส่งแล้ว
</commit_message>
<xml_diff>
--- a/_Doc/Feature.xlsx
+++ b/_Doc/Feature.xlsx
@@ -58,7 +58,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Menu!$A$1:$R$57</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -228,7 +228,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2682" uniqueCount="1937">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2684" uniqueCount="1939">
   <si>
     <t>No.</t>
   </si>
@@ -6579,6 +6579,12 @@
   </si>
   <si>
     <t>Stockin preview รายการไม่แสดง SN</t>
+  </si>
+  <si>
+    <t>1.0.1.19</t>
+  </si>
+  <si>
+    <t>คีย์สั่งขาย --&gt; สินค้าขาดทำสั่งจอง --&gt; กด เซฟ จอง ---&gt;เมื่อกลับมาดูรายการสินค้าจะหายหมด</t>
   </si>
 </sst>
 </file>
@@ -7574,6 +7580,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -7581,6 +7596,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -7594,18 +7612,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -8595,7 +8601,7 @@
       <c r="A1" s="215" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="201" t="s">
+      <c r="B1" s="205" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="217" t="s">
@@ -8623,7 +8629,7 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="216"/>
-      <c r="B2" s="202"/>
+      <c r="B2" s="206"/>
       <c r="C2" s="1">
         <v>1</v>
       </c>
@@ -9316,20 +9322,20 @@
       <c r="B1" s="2"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="201" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="201" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="201" t="s">
+      <c r="A2" s="205" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="205" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="205" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="202"/>
-      <c r="B3" s="202"/>
-      <c r="C3" s="202"/>
+      <c r="A3" s="206"/>
+      <c r="B3" s="206"/>
+      <c r="C3" s="206"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
@@ -10531,12 +10537,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
     <mergeCell ref="B43:C43"/>
     <mergeCell ref="B44:C44"/>
     <mergeCell ref="B45:C45"/>
@@ -10547,6 +10547,12 @@
     <mergeCell ref="B40:C40"/>
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -12378,7 +12384,7 @@
   <dimension ref="A1:C522"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A476" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B482" sqref="B482"/>
+      <selection activeCell="B481" sqref="B481"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21.75" x14ac:dyDescent="0.5"/>
@@ -15177,6 +15183,14 @@
     <row r="479" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B479" s="151" t="s">
         <v>1936</v>
+      </c>
+    </row>
+    <row r="481" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A481" s="151" t="s">
+        <v>1937</v>
+      </c>
+      <c r="B481" s="151" t="s">
+        <v>1938</v>
       </c>
     </row>
     <row r="482" spans="1:3" x14ac:dyDescent="0.5">
@@ -25211,97 +25225,97 @@
     </row>
     <row r="2" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
-      <c r="B2" s="201" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="201" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="201" t="s">
+      <c r="B2" s="205" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="205" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="205" t="s">
         <v>130</v>
       </c>
-      <c r="E2" s="203" t="s">
+      <c r="E2" s="207" t="s">
         <v>723</v>
       </c>
-      <c r="F2" s="198" t="s">
+      <c r="F2" s="201" t="s">
         <v>651</v>
       </c>
-      <c r="G2" s="199"/>
-      <c r="H2" s="199"/>
-      <c r="I2" s="200"/>
-      <c r="J2" s="198" t="s">
+      <c r="G2" s="202"/>
+      <c r="H2" s="202"/>
+      <c r="I2" s="203"/>
+      <c r="J2" s="201" t="s">
         <v>652</v>
       </c>
-      <c r="K2" s="199"/>
-      <c r="L2" s="199"/>
-      <c r="M2" s="200"/>
-      <c r="N2" s="198" t="s">
+      <c r="K2" s="202"/>
+      <c r="L2" s="202"/>
+      <c r="M2" s="203"/>
+      <c r="N2" s="201" t="s">
         <v>653</v>
       </c>
-      <c r="O2" s="199"/>
-      <c r="P2" s="199"/>
-      <c r="Q2" s="200"/>
-      <c r="R2" s="198" t="s">
+      <c r="O2" s="202"/>
+      <c r="P2" s="202"/>
+      <c r="Q2" s="203"/>
+      <c r="R2" s="201" t="s">
         <v>654</v>
       </c>
-      <c r="S2" s="199"/>
-      <c r="T2" s="199"/>
-      <c r="U2" s="208"/>
-      <c r="V2" s="198" t="s">
+      <c r="S2" s="202"/>
+      <c r="T2" s="202"/>
+      <c r="U2" s="204"/>
+      <c r="V2" s="201" t="s">
         <v>655</v>
       </c>
-      <c r="W2" s="199"/>
-      <c r="X2" s="199"/>
-      <c r="Y2" s="208"/>
-      <c r="Z2" s="205" t="s">
+      <c r="W2" s="202"/>
+      <c r="X2" s="202"/>
+      <c r="Y2" s="204"/>
+      <c r="Z2" s="198" t="s">
         <v>656</v>
       </c>
-      <c r="AA2" s="206"/>
-      <c r="AB2" s="206"/>
-      <c r="AC2" s="207"/>
-      <c r="AD2" s="205" t="s">
+      <c r="AA2" s="199"/>
+      <c r="AB2" s="199"/>
+      <c r="AC2" s="200"/>
+      <c r="AD2" s="198" t="s">
         <v>657</v>
       </c>
-      <c r="AE2" s="206"/>
-      <c r="AF2" s="206"/>
-      <c r="AG2" s="207"/>
-      <c r="AH2" s="205" t="s">
+      <c r="AE2" s="199"/>
+      <c r="AF2" s="199"/>
+      <c r="AG2" s="200"/>
+      <c r="AH2" s="198" t="s">
         <v>658</v>
       </c>
-      <c r="AI2" s="206"/>
-      <c r="AJ2" s="206"/>
-      <c r="AK2" s="207"/>
-      <c r="AL2" s="205" t="s">
+      <c r="AI2" s="199"/>
+      <c r="AJ2" s="199"/>
+      <c r="AK2" s="200"/>
+      <c r="AL2" s="198" t="s">
         <v>659</v>
       </c>
-      <c r="AM2" s="206"/>
-      <c r="AN2" s="206"/>
-      <c r="AO2" s="207"/>
-      <c r="AP2" s="205" t="s">
+      <c r="AM2" s="199"/>
+      <c r="AN2" s="199"/>
+      <c r="AO2" s="200"/>
+      <c r="AP2" s="198" t="s">
         <v>660</v>
       </c>
-      <c r="AQ2" s="206"/>
-      <c r="AR2" s="206"/>
-      <c r="AS2" s="207"/>
-      <c r="AT2" s="205" t="s">
+      <c r="AQ2" s="199"/>
+      <c r="AR2" s="199"/>
+      <c r="AS2" s="200"/>
+      <c r="AT2" s="198" t="s">
         <v>722</v>
       </c>
-      <c r="AU2" s="206"/>
-      <c r="AV2" s="206"/>
-      <c r="AW2" s="207"/>
-      <c r="AX2" s="205" t="s">
+      <c r="AU2" s="199"/>
+      <c r="AV2" s="199"/>
+      <c r="AW2" s="200"/>
+      <c r="AX2" s="198" t="s">
         <v>729</v>
       </c>
-      <c r="AY2" s="206"/>
-      <c r="AZ2" s="206"/>
-      <c r="BA2" s="207"/>
+      <c r="AY2" s="199"/>
+      <c r="AZ2" s="199"/>
+      <c r="BA2" s="200"/>
     </row>
     <row r="3" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
-      <c r="B3" s="202"/>
-      <c r="C3" s="202"/>
-      <c r="D3" s="202"/>
-      <c r="E3" s="204"/>
+      <c r="B3" s="206"/>
+      <c r="C3" s="206"/>
+      <c r="D3" s="206"/>
+      <c r="E3" s="208"/>
       <c r="F3" s="80">
         <v>1</v>
       </c>
@@ -30455,6 +30469,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:I2"/>
     <mergeCell ref="AL2:AO2"/>
     <mergeCell ref="AP2:AS2"/>
     <mergeCell ref="AT2:AW2"/>
@@ -30465,12 +30485,6 @@
     <mergeCell ref="Z2:AC2"/>
     <mergeCell ref="AD2:AG2"/>
     <mergeCell ref="AH2:AK2"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:I2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D84" location="ลูกค้า!A1" display="ลูกค้า!A1"/>
@@ -30988,16 +31002,16 @@
     <row r="2" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
-      <c r="C2" s="201" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="201" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="201" t="s">
+      <c r="C2" s="205" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="205" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="205" t="s">
         <v>130</v>
       </c>
-      <c r="F2" s="203" t="s">
+      <c r="F2" s="207" t="s">
         <v>723</v>
       </c>
       <c r="G2" s="209" t="s">
@@ -31064,10 +31078,10 @@
     <row r="3" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
-      <c r="C3" s="202"/>
-      <c r="D3" s="202"/>
-      <c r="E3" s="202"/>
-      <c r="F3" s="204"/>
+      <c r="C3" s="206"/>
+      <c r="D3" s="206"/>
+      <c r="E3" s="206"/>
+      <c r="F3" s="208"/>
       <c r="G3" s="80">
         <v>1</v>
       </c>
@@ -36863,6 +36877,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="AE2:AH2"/>
+    <mergeCell ref="AI2:AL2"/>
+    <mergeCell ref="AM2:AP2"/>
+    <mergeCell ref="AQ2:AT2"/>
+    <mergeCell ref="AA2:AD2"/>
     <mergeCell ref="K2:N2"/>
     <mergeCell ref="O2:R2"/>
     <mergeCell ref="S2:V2"/>
@@ -36872,11 +36891,6 @@
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="G2:J2"/>
-    <mergeCell ref="AE2:AH2"/>
-    <mergeCell ref="AI2:AL2"/>
-    <mergeCell ref="AM2:AP2"/>
-    <mergeCell ref="AQ2:AT2"/>
-    <mergeCell ref="AA2:AD2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E84" location="ลูกค้า!A1" display="ลูกค้า!A1"/>
@@ -37354,98 +37368,98 @@
     <row r="2" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
-      <c r="C2" s="201" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="201" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="201" t="s">
+      <c r="C2" s="205" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="205" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="205" t="s">
         <v>130</v>
       </c>
-      <c r="F2" s="203" t="s">
+      <c r="F2" s="207" t="s">
         <v>723</v>
       </c>
-      <c r="G2" s="198" t="s">
+      <c r="G2" s="201" t="s">
         <v>651</v>
       </c>
-      <c r="H2" s="199"/>
-      <c r="I2" s="199"/>
-      <c r="J2" s="200"/>
-      <c r="K2" s="198" t="s">
+      <c r="H2" s="202"/>
+      <c r="I2" s="202"/>
+      <c r="J2" s="203"/>
+      <c r="K2" s="201" t="s">
         <v>652</v>
       </c>
-      <c r="L2" s="199"/>
-      <c r="M2" s="199"/>
-      <c r="N2" s="200"/>
-      <c r="O2" s="198" t="s">
+      <c r="L2" s="202"/>
+      <c r="M2" s="202"/>
+      <c r="N2" s="203"/>
+      <c r="O2" s="201" t="s">
         <v>653</v>
       </c>
-      <c r="P2" s="199"/>
-      <c r="Q2" s="199"/>
-      <c r="R2" s="200"/>
-      <c r="S2" s="198" t="s">
+      <c r="P2" s="202"/>
+      <c r="Q2" s="202"/>
+      <c r="R2" s="203"/>
+      <c r="S2" s="201" t="s">
         <v>654</v>
       </c>
-      <c r="T2" s="199"/>
-      <c r="U2" s="199"/>
-      <c r="V2" s="208"/>
-      <c r="W2" s="198" t="s">
+      <c r="T2" s="202"/>
+      <c r="U2" s="202"/>
+      <c r="V2" s="204"/>
+      <c r="W2" s="201" t="s">
         <v>655</v>
       </c>
-      <c r="X2" s="199"/>
-      <c r="Y2" s="199"/>
-      <c r="Z2" s="208"/>
-      <c r="AA2" s="205" t="s">
+      <c r="X2" s="202"/>
+      <c r="Y2" s="202"/>
+      <c r="Z2" s="204"/>
+      <c r="AA2" s="198" t="s">
         <v>656</v>
       </c>
-      <c r="AB2" s="206"/>
-      <c r="AC2" s="206"/>
-      <c r="AD2" s="207"/>
-      <c r="AE2" s="205" t="s">
+      <c r="AB2" s="199"/>
+      <c r="AC2" s="199"/>
+      <c r="AD2" s="200"/>
+      <c r="AE2" s="198" t="s">
         <v>657</v>
       </c>
-      <c r="AF2" s="206"/>
-      <c r="AG2" s="206"/>
-      <c r="AH2" s="207"/>
-      <c r="AI2" s="205" t="s">
+      <c r="AF2" s="199"/>
+      <c r="AG2" s="199"/>
+      <c r="AH2" s="200"/>
+      <c r="AI2" s="198" t="s">
         <v>658</v>
       </c>
-      <c r="AJ2" s="206"/>
-      <c r="AK2" s="206"/>
-      <c r="AL2" s="207"/>
-      <c r="AM2" s="205" t="s">
+      <c r="AJ2" s="199"/>
+      <c r="AK2" s="199"/>
+      <c r="AL2" s="200"/>
+      <c r="AM2" s="198" t="s">
         <v>659</v>
       </c>
-      <c r="AN2" s="206"/>
-      <c r="AO2" s="206"/>
-      <c r="AP2" s="207"/>
-      <c r="AQ2" s="205" t="s">
+      <c r="AN2" s="199"/>
+      <c r="AO2" s="199"/>
+      <c r="AP2" s="200"/>
+      <c r="AQ2" s="198" t="s">
         <v>660</v>
       </c>
-      <c r="AR2" s="206"/>
-      <c r="AS2" s="206"/>
-      <c r="AT2" s="207"/>
-      <c r="AU2" s="205" t="s">
+      <c r="AR2" s="199"/>
+      <c r="AS2" s="199"/>
+      <c r="AT2" s="200"/>
+      <c r="AU2" s="198" t="s">
         <v>722</v>
       </c>
-      <c r="AV2" s="206"/>
-      <c r="AW2" s="206"/>
-      <c r="AX2" s="207"/>
-      <c r="AY2" s="205" t="s">
+      <c r="AV2" s="199"/>
+      <c r="AW2" s="199"/>
+      <c r="AX2" s="200"/>
+      <c r="AY2" s="198" t="s">
         <v>729</v>
       </c>
-      <c r="AZ2" s="206"/>
-      <c r="BA2" s="206"/>
-      <c r="BB2" s="207"/>
+      <c r="AZ2" s="199"/>
+      <c r="BA2" s="199"/>
+      <c r="BB2" s="200"/>
     </row>
     <row r="3" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
-      <c r="C3" s="202"/>
-      <c r="D3" s="202"/>
-      <c r="E3" s="202"/>
-      <c r="F3" s="204"/>
+      <c r="C3" s="206"/>
+      <c r="D3" s="206"/>
+      <c r="E3" s="206"/>
+      <c r="F3" s="208"/>
       <c r="G3" s="80">
         <v>1</v>
       </c>
@@ -42858,11 +42872,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="O2:R2"/>
     <mergeCell ref="AU2:AX2"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="AY2:BB2"/>
@@ -42874,6 +42883,11 @@
     <mergeCell ref="AM2:AP2"/>
     <mergeCell ref="AQ2:AT2"/>
     <mergeCell ref="S2:V2"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="O2:R2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E84" location="ลูกค้า!A1" display="ลูกค้า!A1"/>

</xml_diff>